<commit_message>
Correção dos artefatos Versão 2
</commit_message>
<xml_diff>
--- a/Artefatos/17. Análise dos Eventos para cada Cenário.xlsx
+++ b/Artefatos/17. Análise dos Eventos para cada Cenário.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amand\OneDrive\Área de Trabalho\Madará\V2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amand\OneDrive\Área de Trabalho\GIT\OPE-Madara\Artefatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49176B23-E625-484A-96B1-868644E9C11B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08AFEF6D-5306-49F7-8DAA-044894E1FF99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20520" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="REALIZACAO_MATRICULA" sheetId="1" r:id="rId1"/>
@@ -110,9 +110,6 @@
     <t>X(1)</t>
   </si>
   <si>
-    <t>Secretaria trata a matrícula</t>
-  </si>
-  <si>
     <t>X(2)</t>
   </si>
   <si>
@@ -420,6 +417,9 @@
   </si>
   <si>
     <t>Análise dos Eventos para cada Cenário</t>
+  </si>
+  <si>
+    <t>Banco envia extrato de pagamento de boletos</t>
   </si>
 </sst>
 </file>
@@ -746,17 +746,30 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
     </xf>
@@ -771,25 +784,12 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1009,7 +1009,7 @@
   <dimension ref="A1:P961"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1028,34 +1028,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="38" t="s">
-        <v>100</v>
-      </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="40"/>
+      <c r="A1" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="25"/>
     </row>
     <row r="2" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="33"/>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="36" t="s">
+      <c r="A2" s="26"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="35"/>
-      <c r="G2" s="36" t="s">
+      <c r="F2" s="28"/>
+      <c r="G2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="37"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="22"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
@@ -1063,10 +1063,10 @@
       <c r="P2" s="2"/>
     </row>
     <row r="3" spans="1:16" ht="33" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="24"/>
+      <c r="B3" s="31"/>
       <c r="C3" s="3" t="s">
         <v>3</v>
       </c>
@@ -1098,10 +1098,10 @@
       <c r="P3" s="2"/>
     </row>
     <row r="4" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="35" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="5">
@@ -1125,8 +1125,8 @@
       <c r="P4" s="2"/>
     </row>
     <row r="5" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="28"/>
-      <c r="B5" s="28"/>
+      <c r="A5" s="33"/>
+      <c r="B5" s="33"/>
       <c r="C5" s="5">
         <v>2</v>
       </c>
@@ -1147,24 +1147,24 @@
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
     </row>
-    <row r="6" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="29"/>
-      <c r="B6" s="29"/>
+    <row r="6" spans="1:16" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="34"/>
+      <c r="B6" s="34"/>
       <c r="C6" s="5">
         <v>3</v>
       </c>
       <c r="D6" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="7"/>
       <c r="F6" s="7"/>
-      <c r="G6" s="11" t="s">
-        <v>18</v>
-      </c>
+      <c r="G6" s="11"/>
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
       <c r="J6" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
@@ -2129,13 +2129,13 @@
     <row r="961" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B4:B6"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="G2:I2"/>
     <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="B4:B6"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -2162,19 +2162,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="22"/>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="25" t="s">
+      <c r="A1" s="38"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="24"/>
-      <c r="G1" s="25" t="s">
+      <c r="F1" s="31"/>
+      <c r="G1" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
       <c r="J1" s="1"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
@@ -2183,10 +2183,10 @@
       <c r="P1" s="2"/>
     </row>
     <row r="2" spans="1:16" ht="33" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="24"/>
+      <c r="B2" s="31"/>
       <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
@@ -2194,19 +2194,19 @@
         <v>4</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>6</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>8</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>10</v>
@@ -2218,17 +2218,17 @@
       <c r="P2" s="2"/>
     </row>
     <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="35" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="5">
         <v>1</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="8" t="s">
@@ -2245,13 +2245,13 @@
       <c r="P3" s="2"/>
     </row>
     <row r="4" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="28"/>
-      <c r="B4" s="28"/>
+      <c r="A4" s="33"/>
+      <c r="B4" s="33"/>
       <c r="C4" s="5">
         <v>2</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
@@ -2268,18 +2268,18 @@
       <c r="P4" s="2"/>
     </row>
     <row r="5" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="28"/>
-      <c r="B5" s="28"/>
+      <c r="A5" s="33"/>
+      <c r="B5" s="33"/>
       <c r="C5" s="5">
         <v>3</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
       <c r="G5" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H5" s="9"/>
       <c r="I5" s="9"/>
@@ -2291,18 +2291,18 @@
       <c r="P5" s="2"/>
     </row>
     <row r="6" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="28"/>
-      <c r="B6" s="28"/>
+      <c r="A6" s="33"/>
+      <c r="B6" s="33"/>
       <c r="C6" s="5">
         <v>4</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
       <c r="G6" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
@@ -2314,16 +2314,16 @@
       <c r="P6" s="2"/>
     </row>
     <row r="7" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="28"/>
-      <c r="B7" s="28"/>
+      <c r="A7" s="33"/>
+      <c r="B7" s="33"/>
       <c r="C7" s="5">
         <v>5</v>
       </c>
       <c r="D7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>28</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>29</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="9"/>
@@ -2337,18 +2337,18 @@
       <c r="P7" s="2"/>
     </row>
     <row r="8" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="28"/>
-      <c r="B8" s="28"/>
+      <c r="A8" s="33"/>
+      <c r="B8" s="33"/>
       <c r="C8" s="5">
         <v>6</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="G8" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
@@ -2360,18 +2360,18 @@
       <c r="P8" s="2"/>
     </row>
     <row r="9" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="28"/>
-      <c r="B9" s="28"/>
+      <c r="A9" s="33"/>
+      <c r="B9" s="33"/>
       <c r="C9" s="5">
         <v>7</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
       <c r="G9" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
@@ -2383,18 +2383,18 @@
       <c r="P9" s="2"/>
     </row>
     <row r="10" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
-      <c r="B10" s="29"/>
+      <c r="A10" s="33"/>
+      <c r="B10" s="34"/>
       <c r="C10" s="5">
         <v>8</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
       <c r="G10" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
@@ -2406,15 +2406,15 @@
       <c r="P10" s="2"/>
     </row>
     <row r="11" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="28"/>
-      <c r="B11" s="30" t="s">
-        <v>36</v>
+      <c r="A11" s="33"/>
+      <c r="B11" s="35" t="s">
+        <v>35</v>
       </c>
       <c r="C11" s="5">
         <v>9</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
@@ -2431,16 +2431,16 @@
       <c r="P11" s="2"/>
     </row>
     <row r="12" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="28"/>
-      <c r="B12" s="28"/>
+      <c r="A12" s="33"/>
+      <c r="B12" s="33"/>
       <c r="C12" s="5">
         <v>10</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F12" s="7"/>
       <c r="G12" s="9"/>
@@ -2454,20 +2454,20 @@
       <c r="P12" s="2"/>
     </row>
     <row r="13" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="29"/>
-      <c r="B13" s="29"/>
+      <c r="A13" s="34"/>
+      <c r="B13" s="34"/>
       <c r="C13" s="5">
         <v>11</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
       <c r="I13" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J13" s="10"/>
       <c r="L13" s="2"/>
@@ -2477,17 +2477,17 @@
       <c r="P13" s="2"/>
     </row>
     <row r="14" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="B14" s="30" t="s">
+      <c r="A14" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="35" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="5">
         <v>12</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
@@ -2504,16 +2504,16 @@
       <c r="P14" s="2"/>
     </row>
     <row r="15" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="28"/>
-      <c r="B15" s="28"/>
+      <c r="A15" s="33"/>
+      <c r="B15" s="33"/>
       <c r="C15" s="5">
         <v>13</v>
       </c>
       <c r="D15" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" s="8" t="s">
         <v>42</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>43</v>
       </c>
       <c r="F15" s="7"/>
       <c r="G15" s="9"/>
@@ -2527,18 +2527,18 @@
       <c r="P15" s="2"/>
     </row>
     <row r="16" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="28"/>
-      <c r="B16" s="28"/>
+      <c r="A16" s="33"/>
+      <c r="B16" s="33"/>
       <c r="C16" s="5">
         <v>14</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
       <c r="G16" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H16" s="9"/>
       <c r="I16" s="9"/>
@@ -2550,16 +2550,16 @@
       <c r="P16" s="2"/>
     </row>
     <row r="17" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="28"/>
-      <c r="B17" s="28"/>
+      <c r="A17" s="33"/>
+      <c r="B17" s="33"/>
       <c r="C17" s="5">
         <v>15</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F17" s="7"/>
       <c r="G17" s="9"/>
@@ -2573,18 +2573,18 @@
       <c r="P17" s="2"/>
     </row>
     <row r="18" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="28"/>
-      <c r="B18" s="28"/>
+      <c r="A18" s="33"/>
+      <c r="B18" s="33"/>
       <c r="C18" s="5">
         <v>16</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
       <c r="G18" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H18" s="9"/>
       <c r="I18" s="9"/>
@@ -2596,18 +2596,18 @@
       <c r="P18" s="2"/>
     </row>
     <row r="19" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="28"/>
-      <c r="B19" s="28"/>
+      <c r="A19" s="33"/>
+      <c r="B19" s="33"/>
       <c r="C19" s="5">
         <v>17</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
       <c r="G19" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H19" s="9"/>
       <c r="I19" s="9"/>
@@ -2619,13 +2619,13 @@
       <c r="P19" s="2"/>
     </row>
     <row r="20" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="28"/>
-      <c r="B20" s="29"/>
+      <c r="A20" s="33"/>
+      <c r="B20" s="34"/>
       <c r="C20" s="5">
         <v>18</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
@@ -2642,18 +2642,18 @@
       <c r="P20" s="2"/>
     </row>
     <row r="21" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="28"/>
-      <c r="B21" s="30" t="s">
-        <v>36</v>
+      <c r="A21" s="33"/>
+      <c r="B21" s="35" t="s">
+        <v>35</v>
       </c>
       <c r="C21" s="5">
         <v>19</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="9"/>
@@ -2667,18 +2667,18 @@
       <c r="P21" s="2"/>
     </row>
     <row r="22" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="28"/>
-      <c r="B22" s="28"/>
+      <c r="A22" s="33"/>
+      <c r="B22" s="33"/>
       <c r="C22" s="5">
         <v>20</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
       <c r="G22" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>
@@ -2690,13 +2690,13 @@
       <c r="P22" s="2"/>
     </row>
     <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="29"/>
-      <c r="B23" s="29"/>
+      <c r="A23" s="34"/>
+      <c r="B23" s="34"/>
       <c r="C23" s="5">
         <v>21</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E23" s="7"/>
       <c r="F23" s="8" t="s">
@@ -2713,17 +2713,17 @@
       <c r="P23" s="2"/>
     </row>
     <row r="24" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="B24" s="30" t="s">
+      <c r="A24" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24" s="35" t="s">
         <v>12</v>
       </c>
       <c r="C24" s="5">
         <v>22</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E24" s="7"/>
       <c r="F24" s="8" t="s">
@@ -2740,18 +2740,18 @@
       <c r="P24" s="2"/>
     </row>
     <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="28"/>
-      <c r="B25" s="28"/>
+      <c r="A25" s="33"/>
+      <c r="B25" s="33"/>
       <c r="C25" s="5">
         <v>23</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
       <c r="G25" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H25" s="9"/>
       <c r="I25" s="9"/>
@@ -2763,18 +2763,18 @@
       <c r="P25" s="2"/>
     </row>
     <row r="26" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="28"/>
-      <c r="B26" s="28"/>
+      <c r="A26" s="33"/>
+      <c r="B26" s="33"/>
       <c r="C26" s="5">
         <v>24</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
       <c r="G26" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H26" s="9"/>
       <c r="I26" s="9"/>
@@ -2786,18 +2786,18 @@
       <c r="P26" s="2"/>
     </row>
     <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="28"/>
-      <c r="B27" s="28"/>
+      <c r="A27" s="33"/>
+      <c r="B27" s="33"/>
       <c r="C27" s="5">
         <v>25</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
       <c r="G27" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H27" s="9"/>
       <c r="I27" s="9"/>
@@ -2809,18 +2809,18 @@
       <c r="P27" s="2"/>
     </row>
     <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="29"/>
-      <c r="B28" s="29"/>
+      <c r="A28" s="34"/>
+      <c r="B28" s="34"/>
       <c r="C28" s="5">
         <v>26</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E28" s="7"/>
       <c r="F28" s="7"/>
       <c r="G28" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H28" s="9"/>
       <c r="I28" s="9"/>
@@ -2832,17 +2832,17 @@
       <c r="P28" s="2"/>
     </row>
     <row r="29" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="B29" s="30" t="s">
+      <c r="A29" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="B29" s="35" t="s">
         <v>12</v>
       </c>
       <c r="C29" s="5">
         <v>27</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E29" s="7"/>
       <c r="F29" s="8" t="s">
@@ -2859,18 +2859,18 @@
       <c r="P29" s="2"/>
     </row>
     <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="28"/>
-      <c r="B30" s="28"/>
+      <c r="A30" s="33"/>
+      <c r="B30" s="33"/>
       <c r="C30" s="5">
         <v>28</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E30" s="7"/>
       <c r="F30" s="7"/>
       <c r="G30" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H30" s="9"/>
       <c r="I30" s="9"/>
@@ -2882,18 +2882,18 @@
       <c r="P30" s="2"/>
     </row>
     <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="28"/>
-      <c r="B31" s="28"/>
+      <c r="A31" s="33"/>
+      <c r="B31" s="33"/>
       <c r="C31" s="5">
         <v>29</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
       <c r="G31" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H31" s="9"/>
       <c r="I31" s="9"/>
@@ -2905,18 +2905,18 @@
       <c r="P31" s="2"/>
     </row>
     <row r="32" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="28"/>
-      <c r="B32" s="28"/>
+      <c r="A32" s="33"/>
+      <c r="B32" s="33"/>
       <c r="C32" s="5">
         <v>30</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E32" s="7"/>
       <c r="F32" s="7"/>
       <c r="G32" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H32" s="9"/>
       <c r="I32" s="9"/>
@@ -2928,18 +2928,18 @@
       <c r="P32" s="2"/>
     </row>
     <row r="33" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="28"/>
-      <c r="B33" s="28"/>
+      <c r="A33" s="33"/>
+      <c r="B33" s="33"/>
       <c r="C33" s="5">
         <v>31</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
       <c r="G33" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H33" s="9"/>
       <c r="I33" s="9"/>
@@ -2951,18 +2951,18 @@
       <c r="P33" s="2"/>
     </row>
     <row r="34" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="28"/>
-      <c r="B34" s="29"/>
+      <c r="A34" s="33"/>
+      <c r="B34" s="34"/>
       <c r="C34" s="5">
         <v>32</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E34" s="7"/>
       <c r="F34" s="7"/>
       <c r="G34" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H34" s="9"/>
       <c r="I34" s="9"/>
@@ -2974,20 +2974,20 @@
       <c r="P34" s="2"/>
     </row>
     <row r="35" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="29"/>
+      <c r="A35" s="34"/>
       <c r="B35" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C35" s="5">
         <v>33</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E35" s="7"/>
       <c r="F35" s="7"/>
       <c r="G35" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H35" s="9"/>
       <c r="I35" s="9"/>
@@ -2999,17 +2999,17 @@
       <c r="P35" s="2"/>
     </row>
     <row r="36" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="31" t="s">
-        <v>77</v>
-      </c>
-      <c r="B36" s="30" t="s">
+      <c r="A36" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="B36" s="35" t="s">
         <v>12</v>
       </c>
       <c r="C36" s="5">
         <v>34</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E36" s="7"/>
       <c r="F36" s="8" t="s">
@@ -3026,18 +3026,18 @@
       <c r="P36" s="2"/>
     </row>
     <row r="37" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="28"/>
-      <c r="B37" s="28"/>
+      <c r="A37" s="33"/>
+      <c r="B37" s="33"/>
       <c r="C37" s="5">
         <v>35</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E37" s="7"/>
       <c r="F37" s="7"/>
       <c r="G37" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H37" s="9"/>
       <c r="I37" s="9"/>
@@ -3049,18 +3049,18 @@
       <c r="P37" s="2"/>
     </row>
     <row r="38" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="28"/>
-      <c r="B38" s="28"/>
+      <c r="A38" s="33"/>
+      <c r="B38" s="33"/>
       <c r="C38" s="5">
         <v>36</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E38" s="7"/>
       <c r="F38" s="7"/>
       <c r="G38" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H38" s="9"/>
       <c r="I38" s="9"/>
@@ -3072,18 +3072,18 @@
       <c r="P38" s="2"/>
     </row>
     <row r="39" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="28"/>
-      <c r="B39" s="28"/>
+      <c r="A39" s="33"/>
+      <c r="B39" s="33"/>
       <c r="C39" s="5">
         <v>37</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E39" s="7"/>
       <c r="F39" s="7"/>
       <c r="G39" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H39" s="9"/>
       <c r="I39" s="9"/>
@@ -3095,18 +3095,18 @@
       <c r="P39" s="2"/>
     </row>
     <row r="40" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="28"/>
-      <c r="B40" s="29"/>
+      <c r="A40" s="33"/>
+      <c r="B40" s="34"/>
       <c r="C40" s="5">
         <v>38</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E40" s="7"/>
       <c r="F40" s="7"/>
       <c r="G40" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H40" s="9"/>
       <c r="I40" s="9"/>
@@ -3118,20 +3118,20 @@
       <c r="P40" s="2"/>
     </row>
     <row r="41" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="29"/>
+      <c r="A41" s="34"/>
       <c r="B41" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C41" s="5">
         <v>39</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
       <c r="G41" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H41" s="9"/>
       <c r="I41" s="9"/>
@@ -3143,8 +3143,8 @@
       <c r="P41" s="2"/>
     </row>
     <row r="42" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="32" t="s">
-        <v>89</v>
+      <c r="A42" s="37" t="s">
+        <v>88</v>
       </c>
       <c r="B42" s="15" t="s">
         <v>12</v>
@@ -3153,7 +3153,7 @@
         <v>40</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
@@ -3170,22 +3170,22 @@
       <c r="P42" s="2"/>
     </row>
     <row r="43" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="28"/>
-      <c r="B43" s="30" t="s">
-        <v>91</v>
+      <c r="A43" s="33"/>
+      <c r="B43" s="35" t="s">
+        <v>90</v>
       </c>
       <c r="C43" s="5">
         <v>41</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="9"/>
       <c r="H43" s="9"/>
       <c r="I43" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J43" s="10"/>
       <c r="L43" s="2"/>
@@ -3195,16 +3195,16 @@
       <c r="P43" s="2"/>
     </row>
     <row r="44" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="28"/>
-      <c r="B44" s="28"/>
+      <c r="A44" s="33"/>
+      <c r="B44" s="33"/>
       <c r="C44" s="5">
         <v>42</v>
       </c>
       <c r="D44" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="E44" s="8" t="s">
         <v>93</v>
-      </c>
-      <c r="E44" s="8" t="s">
-        <v>94</v>
       </c>
       <c r="F44" s="7"/>
       <c r="G44" s="9"/>
@@ -3218,20 +3218,20 @@
       <c r="P44" s="2"/>
     </row>
     <row r="45" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="28"/>
-      <c r="B45" s="28"/>
+      <c r="A45" s="33"/>
+      <c r="B45" s="33"/>
       <c r="C45" s="5">
         <v>43</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E45" s="7"/>
       <c r="F45" s="7"/>
       <c r="G45" s="9"/>
       <c r="H45" s="9"/>
       <c r="I45" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J45" s="10"/>
       <c r="L45" s="2"/>
@@ -3241,18 +3241,18 @@
       <c r="P45" s="2"/>
     </row>
     <row r="46" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="29"/>
-      <c r="B46" s="29"/>
+      <c r="A46" s="34"/>
+      <c r="B46" s="34"/>
       <c r="C46" s="18">
         <v>44</v>
       </c>
       <c r="D46" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E46" s="19"/>
       <c r="F46" s="19"/>
       <c r="G46" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H46" s="20"/>
       <c r="I46" s="20"/>
@@ -4219,6 +4219,13 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:A13"/>
+    <mergeCell ref="B3:B10"/>
+    <mergeCell ref="B11:B13"/>
     <mergeCell ref="A14:A23"/>
     <mergeCell ref="B21:B23"/>
     <mergeCell ref="A36:A41"/>
@@ -4230,13 +4237,6 @@
     <mergeCell ref="A29:A35"/>
     <mergeCell ref="B29:B34"/>
     <mergeCell ref="B36:B40"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:A13"/>
-    <mergeCell ref="B3:B10"/>
-    <mergeCell ref="B11:B13"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -4263,19 +4263,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="22"/>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="25" t="s">
+      <c r="A1" s="38"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="24"/>
-      <c r="G1" s="25" t="s">
+      <c r="F1" s="31"/>
+      <c r="G1" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
       <c r="J1" s="1"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
@@ -4284,10 +4284,10 @@
       <c r="P1" s="2"/>
     </row>
     <row r="2" spans="1:16" ht="33" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="24"/>
+      <c r="B2" s="31"/>
       <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
@@ -4295,19 +4295,19 @@
         <v>4</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>6</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>8</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>10</v>
@@ -4319,17 +4319,17 @@
       <c r="P2" s="2"/>
     </row>
     <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="35" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="5">
         <v>1</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="8" t="s">
@@ -4346,13 +4346,13 @@
       <c r="P3" s="2"/>
     </row>
     <row r="4" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="28"/>
-      <c r="B4" s="28"/>
+      <c r="A4" s="33"/>
+      <c r="B4" s="33"/>
       <c r="C4" s="5">
         <v>2</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
@@ -4369,18 +4369,18 @@
       <c r="P4" s="2"/>
     </row>
     <row r="5" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="28"/>
-      <c r="B5" s="28"/>
+      <c r="A5" s="33"/>
+      <c r="B5" s="33"/>
       <c r="C5" s="5">
         <v>3</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
       <c r="G5" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H5" s="9"/>
       <c r="I5" s="9"/>
@@ -4392,18 +4392,18 @@
       <c r="P5" s="2"/>
     </row>
     <row r="6" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="28"/>
-      <c r="B6" s="28"/>
+      <c r="A6" s="33"/>
+      <c r="B6" s="33"/>
       <c r="C6" s="5">
         <v>4</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
       <c r="G6" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
@@ -4415,16 +4415,16 @@
       <c r="P6" s="2"/>
     </row>
     <row r="7" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="28"/>
-      <c r="B7" s="28"/>
+      <c r="A7" s="33"/>
+      <c r="B7" s="33"/>
       <c r="C7" s="5">
         <v>5</v>
       </c>
       <c r="D7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>28</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>29</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="9"/>
@@ -4438,18 +4438,18 @@
       <c r="P7" s="2"/>
     </row>
     <row r="8" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="28"/>
-      <c r="B8" s="28"/>
+      <c r="A8" s="33"/>
+      <c r="B8" s="33"/>
       <c r="C8" s="5">
         <v>6</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="G8" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
@@ -4461,18 +4461,18 @@
       <c r="P8" s="2"/>
     </row>
     <row r="9" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="28"/>
-      <c r="B9" s="28"/>
+      <c r="A9" s="33"/>
+      <c r="B9" s="33"/>
       <c r="C9" s="5">
         <v>7</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
       <c r="G9" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
@@ -4484,18 +4484,18 @@
       <c r="P9" s="2"/>
     </row>
     <row r="10" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
-      <c r="B10" s="29"/>
+      <c r="A10" s="33"/>
+      <c r="B10" s="34"/>
       <c r="C10" s="5">
         <v>8</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
       <c r="G10" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
@@ -4507,15 +4507,15 @@
       <c r="P10" s="2"/>
     </row>
     <row r="11" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="28"/>
-      <c r="B11" s="30" t="s">
-        <v>36</v>
+      <c r="A11" s="33"/>
+      <c r="B11" s="35" t="s">
+        <v>35</v>
       </c>
       <c r="C11" s="5">
         <v>9</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
@@ -4532,16 +4532,16 @@
       <c r="P11" s="2"/>
     </row>
     <row r="12" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="28"/>
-      <c r="B12" s="28"/>
+      <c r="A12" s="33"/>
+      <c r="B12" s="33"/>
       <c r="C12" s="5">
         <v>10</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F12" s="7"/>
       <c r="G12" s="9"/>
@@ -4555,20 +4555,20 @@
       <c r="P12" s="2"/>
     </row>
     <row r="13" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="29"/>
-      <c r="B13" s="29"/>
+      <c r="A13" s="34"/>
+      <c r="B13" s="34"/>
       <c r="C13" s="5">
         <v>11</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
       <c r="I13" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J13" s="10"/>
       <c r="L13" s="2"/>
@@ -4578,17 +4578,17 @@
       <c r="P13" s="2"/>
     </row>
     <row r="14" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="B14" s="30" t="s">
+      <c r="A14" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="35" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="5">
         <v>12</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
@@ -4605,16 +4605,16 @@
       <c r="P14" s="2"/>
     </row>
     <row r="15" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="28"/>
-      <c r="B15" s="28"/>
+      <c r="A15" s="33"/>
+      <c r="B15" s="33"/>
       <c r="C15" s="5">
         <v>13</v>
       </c>
       <c r="D15" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" s="8" t="s">
         <v>42</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>43</v>
       </c>
       <c r="F15" s="7"/>
       <c r="G15" s="9"/>
@@ -4628,18 +4628,18 @@
       <c r="P15" s="2"/>
     </row>
     <row r="16" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="28"/>
-      <c r="B16" s="28"/>
+      <c r="A16" s="33"/>
+      <c r="B16" s="33"/>
       <c r="C16" s="5">
         <v>14</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
       <c r="G16" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H16" s="9"/>
       <c r="I16" s="9"/>
@@ -4651,16 +4651,16 @@
       <c r="P16" s="2"/>
     </row>
     <row r="17" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="28"/>
-      <c r="B17" s="28"/>
+      <c r="A17" s="33"/>
+      <c r="B17" s="33"/>
       <c r="C17" s="5">
         <v>15</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F17" s="7"/>
       <c r="G17" s="9"/>
@@ -4674,18 +4674,18 @@
       <c r="P17" s="2"/>
     </row>
     <row r="18" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="28"/>
-      <c r="B18" s="28"/>
+      <c r="A18" s="33"/>
+      <c r="B18" s="33"/>
       <c r="C18" s="5">
         <v>16</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
       <c r="G18" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H18" s="9"/>
       <c r="I18" s="9"/>
@@ -4697,18 +4697,18 @@
       <c r="P18" s="2"/>
     </row>
     <row r="19" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="28"/>
-      <c r="B19" s="28"/>
+      <c r="A19" s="33"/>
+      <c r="B19" s="33"/>
       <c r="C19" s="5">
         <v>17</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
       <c r="G19" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H19" s="9"/>
       <c r="I19" s="9"/>
@@ -4720,13 +4720,13 @@
       <c r="P19" s="2"/>
     </row>
     <row r="20" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="28"/>
-      <c r="B20" s="29"/>
+      <c r="A20" s="33"/>
+      <c r="B20" s="34"/>
       <c r="C20" s="5">
         <v>18</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
@@ -4743,18 +4743,18 @@
       <c r="P20" s="2"/>
     </row>
     <row r="21" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="28"/>
-      <c r="B21" s="30" t="s">
-        <v>36</v>
+      <c r="A21" s="33"/>
+      <c r="B21" s="35" t="s">
+        <v>35</v>
       </c>
       <c r="C21" s="5">
         <v>19</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="9"/>
@@ -4768,18 +4768,18 @@
       <c r="P21" s="2"/>
     </row>
     <row r="22" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="28"/>
-      <c r="B22" s="28"/>
+      <c r="A22" s="33"/>
+      <c r="B22" s="33"/>
       <c r="C22" s="5">
         <v>20</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
       <c r="G22" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>
@@ -4791,13 +4791,13 @@
       <c r="P22" s="2"/>
     </row>
     <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="29"/>
-      <c r="B23" s="29"/>
+      <c r="A23" s="34"/>
+      <c r="B23" s="34"/>
       <c r="C23" s="5">
         <v>21</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E23" s="7"/>
       <c r="F23" s="8" t="s">
@@ -4814,17 +4814,17 @@
       <c r="P23" s="2"/>
     </row>
     <row r="24" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="B24" s="30" t="s">
+      <c r="A24" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24" s="35" t="s">
         <v>12</v>
       </c>
       <c r="C24" s="5">
         <v>22</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E24" s="7"/>
       <c r="F24" s="8" t="s">
@@ -4841,18 +4841,18 @@
       <c r="P24" s="2"/>
     </row>
     <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="28"/>
-      <c r="B25" s="28"/>
+      <c r="A25" s="33"/>
+      <c r="B25" s="33"/>
       <c r="C25" s="5">
         <v>23</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
       <c r="G25" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H25" s="9"/>
       <c r="I25" s="9"/>
@@ -4864,18 +4864,18 @@
       <c r="P25" s="2"/>
     </row>
     <row r="26" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="28"/>
-      <c r="B26" s="28"/>
+      <c r="A26" s="33"/>
+      <c r="B26" s="33"/>
       <c r="C26" s="5">
         <v>24</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
       <c r="G26" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H26" s="9"/>
       <c r="I26" s="9"/>
@@ -4887,18 +4887,18 @@
       <c r="P26" s="2"/>
     </row>
     <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="28"/>
-      <c r="B27" s="28"/>
+      <c r="A27" s="33"/>
+      <c r="B27" s="33"/>
       <c r="C27" s="5">
         <v>25</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
       <c r="G27" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H27" s="9"/>
       <c r="I27" s="9"/>
@@ -4910,18 +4910,18 @@
       <c r="P27" s="2"/>
     </row>
     <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="29"/>
-      <c r="B28" s="29"/>
+      <c r="A28" s="34"/>
+      <c r="B28" s="34"/>
       <c r="C28" s="5">
         <v>26</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E28" s="7"/>
       <c r="F28" s="7"/>
       <c r="G28" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H28" s="9"/>
       <c r="I28" s="9"/>
@@ -4933,17 +4933,17 @@
       <c r="P28" s="2"/>
     </row>
     <row r="29" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="B29" s="30" t="s">
+      <c r="A29" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="B29" s="35" t="s">
         <v>12</v>
       </c>
       <c r="C29" s="5">
         <v>27</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E29" s="7"/>
       <c r="F29" s="8" t="s">
@@ -4960,18 +4960,18 @@
       <c r="P29" s="2"/>
     </row>
     <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="28"/>
-      <c r="B30" s="28"/>
+      <c r="A30" s="33"/>
+      <c r="B30" s="33"/>
       <c r="C30" s="5">
         <v>28</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E30" s="7"/>
       <c r="F30" s="7"/>
       <c r="G30" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H30" s="9"/>
       <c r="I30" s="9"/>
@@ -4983,18 +4983,18 @@
       <c r="P30" s="2"/>
     </row>
     <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="28"/>
-      <c r="B31" s="28"/>
+      <c r="A31" s="33"/>
+      <c r="B31" s="33"/>
       <c r="C31" s="5">
         <v>29</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
       <c r="G31" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H31" s="9"/>
       <c r="I31" s="9"/>
@@ -5006,18 +5006,18 @@
       <c r="P31" s="2"/>
     </row>
     <row r="32" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="28"/>
-      <c r="B32" s="28"/>
+      <c r="A32" s="33"/>
+      <c r="B32" s="33"/>
       <c r="C32" s="5">
         <v>30</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E32" s="7"/>
       <c r="F32" s="7"/>
       <c r="G32" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H32" s="9"/>
       <c r="I32" s="9"/>
@@ -5029,18 +5029,18 @@
       <c r="P32" s="2"/>
     </row>
     <row r="33" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="28"/>
-      <c r="B33" s="28"/>
+      <c r="A33" s="33"/>
+      <c r="B33" s="33"/>
       <c r="C33" s="5">
         <v>31</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
       <c r="G33" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H33" s="9"/>
       <c r="I33" s="9"/>
@@ -5052,18 +5052,18 @@
       <c r="P33" s="2"/>
     </row>
     <row r="34" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="28"/>
-      <c r="B34" s="29"/>
+      <c r="A34" s="33"/>
+      <c r="B34" s="34"/>
       <c r="C34" s="5">
         <v>32</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E34" s="7"/>
       <c r="F34" s="7"/>
       <c r="G34" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H34" s="9"/>
       <c r="I34" s="9"/>
@@ -5075,20 +5075,20 @@
       <c r="P34" s="2"/>
     </row>
     <row r="35" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="29"/>
+      <c r="A35" s="34"/>
       <c r="B35" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C35" s="5">
         <v>33</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E35" s="7"/>
       <c r="F35" s="7"/>
       <c r="G35" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H35" s="9"/>
       <c r="I35" s="9"/>
@@ -5100,17 +5100,17 @@
       <c r="P35" s="2"/>
     </row>
     <row r="36" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="31" t="s">
-        <v>77</v>
-      </c>
-      <c r="B36" s="30" t="s">
+      <c r="A36" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="B36" s="35" t="s">
         <v>12</v>
       </c>
       <c r="C36" s="5">
         <v>34</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E36" s="7"/>
       <c r="F36" s="8" t="s">
@@ -5127,18 +5127,18 @@
       <c r="P36" s="2"/>
     </row>
     <row r="37" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="28"/>
-      <c r="B37" s="28"/>
+      <c r="A37" s="33"/>
+      <c r="B37" s="33"/>
       <c r="C37" s="5">
         <v>35</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E37" s="7"/>
       <c r="F37" s="7"/>
       <c r="G37" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H37" s="9"/>
       <c r="I37" s="9"/>
@@ -5150,18 +5150,18 @@
       <c r="P37" s="2"/>
     </row>
     <row r="38" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="28"/>
-      <c r="B38" s="28"/>
+      <c r="A38" s="33"/>
+      <c r="B38" s="33"/>
       <c r="C38" s="5">
         <v>36</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E38" s="7"/>
       <c r="F38" s="7"/>
       <c r="G38" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H38" s="9"/>
       <c r="I38" s="9"/>
@@ -5173,18 +5173,18 @@
       <c r="P38" s="2"/>
     </row>
     <row r="39" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="28"/>
-      <c r="B39" s="28"/>
+      <c r="A39" s="33"/>
+      <c r="B39" s="33"/>
       <c r="C39" s="5">
         <v>37</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E39" s="7"/>
       <c r="F39" s="7"/>
       <c r="G39" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H39" s="9"/>
       <c r="I39" s="9"/>
@@ -5196,18 +5196,18 @@
       <c r="P39" s="2"/>
     </row>
     <row r="40" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="28"/>
-      <c r="B40" s="29"/>
+      <c r="A40" s="33"/>
+      <c r="B40" s="34"/>
       <c r="C40" s="5">
         <v>38</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E40" s="7"/>
       <c r="F40" s="7"/>
       <c r="G40" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H40" s="9"/>
       <c r="I40" s="9"/>
@@ -5219,20 +5219,20 @@
       <c r="P40" s="2"/>
     </row>
     <row r="41" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="29"/>
+      <c r="A41" s="34"/>
       <c r="B41" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C41" s="5">
         <v>39</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
       <c r="G41" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H41" s="9"/>
       <c r="I41" s="9"/>
@@ -5244,8 +5244,8 @@
       <c r="P41" s="2"/>
     </row>
     <row r="42" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="32" t="s">
-        <v>89</v>
+      <c r="A42" s="37" t="s">
+        <v>88</v>
       </c>
       <c r="B42" s="15" t="s">
         <v>12</v>
@@ -5254,7 +5254,7 @@
         <v>40</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
@@ -5271,22 +5271,22 @@
       <c r="P42" s="2"/>
     </row>
     <row r="43" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="28"/>
-      <c r="B43" s="30" t="s">
-        <v>91</v>
+      <c r="A43" s="33"/>
+      <c r="B43" s="35" t="s">
+        <v>90</v>
       </c>
       <c r="C43" s="5">
         <v>41</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="9"/>
       <c r="H43" s="9"/>
       <c r="I43" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J43" s="10"/>
       <c r="L43" s="2"/>
@@ -5296,16 +5296,16 @@
       <c r="P43" s="2"/>
     </row>
     <row r="44" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="28"/>
-      <c r="B44" s="28"/>
+      <c r="A44" s="33"/>
+      <c r="B44" s="33"/>
       <c r="C44" s="5">
         <v>42</v>
       </c>
       <c r="D44" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="E44" s="8" t="s">
         <v>93</v>
-      </c>
-      <c r="E44" s="8" t="s">
-        <v>94</v>
       </c>
       <c r="F44" s="7"/>
       <c r="G44" s="9"/>
@@ -5319,20 +5319,20 @@
       <c r="P44" s="2"/>
     </row>
     <row r="45" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="28"/>
-      <c r="B45" s="28"/>
+      <c r="A45" s="33"/>
+      <c r="B45" s="33"/>
       <c r="C45" s="5">
         <v>43</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E45" s="7"/>
       <c r="F45" s="7"/>
       <c r="G45" s="9"/>
       <c r="H45" s="9"/>
       <c r="I45" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J45" s="10"/>
       <c r="L45" s="2"/>
@@ -5342,18 +5342,18 @@
       <c r="P45" s="2"/>
     </row>
     <row r="46" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="29"/>
-      <c r="B46" s="29"/>
+      <c r="A46" s="34"/>
+      <c r="B46" s="34"/>
       <c r="C46" s="18">
         <v>44</v>
       </c>
       <c r="D46" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E46" s="19"/>
       <c r="F46" s="19"/>
       <c r="G46" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H46" s="20"/>
       <c r="I46" s="20"/>
@@ -6320,6 +6320,13 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:A13"/>
+    <mergeCell ref="B3:B10"/>
+    <mergeCell ref="B11:B13"/>
     <mergeCell ref="A14:A23"/>
     <mergeCell ref="B21:B23"/>
     <mergeCell ref="A36:A41"/>
@@ -6331,13 +6338,6 @@
     <mergeCell ref="A29:A35"/>
     <mergeCell ref="B29:B34"/>
     <mergeCell ref="B36:B40"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:A13"/>
-    <mergeCell ref="B3:B10"/>
-    <mergeCell ref="B11:B13"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
Atualização com correção dos artefatos 12 e 17
</commit_message>
<xml_diff>
--- a/Artefatos/17. Análise dos Eventos para cada Cenário.xlsx
+++ b/Artefatos/17. Análise dos Eventos para cada Cenário.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amand\OneDrive\Área de Trabalho\GIT\OPE-Madara\Artefatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08AFEF6D-5306-49F7-8DAA-044894E1FF99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87C660AA-7A9D-4D8D-9AA8-E3691BE14C15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -749,6 +749,14 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -770,26 +778,18 @@
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1009,7 +1009,7 @@
   <dimension ref="A1:P961"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1028,33 +1028,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="25"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="29"/>
     </row>
     <row r="2" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="26"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="29" t="s">
+      <c r="A2" s="30"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="28"/>
-      <c r="G2" s="29" t="s">
+      <c r="F2" s="32"/>
+      <c r="G2" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
       <c r="J2" s="22"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
@@ -1063,10 +1063,10 @@
       <c r="P2" s="2"/>
     </row>
     <row r="3" spans="1:16" ht="33" x14ac:dyDescent="0.25">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="31"/>
+      <c r="B3" s="35"/>
       <c r="C3" s="3" t="s">
         <v>3</v>
       </c>
@@ -1098,10 +1098,10 @@
       <c r="P3" s="2"/>
     </row>
     <row r="4" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="26" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="5">
@@ -1125,8 +1125,8 @@
       <c r="P4" s="2"/>
     </row>
     <row r="5" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="33"/>
-      <c r="B5" s="33"/>
+      <c r="A5" s="24"/>
+      <c r="B5" s="24"/>
       <c r="C5" s="5">
         <v>2</v>
       </c>
@@ -1148,8 +1148,8 @@
       <c r="P5" s="2"/>
     </row>
     <row r="6" spans="1:16" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="34"/>
-      <c r="B6" s="34"/>
+      <c r="A6" s="25"/>
+      <c r="B6" s="25"/>
       <c r="C6" s="5">
         <v>3</v>
       </c>
@@ -2162,19 +2162,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="38"/>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="40" t="s">
+      <c r="A1" s="36"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="31"/>
-      <c r="G1" s="40" t="s">
+      <c r="F1" s="35"/>
+      <c r="G1" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
       <c r="J1" s="1"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
@@ -2183,10 +2183,10 @@
       <c r="P1" s="2"/>
     </row>
     <row r="2" spans="1:16" ht="33" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="31"/>
+      <c r="B2" s="35"/>
       <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
@@ -2218,10 +2218,10 @@
       <c r="P2" s="2"/>
     </row>
     <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="26" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="5">
@@ -2245,8 +2245,8 @@
       <c r="P3" s="2"/>
     </row>
     <row r="4" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="33"/>
-      <c r="B4" s="33"/>
+      <c r="A4" s="24"/>
+      <c r="B4" s="24"/>
       <c r="C4" s="5">
         <v>2</v>
       </c>
@@ -2268,8 +2268,8 @@
       <c r="P4" s="2"/>
     </row>
     <row r="5" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="33"/>
-      <c r="B5" s="33"/>
+      <c r="A5" s="24"/>
+      <c r="B5" s="24"/>
       <c r="C5" s="5">
         <v>3</v>
       </c>
@@ -2291,8 +2291,8 @@
       <c r="P5" s="2"/>
     </row>
     <row r="6" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="33"/>
-      <c r="B6" s="33"/>
+      <c r="A6" s="24"/>
+      <c r="B6" s="24"/>
       <c r="C6" s="5">
         <v>4</v>
       </c>
@@ -2314,8 +2314,8 @@
       <c r="P6" s="2"/>
     </row>
     <row r="7" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="33"/>
-      <c r="B7" s="33"/>
+      <c r="A7" s="24"/>
+      <c r="B7" s="24"/>
       <c r="C7" s="5">
         <v>5</v>
       </c>
@@ -2337,8 +2337,8 @@
       <c r="P7" s="2"/>
     </row>
     <row r="8" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="33"/>
-      <c r="B8" s="33"/>
+      <c r="A8" s="24"/>
+      <c r="B8" s="24"/>
       <c r="C8" s="5">
         <v>6</v>
       </c>
@@ -2360,8 +2360,8 @@
       <c r="P8" s="2"/>
     </row>
     <row r="9" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="33"/>
-      <c r="B9" s="33"/>
+      <c r="A9" s="24"/>
+      <c r="B9" s="24"/>
       <c r="C9" s="5">
         <v>7</v>
       </c>
@@ -2383,8 +2383,8 @@
       <c r="P9" s="2"/>
     </row>
     <row r="10" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="33"/>
-      <c r="B10" s="34"/>
+      <c r="A10" s="24"/>
+      <c r="B10" s="25"/>
       <c r="C10" s="5">
         <v>8</v>
       </c>
@@ -2406,8 +2406,8 @@
       <c r="P10" s="2"/>
     </row>
     <row r="11" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="33"/>
-      <c r="B11" s="35" t="s">
+      <c r="A11" s="24"/>
+      <c r="B11" s="26" t="s">
         <v>35</v>
       </c>
       <c r="C11" s="5">
@@ -2431,8 +2431,8 @@
       <c r="P11" s="2"/>
     </row>
     <row r="12" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="33"/>
-      <c r="B12" s="33"/>
+      <c r="A12" s="24"/>
+      <c r="B12" s="24"/>
       <c r="C12" s="5">
         <v>10</v>
       </c>
@@ -2454,8 +2454,8 @@
       <c r="P12" s="2"/>
     </row>
     <row r="13" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="34"/>
-      <c r="B13" s="34"/>
+      <c r="A13" s="25"/>
+      <c r="B13" s="25"/>
       <c r="C13" s="5">
         <v>11</v>
       </c>
@@ -2477,10 +2477,10 @@
       <c r="P13" s="2"/>
     </row>
     <row r="14" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="36" t="s">
+      <c r="A14" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="35" t="s">
+      <c r="B14" s="26" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="5">
@@ -2504,8 +2504,8 @@
       <c r="P14" s="2"/>
     </row>
     <row r="15" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="33"/>
-      <c r="B15" s="33"/>
+      <c r="A15" s="24"/>
+      <c r="B15" s="24"/>
       <c r="C15" s="5">
         <v>13</v>
       </c>
@@ -2527,8 +2527,8 @@
       <c r="P15" s="2"/>
     </row>
     <row r="16" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="33"/>
-      <c r="B16" s="33"/>
+      <c r="A16" s="24"/>
+      <c r="B16" s="24"/>
       <c r="C16" s="5">
         <v>14</v>
       </c>
@@ -2550,8 +2550,8 @@
       <c r="P16" s="2"/>
     </row>
     <row r="17" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="33"/>
-      <c r="B17" s="33"/>
+      <c r="A17" s="24"/>
+      <c r="B17" s="24"/>
       <c r="C17" s="5">
         <v>15</v>
       </c>
@@ -2573,8 +2573,8 @@
       <c r="P17" s="2"/>
     </row>
     <row r="18" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="33"/>
-      <c r="B18" s="33"/>
+      <c r="A18" s="24"/>
+      <c r="B18" s="24"/>
       <c r="C18" s="5">
         <v>16</v>
       </c>
@@ -2596,8 +2596,8 @@
       <c r="P18" s="2"/>
     </row>
     <row r="19" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="33"/>
-      <c r="B19" s="33"/>
+      <c r="A19" s="24"/>
+      <c r="B19" s="24"/>
       <c r="C19" s="5">
         <v>17</v>
       </c>
@@ -2619,8 +2619,8 @@
       <c r="P19" s="2"/>
     </row>
     <row r="20" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="33"/>
-      <c r="B20" s="34"/>
+      <c r="A20" s="24"/>
+      <c r="B20" s="25"/>
       <c r="C20" s="5">
         <v>18</v>
       </c>
@@ -2642,8 +2642,8 @@
       <c r="P20" s="2"/>
     </row>
     <row r="21" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="33"/>
-      <c r="B21" s="35" t="s">
+      <c r="A21" s="24"/>
+      <c r="B21" s="26" t="s">
         <v>35</v>
       </c>
       <c r="C21" s="5">
@@ -2667,8 +2667,8 @@
       <c r="P21" s="2"/>
     </row>
     <row r="22" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="33"/>
-      <c r="B22" s="33"/>
+      <c r="A22" s="24"/>
+      <c r="B22" s="24"/>
       <c r="C22" s="5">
         <v>20</v>
       </c>
@@ -2690,8 +2690,8 @@
       <c r="P22" s="2"/>
     </row>
     <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="34"/>
-      <c r="B23" s="34"/>
+      <c r="A23" s="25"/>
+      <c r="B23" s="25"/>
       <c r="C23" s="5">
         <v>21</v>
       </c>
@@ -2713,10 +2713,10 @@
       <c r="P23" s="2"/>
     </row>
     <row r="24" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="37" t="s">
+      <c r="A24" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="B24" s="35" t="s">
+      <c r="B24" s="26" t="s">
         <v>12</v>
       </c>
       <c r="C24" s="5">
@@ -2740,8 +2740,8 @@
       <c r="P24" s="2"/>
     </row>
     <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="33"/>
-      <c r="B25" s="33"/>
+      <c r="A25" s="24"/>
+      <c r="B25" s="24"/>
       <c r="C25" s="5">
         <v>23</v>
       </c>
@@ -2763,8 +2763,8 @@
       <c r="P25" s="2"/>
     </row>
     <row r="26" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="33"/>
-      <c r="B26" s="33"/>
+      <c r="A26" s="24"/>
+      <c r="B26" s="24"/>
       <c r="C26" s="5">
         <v>24</v>
       </c>
@@ -2786,8 +2786,8 @@
       <c r="P26" s="2"/>
     </row>
     <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="33"/>
-      <c r="B27" s="33"/>
+      <c r="A27" s="24"/>
+      <c r="B27" s="24"/>
       <c r="C27" s="5">
         <v>25</v>
       </c>
@@ -2809,8 +2809,8 @@
       <c r="P27" s="2"/>
     </row>
     <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="34"/>
-      <c r="B28" s="34"/>
+      <c r="A28" s="25"/>
+      <c r="B28" s="25"/>
       <c r="C28" s="5">
         <v>26</v>
       </c>
@@ -2832,10 +2832,10 @@
       <c r="P28" s="2"/>
     </row>
     <row r="29" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="32" t="s">
+      <c r="A29" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="B29" s="35" t="s">
+      <c r="B29" s="26" t="s">
         <v>12</v>
       </c>
       <c r="C29" s="5">
@@ -2859,8 +2859,8 @@
       <c r="P29" s="2"/>
     </row>
     <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="33"/>
-      <c r="B30" s="33"/>
+      <c r="A30" s="24"/>
+      <c r="B30" s="24"/>
       <c r="C30" s="5">
         <v>28</v>
       </c>
@@ -2882,8 +2882,8 @@
       <c r="P30" s="2"/>
     </row>
     <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="33"/>
-      <c r="B31" s="33"/>
+      <c r="A31" s="24"/>
+      <c r="B31" s="24"/>
       <c r="C31" s="5">
         <v>29</v>
       </c>
@@ -2905,8 +2905,8 @@
       <c r="P31" s="2"/>
     </row>
     <row r="32" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="33"/>
-      <c r="B32" s="33"/>
+      <c r="A32" s="24"/>
+      <c r="B32" s="24"/>
       <c r="C32" s="5">
         <v>30</v>
       </c>
@@ -2928,8 +2928,8 @@
       <c r="P32" s="2"/>
     </row>
     <row r="33" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="33"/>
-      <c r="B33" s="33"/>
+      <c r="A33" s="24"/>
+      <c r="B33" s="24"/>
       <c r="C33" s="5">
         <v>31</v>
       </c>
@@ -2951,8 +2951,8 @@
       <c r="P33" s="2"/>
     </row>
     <row r="34" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="33"/>
-      <c r="B34" s="34"/>
+      <c r="A34" s="24"/>
+      <c r="B34" s="25"/>
       <c r="C34" s="5">
         <v>32</v>
       </c>
@@ -2974,7 +2974,7 @@
       <c r="P34" s="2"/>
     </row>
     <row r="35" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="34"/>
+      <c r="A35" s="25"/>
       <c r="B35" s="14" t="s">
         <v>35</v>
       </c>
@@ -2999,10 +2999,10 @@
       <c r="P35" s="2"/>
     </row>
     <row r="36" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="36" t="s">
+      <c r="A36" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="B36" s="35" t="s">
+      <c r="B36" s="26" t="s">
         <v>12</v>
       </c>
       <c r="C36" s="5">
@@ -3026,8 +3026,8 @@
       <c r="P36" s="2"/>
     </row>
     <row r="37" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="33"/>
-      <c r="B37" s="33"/>
+      <c r="A37" s="24"/>
+      <c r="B37" s="24"/>
       <c r="C37" s="5">
         <v>35</v>
       </c>
@@ -3049,8 +3049,8 @@
       <c r="P37" s="2"/>
     </row>
     <row r="38" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="33"/>
-      <c r="B38" s="33"/>
+      <c r="A38" s="24"/>
+      <c r="B38" s="24"/>
       <c r="C38" s="5">
         <v>36</v>
       </c>
@@ -3072,8 +3072,8 @@
       <c r="P38" s="2"/>
     </row>
     <row r="39" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="33"/>
-      <c r="B39" s="33"/>
+      <c r="A39" s="24"/>
+      <c r="B39" s="24"/>
       <c r="C39" s="5">
         <v>37</v>
       </c>
@@ -3095,8 +3095,8 @@
       <c r="P39" s="2"/>
     </row>
     <row r="40" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="33"/>
-      <c r="B40" s="34"/>
+      <c r="A40" s="24"/>
+      <c r="B40" s="25"/>
       <c r="C40" s="5">
         <v>38</v>
       </c>
@@ -3118,7 +3118,7 @@
       <c r="P40" s="2"/>
     </row>
     <row r="41" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="34"/>
+      <c r="A41" s="25"/>
       <c r="B41" s="14" t="s">
         <v>35</v>
       </c>
@@ -3143,7 +3143,7 @@
       <c r="P41" s="2"/>
     </row>
     <row r="42" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="37" t="s">
+      <c r="A42" s="40" t="s">
         <v>88</v>
       </c>
       <c r="B42" s="15" t="s">
@@ -3170,8 +3170,8 @@
       <c r="P42" s="2"/>
     </row>
     <row r="43" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="33"/>
-      <c r="B43" s="35" t="s">
+      <c r="A43" s="24"/>
+      <c r="B43" s="26" t="s">
         <v>90</v>
       </c>
       <c r="C43" s="5">
@@ -3195,8 +3195,8 @@
       <c r="P43" s="2"/>
     </row>
     <row r="44" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="33"/>
-      <c r="B44" s="33"/>
+      <c r="A44" s="24"/>
+      <c r="B44" s="24"/>
       <c r="C44" s="5">
         <v>42</v>
       </c>
@@ -3218,8 +3218,8 @@
       <c r="P44" s="2"/>
     </row>
     <row r="45" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="33"/>
-      <c r="B45" s="33"/>
+      <c r="A45" s="24"/>
+      <c r="B45" s="24"/>
       <c r="C45" s="5">
         <v>43</v>
       </c>
@@ -3241,8 +3241,8 @@
       <c r="P45" s="2"/>
     </row>
     <row r="46" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="34"/>
-      <c r="B46" s="34"/>
+      <c r="A46" s="25"/>
+      <c r="B46" s="25"/>
       <c r="C46" s="18">
         <v>44</v>
       </c>
@@ -4219,13 +4219,6 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:A13"/>
-    <mergeCell ref="B3:B10"/>
-    <mergeCell ref="B11:B13"/>
     <mergeCell ref="A14:A23"/>
     <mergeCell ref="B21:B23"/>
     <mergeCell ref="A36:A41"/>
@@ -4237,6 +4230,13 @@
     <mergeCell ref="A29:A35"/>
     <mergeCell ref="B29:B34"/>
     <mergeCell ref="B36:B40"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:A13"/>
+    <mergeCell ref="B3:B10"/>
+    <mergeCell ref="B11:B13"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -4263,19 +4263,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="38"/>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="40" t="s">
+      <c r="A1" s="36"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="31"/>
-      <c r="G1" s="40" t="s">
+      <c r="F1" s="35"/>
+      <c r="G1" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
       <c r="J1" s="1"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
@@ -4284,10 +4284,10 @@
       <c r="P1" s="2"/>
     </row>
     <row r="2" spans="1:16" ht="33" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="31"/>
+      <c r="B2" s="35"/>
       <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
@@ -4319,10 +4319,10 @@
       <c r="P2" s="2"/>
     </row>
     <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="26" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="5">
@@ -4346,8 +4346,8 @@
       <c r="P3" s="2"/>
     </row>
     <row r="4" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="33"/>
-      <c r="B4" s="33"/>
+      <c r="A4" s="24"/>
+      <c r="B4" s="24"/>
       <c r="C4" s="5">
         <v>2</v>
       </c>
@@ -4369,8 +4369,8 @@
       <c r="P4" s="2"/>
     </row>
     <row r="5" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="33"/>
-      <c r="B5" s="33"/>
+      <c r="A5" s="24"/>
+      <c r="B5" s="24"/>
       <c r="C5" s="5">
         <v>3</v>
       </c>
@@ -4392,8 +4392,8 @@
       <c r="P5" s="2"/>
     </row>
     <row r="6" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="33"/>
-      <c r="B6" s="33"/>
+      <c r="A6" s="24"/>
+      <c r="B6" s="24"/>
       <c r="C6" s="5">
         <v>4</v>
       </c>
@@ -4415,8 +4415,8 @@
       <c r="P6" s="2"/>
     </row>
     <row r="7" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="33"/>
-      <c r="B7" s="33"/>
+      <c r="A7" s="24"/>
+      <c r="B7" s="24"/>
       <c r="C7" s="5">
         <v>5</v>
       </c>
@@ -4438,8 +4438,8 @@
       <c r="P7" s="2"/>
     </row>
     <row r="8" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="33"/>
-      <c r="B8" s="33"/>
+      <c r="A8" s="24"/>
+      <c r="B8" s="24"/>
       <c r="C8" s="5">
         <v>6</v>
       </c>
@@ -4461,8 +4461,8 @@
       <c r="P8" s="2"/>
     </row>
     <row r="9" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="33"/>
-      <c r="B9" s="33"/>
+      <c r="A9" s="24"/>
+      <c r="B9" s="24"/>
       <c r="C9" s="5">
         <v>7</v>
       </c>
@@ -4484,8 +4484,8 @@
       <c r="P9" s="2"/>
     </row>
     <row r="10" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="33"/>
-      <c r="B10" s="34"/>
+      <c r="A10" s="24"/>
+      <c r="B10" s="25"/>
       <c r="C10" s="5">
         <v>8</v>
       </c>
@@ -4507,8 +4507,8 @@
       <c r="P10" s="2"/>
     </row>
     <row r="11" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="33"/>
-      <c r="B11" s="35" t="s">
+      <c r="A11" s="24"/>
+      <c r="B11" s="26" t="s">
         <v>35</v>
       </c>
       <c r="C11" s="5">
@@ -4532,8 +4532,8 @@
       <c r="P11" s="2"/>
     </row>
     <row r="12" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="33"/>
-      <c r="B12" s="33"/>
+      <c r="A12" s="24"/>
+      <c r="B12" s="24"/>
       <c r="C12" s="5">
         <v>10</v>
       </c>
@@ -4555,8 +4555,8 @@
       <c r="P12" s="2"/>
     </row>
     <row r="13" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="34"/>
-      <c r="B13" s="34"/>
+      <c r="A13" s="25"/>
+      <c r="B13" s="25"/>
       <c r="C13" s="5">
         <v>11</v>
       </c>
@@ -4578,10 +4578,10 @@
       <c r="P13" s="2"/>
     </row>
     <row r="14" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="36" t="s">
+      <c r="A14" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="35" t="s">
+      <c r="B14" s="26" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="5">
@@ -4605,8 +4605,8 @@
       <c r="P14" s="2"/>
     </row>
     <row r="15" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="33"/>
-      <c r="B15" s="33"/>
+      <c r="A15" s="24"/>
+      <c r="B15" s="24"/>
       <c r="C15" s="5">
         <v>13</v>
       </c>
@@ -4628,8 +4628,8 @@
       <c r="P15" s="2"/>
     </row>
     <row r="16" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="33"/>
-      <c r="B16" s="33"/>
+      <c r="A16" s="24"/>
+      <c r="B16" s="24"/>
       <c r="C16" s="5">
         <v>14</v>
       </c>
@@ -4651,8 +4651,8 @@
       <c r="P16" s="2"/>
     </row>
     <row r="17" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="33"/>
-      <c r="B17" s="33"/>
+      <c r="A17" s="24"/>
+      <c r="B17" s="24"/>
       <c r="C17" s="5">
         <v>15</v>
       </c>
@@ -4674,8 +4674,8 @@
       <c r="P17" s="2"/>
     </row>
     <row r="18" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="33"/>
-      <c r="B18" s="33"/>
+      <c r="A18" s="24"/>
+      <c r="B18" s="24"/>
       <c r="C18" s="5">
         <v>16</v>
       </c>
@@ -4697,8 +4697,8 @@
       <c r="P18" s="2"/>
     </row>
     <row r="19" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="33"/>
-      <c r="B19" s="33"/>
+      <c r="A19" s="24"/>
+      <c r="B19" s="24"/>
       <c r="C19" s="5">
         <v>17</v>
       </c>
@@ -4720,8 +4720,8 @@
       <c r="P19" s="2"/>
     </row>
     <row r="20" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="33"/>
-      <c r="B20" s="34"/>
+      <c r="A20" s="24"/>
+      <c r="B20" s="25"/>
       <c r="C20" s="5">
         <v>18</v>
       </c>
@@ -4743,8 +4743,8 @@
       <c r="P20" s="2"/>
     </row>
     <row r="21" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="33"/>
-      <c r="B21" s="35" t="s">
+      <c r="A21" s="24"/>
+      <c r="B21" s="26" t="s">
         <v>35</v>
       </c>
       <c r="C21" s="5">
@@ -4768,8 +4768,8 @@
       <c r="P21" s="2"/>
     </row>
     <row r="22" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="33"/>
-      <c r="B22" s="33"/>
+      <c r="A22" s="24"/>
+      <c r="B22" s="24"/>
       <c r="C22" s="5">
         <v>20</v>
       </c>
@@ -4791,8 +4791,8 @@
       <c r="P22" s="2"/>
     </row>
     <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="34"/>
-      <c r="B23" s="34"/>
+      <c r="A23" s="25"/>
+      <c r="B23" s="25"/>
       <c r="C23" s="5">
         <v>21</v>
       </c>
@@ -4814,10 +4814,10 @@
       <c r="P23" s="2"/>
     </row>
     <row r="24" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="37" t="s">
+      <c r="A24" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="B24" s="35" t="s">
+      <c r="B24" s="26" t="s">
         <v>12</v>
       </c>
       <c r="C24" s="5">
@@ -4841,8 +4841,8 @@
       <c r="P24" s="2"/>
     </row>
     <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="33"/>
-      <c r="B25" s="33"/>
+      <c r="A25" s="24"/>
+      <c r="B25" s="24"/>
       <c r="C25" s="5">
         <v>23</v>
       </c>
@@ -4864,8 +4864,8 @@
       <c r="P25" s="2"/>
     </row>
     <row r="26" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="33"/>
-      <c r="B26" s="33"/>
+      <c r="A26" s="24"/>
+      <c r="B26" s="24"/>
       <c r="C26" s="5">
         <v>24</v>
       </c>
@@ -4887,8 +4887,8 @@
       <c r="P26" s="2"/>
     </row>
     <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="33"/>
-      <c r="B27" s="33"/>
+      <c r="A27" s="24"/>
+      <c r="B27" s="24"/>
       <c r="C27" s="5">
         <v>25</v>
       </c>
@@ -4910,8 +4910,8 @@
       <c r="P27" s="2"/>
     </row>
     <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="34"/>
-      <c r="B28" s="34"/>
+      <c r="A28" s="25"/>
+      <c r="B28" s="25"/>
       <c r="C28" s="5">
         <v>26</v>
       </c>
@@ -4933,10 +4933,10 @@
       <c r="P28" s="2"/>
     </row>
     <row r="29" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="32" t="s">
+      <c r="A29" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="B29" s="35" t="s">
+      <c r="B29" s="26" t="s">
         <v>12</v>
       </c>
       <c r="C29" s="5">
@@ -4960,8 +4960,8 @@
       <c r="P29" s="2"/>
     </row>
     <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="33"/>
-      <c r="B30" s="33"/>
+      <c r="A30" s="24"/>
+      <c r="B30" s="24"/>
       <c r="C30" s="5">
         <v>28</v>
       </c>
@@ -4983,8 +4983,8 @@
       <c r="P30" s="2"/>
     </row>
     <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="33"/>
-      <c r="B31" s="33"/>
+      <c r="A31" s="24"/>
+      <c r="B31" s="24"/>
       <c r="C31" s="5">
         <v>29</v>
       </c>
@@ -5006,8 +5006,8 @@
       <c r="P31" s="2"/>
     </row>
     <row r="32" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="33"/>
-      <c r="B32" s="33"/>
+      <c r="A32" s="24"/>
+      <c r="B32" s="24"/>
       <c r="C32" s="5">
         <v>30</v>
       </c>
@@ -5029,8 +5029,8 @@
       <c r="P32" s="2"/>
     </row>
     <row r="33" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="33"/>
-      <c r="B33" s="33"/>
+      <c r="A33" s="24"/>
+      <c r="B33" s="24"/>
       <c r="C33" s="5">
         <v>31</v>
       </c>
@@ -5052,8 +5052,8 @@
       <c r="P33" s="2"/>
     </row>
     <row r="34" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="33"/>
-      <c r="B34" s="34"/>
+      <c r="A34" s="24"/>
+      <c r="B34" s="25"/>
       <c r="C34" s="5">
         <v>32</v>
       </c>
@@ -5075,7 +5075,7 @@
       <c r="P34" s="2"/>
     </row>
     <row r="35" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="34"/>
+      <c r="A35" s="25"/>
       <c r="B35" s="14" t="s">
         <v>35</v>
       </c>
@@ -5100,10 +5100,10 @@
       <c r="P35" s="2"/>
     </row>
     <row r="36" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="36" t="s">
+      <c r="A36" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="B36" s="35" t="s">
+      <c r="B36" s="26" t="s">
         <v>12</v>
       </c>
       <c r="C36" s="5">
@@ -5127,8 +5127,8 @@
       <c r="P36" s="2"/>
     </row>
     <row r="37" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="33"/>
-      <c r="B37" s="33"/>
+      <c r="A37" s="24"/>
+      <c r="B37" s="24"/>
       <c r="C37" s="5">
         <v>35</v>
       </c>
@@ -5150,8 +5150,8 @@
       <c r="P37" s="2"/>
     </row>
     <row r="38" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="33"/>
-      <c r="B38" s="33"/>
+      <c r="A38" s="24"/>
+      <c r="B38" s="24"/>
       <c r="C38" s="5">
         <v>36</v>
       </c>
@@ -5173,8 +5173,8 @@
       <c r="P38" s="2"/>
     </row>
     <row r="39" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="33"/>
-      <c r="B39" s="33"/>
+      <c r="A39" s="24"/>
+      <c r="B39" s="24"/>
       <c r="C39" s="5">
         <v>37</v>
       </c>
@@ -5196,8 +5196,8 @@
       <c r="P39" s="2"/>
     </row>
     <row r="40" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="33"/>
-      <c r="B40" s="34"/>
+      <c r="A40" s="24"/>
+      <c r="B40" s="25"/>
       <c r="C40" s="5">
         <v>38</v>
       </c>
@@ -5219,7 +5219,7 @@
       <c r="P40" s="2"/>
     </row>
     <row r="41" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="34"/>
+      <c r="A41" s="25"/>
       <c r="B41" s="14" t="s">
         <v>35</v>
       </c>
@@ -5244,7 +5244,7 @@
       <c r="P41" s="2"/>
     </row>
     <row r="42" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="37" t="s">
+      <c r="A42" s="40" t="s">
         <v>88</v>
       </c>
       <c r="B42" s="15" t="s">
@@ -5271,8 +5271,8 @@
       <c r="P42" s="2"/>
     </row>
     <row r="43" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="33"/>
-      <c r="B43" s="35" t="s">
+      <c r="A43" s="24"/>
+      <c r="B43" s="26" t="s">
         <v>90</v>
       </c>
       <c r="C43" s="5">
@@ -5296,8 +5296,8 @@
       <c r="P43" s="2"/>
     </row>
     <row r="44" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="33"/>
-      <c r="B44" s="33"/>
+      <c r="A44" s="24"/>
+      <c r="B44" s="24"/>
       <c r="C44" s="5">
         <v>42</v>
       </c>
@@ -5319,8 +5319,8 @@
       <c r="P44" s="2"/>
     </row>
     <row r="45" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="33"/>
-      <c r="B45" s="33"/>
+      <c r="A45" s="24"/>
+      <c r="B45" s="24"/>
       <c r="C45" s="5">
         <v>43</v>
       </c>
@@ -5342,8 +5342,8 @@
       <c r="P45" s="2"/>
     </row>
     <row r="46" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="34"/>
-      <c r="B46" s="34"/>
+      <c r="A46" s="25"/>
+      <c r="B46" s="25"/>
       <c r="C46" s="18">
         <v>44</v>
       </c>
@@ -6320,13 +6320,6 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:A13"/>
-    <mergeCell ref="B3:B10"/>
-    <mergeCell ref="B11:B13"/>
     <mergeCell ref="A14:A23"/>
     <mergeCell ref="B21:B23"/>
     <mergeCell ref="A36:A41"/>
@@ -6338,6 +6331,13 @@
     <mergeCell ref="A29:A35"/>
     <mergeCell ref="B29:B34"/>
     <mergeCell ref="B36:B40"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:A13"/>
+    <mergeCell ref="B3:B10"/>
+    <mergeCell ref="B11:B13"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
Correção dos Artefatos 15 a 19 + 22 + 31
</commit_message>
<xml_diff>
--- a/Artefatos/17. Análise dos Eventos para cada Cenário.xlsx
+++ b/Artefatos/17. Análise dos Eventos para cada Cenário.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amand\OneDrive\Área de Trabalho\GIT\OPE-Madara\Artefatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87C660AA-7A9D-4D8D-9AA8-E3691BE14C15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{842BF181-082F-4D68-9AB1-FD78ADE9B7C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20520" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="REALIZACAO_MATRICULA" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="102">
   <si>
     <t>Externo</t>
   </si>
@@ -421,12 +421,15 @@
   <si>
     <t>Banco envia extrato de pagamento de boletos</t>
   </si>
+  <si>
+    <t>Secretaria trata inadimpência da primeira mesalidade</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -466,6 +469,12 @@
       <b/>
       <sz val="16"/>
       <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -514,7 +523,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -679,11 +688,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
@@ -778,6 +802,12 @@
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -785,11 +815,11 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1006,10 +1036,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P961"/>
+  <dimension ref="A1:P962"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1126,7 +1156,7 @@
     </row>
     <row r="5" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="24"/>
-      <c r="B5" s="24"/>
+      <c r="B5" s="41"/>
       <c r="C5" s="5">
         <v>2</v>
       </c>
@@ -1135,10 +1165,10 @@
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
-      <c r="G5" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" s="9"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="9" t="s">
+        <v>14</v>
+      </c>
       <c r="I5" s="9"/>
       <c r="J5" s="10"/>
       <c r="L5" s="2"/>
@@ -1148,31 +1178,55 @@
       <c r="P5" s="2"/>
     </row>
     <row r="6" spans="1:16" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="25"/>
-      <c r="B6" s="25"/>
-      <c r="C6" s="5">
+      <c r="A6" s="24"/>
+      <c r="B6" s="41"/>
+      <c r="C6" s="6">
         <v>3</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="7"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="12" t="s">
-        <v>18</v>
-      </c>
+      <c r="F6" s="19"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="21"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
     </row>
-    <row r="7" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:16" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="25"/>
+      <c r="B7" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="5">
+        <v>4</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" s="9"/>
+      <c r="J7" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+    </row>
     <row r="8" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="9" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="10" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2127,15 +2181,16 @@
     <row r="959" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="960" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="961" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="962" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="A4:A7"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="G2:I2"/>
     <mergeCell ref="A3:B3"/>
+    <mergeCell ref="B4:B6"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -2162,19 +2217,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="36"/>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
+      <c r="A1" s="38"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
       <c r="D1" s="35"/>
-      <c r="E1" s="38" t="s">
+      <c r="E1" s="40" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="35"/>
-      <c r="G1" s="38" t="s">
+      <c r="G1" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
       <c r="J1" s="1"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
@@ -2477,7 +2532,7 @@
       <c r="P13" s="2"/>
     </row>
     <row r="14" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="39" t="s">
+      <c r="A14" s="36" t="s">
         <v>39</v>
       </c>
       <c r="B14" s="26" t="s">
@@ -2713,7 +2768,7 @@
       <c r="P23" s="2"/>
     </row>
     <row r="24" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="40" t="s">
+      <c r="A24" s="37" t="s">
         <v>55</v>
       </c>
       <c r="B24" s="26" t="s">
@@ -2999,7 +3054,7 @@
       <c r="P35" s="2"/>
     </row>
     <row r="36" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="39" t="s">
+      <c r="A36" s="36" t="s">
         <v>76</v>
       </c>
       <c r="B36" s="26" t="s">
@@ -3143,7 +3198,7 @@
       <c r="P41" s="2"/>
     </row>
     <row r="42" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="40" t="s">
+      <c r="A42" s="37" t="s">
         <v>88</v>
       </c>
       <c r="B42" s="15" t="s">
@@ -4219,6 +4274,13 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:A13"/>
+    <mergeCell ref="B3:B10"/>
+    <mergeCell ref="B11:B13"/>
     <mergeCell ref="A14:A23"/>
     <mergeCell ref="B21:B23"/>
     <mergeCell ref="A36:A41"/>
@@ -4230,13 +4292,6 @@
     <mergeCell ref="A29:A35"/>
     <mergeCell ref="B29:B34"/>
     <mergeCell ref="B36:B40"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:A13"/>
-    <mergeCell ref="B3:B10"/>
-    <mergeCell ref="B11:B13"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -4263,19 +4318,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="36"/>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
+      <c r="A1" s="38"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
       <c r="D1" s="35"/>
-      <c r="E1" s="38" t="s">
+      <c r="E1" s="40" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="35"/>
-      <c r="G1" s="38" t="s">
+      <c r="G1" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
       <c r="J1" s="1"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
@@ -4578,7 +4633,7 @@
       <c r="P13" s="2"/>
     </row>
     <row r="14" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="39" t="s">
+      <c r="A14" s="36" t="s">
         <v>39</v>
       </c>
       <c r="B14" s="26" t="s">
@@ -4814,7 +4869,7 @@
       <c r="P23" s="2"/>
     </row>
     <row r="24" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="40" t="s">
+      <c r="A24" s="37" t="s">
         <v>55</v>
       </c>
       <c r="B24" s="26" t="s">
@@ -5100,7 +5155,7 @@
       <c r="P35" s="2"/>
     </row>
     <row r="36" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="39" t="s">
+      <c r="A36" s="36" t="s">
         <v>76</v>
       </c>
       <c r="B36" s="26" t="s">
@@ -5244,7 +5299,7 @@
       <c r="P41" s="2"/>
     </row>
     <row r="42" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="40" t="s">
+      <c r="A42" s="37" t="s">
         <v>88</v>
       </c>
       <c r="B42" s="15" t="s">
@@ -6320,6 +6375,13 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:A13"/>
+    <mergeCell ref="B3:B10"/>
+    <mergeCell ref="B11:B13"/>
     <mergeCell ref="A14:A23"/>
     <mergeCell ref="B21:B23"/>
     <mergeCell ref="A36:A41"/>
@@ -6331,13 +6393,6 @@
     <mergeCell ref="A29:A35"/>
     <mergeCell ref="B29:B34"/>
     <mergeCell ref="B36:B40"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:A13"/>
-    <mergeCell ref="B3:B10"/>
-    <mergeCell ref="B11:B13"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
Realização dos Artefatos 15, 16, 17, 18 de cada cenário.
</commit_message>
<xml_diff>
--- a/Artefatos/17. Análise dos Eventos para cada Cenário.xlsx
+++ b/Artefatos/17. Análise dos Eventos para cada Cenário.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amand\OneDrive\Área de Trabalho\GIT\OPE-Madara\Artefatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{842BF181-082F-4D68-9AB1-FD78ADE9B7C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24EE6ECD-5FFD-43ED-89F4-50D0B616BD48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20520" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="111">
   <si>
     <t>Externo</t>
   </si>
@@ -42,6 +42,36 @@
   </si>
   <si>
     <t>Evento</t>
+  </si>
+  <si>
+    <t>Não Previsível</t>
+  </si>
+  <si>
+    <t>Absoluto</t>
+  </si>
+  <si>
+    <t>Extemporâneo</t>
+  </si>
+  <si>
+    <t>Realização de matrícula</t>
+  </si>
+  <si>
+    <t>FB</t>
+  </si>
+  <si>
+    <t>Aluno se inscreve no curso</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Secretaria solicita o extrato da conta</t>
+  </si>
+  <si>
+    <t>X(1)</t>
+  </si>
+  <si>
+    <t>X(2)</t>
   </si>
   <si>
     <r>
@@ -57,9 +87,6 @@
     </r>
   </si>
   <si>
-    <t>Não Previsível</t>
-  </si>
-  <si>
     <r>
       <t>Relativo</t>
     </r>
@@ -73,9 +100,6 @@
     </r>
   </si>
   <si>
-    <t>Absoluto</t>
-  </si>
-  <si>
     <r>
       <t>Não Evento</t>
     </r>
@@ -89,31 +113,226 @@
     </r>
   </si>
   <si>
-    <t>Extemporâneo</t>
-  </si>
-  <si>
-    <t>Realização de matrícula</t>
-  </si>
-  <si>
-    <t>FB</t>
-  </si>
-  <si>
-    <t>Aluno se inscreve no curso</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>Secretaria solicita o extrato da conta</t>
-  </si>
-  <si>
-    <t>X(1)</t>
-  </si>
-  <si>
-    <t>X(2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
+    <t>Aluno entrega documentação e curso desejado</t>
+  </si>
+  <si>
+    <t>Secretária aprova documentação</t>
+  </si>
+  <si>
+    <t>Secretária cadastra o aluno</t>
+  </si>
+  <si>
+    <t>Secretária faz a cobrança da primeira mensalidade</t>
+  </si>
+  <si>
+    <t>X(3)</t>
+  </si>
+  <si>
+    <t>Aluno paga primeira mensalidade</t>
+  </si>
+  <si>
+    <t>X(4)</t>
+  </si>
+  <si>
+    <t>Secretária aprova o pagamento</t>
+  </si>
+  <si>
+    <t>X(5)</t>
+  </si>
+  <si>
+    <t>Secretária inclui o aluno na turma</t>
+  </si>
+  <si>
+    <t>X(6)</t>
+  </si>
+  <si>
+    <t>Finalização da matrícula</t>
+  </si>
+  <si>
+    <t>X(7)</t>
+  </si>
+  <si>
+    <t>FA</t>
+  </si>
+  <si>
+    <t>Secretária reprova da documentação</t>
+  </si>
+  <si>
+    <t>Aluno desiste do curso</t>
+  </si>
+  <si>
+    <t>Pagamento não realizado</t>
+  </si>
+  <si>
+    <t>Participação das aulas</t>
+  </si>
+  <si>
+    <t>Professor leciona aula</t>
+  </si>
+  <si>
+    <t>Aluno comparece à aula</t>
+  </si>
+  <si>
+    <t>X(12)</t>
+  </si>
+  <si>
+    <t>Professor registra presença</t>
+  </si>
+  <si>
+    <t>X(13)</t>
+  </si>
+  <si>
+    <t>Aluno realiza atividades</t>
+  </si>
+  <si>
+    <t>Professor avalia as atividades</t>
+  </si>
+  <si>
+    <t>X(15)</t>
+  </si>
+  <si>
+    <t>Professor registra as notas</t>
+  </si>
+  <si>
+    <t>X(16)</t>
+  </si>
+  <si>
+    <t>Escola valida a conclusão do módulo</t>
+  </si>
+  <si>
+    <t>Aluno não comparece às aulas</t>
+  </si>
+  <si>
+    <t>Professor registra ausência</t>
+  </si>
+  <si>
+    <t>X(19)</t>
+  </si>
+  <si>
+    <t>Aluno não realiza as provas</t>
+  </si>
+  <si>
+    <t>Trancamento de matrícula</t>
+  </si>
+  <si>
+    <t>Aluno solicita trancameto da matrícula</t>
+  </si>
+  <si>
+    <t>Secretária recebe a solicitação</t>
+  </si>
+  <si>
+    <t>X(22)</t>
+  </si>
+  <si>
+    <t>Secretária aprova a solicitação</t>
+  </si>
+  <si>
+    <t>X(23)</t>
+  </si>
+  <si>
+    <t>Secretária suspende cobrança das mensalidades</t>
+  </si>
+  <si>
+    <t>X(24)</t>
+  </si>
+  <si>
+    <t>Aluno é retidado da turma</t>
+  </si>
+  <si>
+    <t>Reabertura de matrícula</t>
+  </si>
+  <si>
+    <t>Aluno solicita reabertura da matrícula</t>
+  </si>
+  <si>
+    <t>Secretária compara cronograma e histórico do aluno</t>
+  </si>
+  <si>
+    <t>X(27)</t>
+  </si>
+  <si>
+    <t>Secretária aprova reabertura da matrícula</t>
+  </si>
+  <si>
+    <t>X(28)</t>
+  </si>
+  <si>
+    <t>Reativação das cobranças de mensalidades</t>
+  </si>
+  <si>
+    <t>X(29)</t>
+  </si>
+  <si>
+    <t>Inclusão do aluno na nova turma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Informa Cronograma da turma </t>
+  </si>
+  <si>
+    <t>X(31)</t>
+  </si>
+  <si>
+    <t>Cronograma não coincide com aulas necessárias para o aluno</t>
+  </si>
+  <si>
+    <t>Transferência  de Turma</t>
+  </si>
+  <si>
+    <t>Aluno solicita transferência de turma</t>
+  </si>
+  <si>
+    <t>Secretária  recebe a solicitação</t>
+  </si>
+  <si>
+    <t>X(34)</t>
+  </si>
+  <si>
+    <t>Secretária consulta cronograma e vagas da turma</t>
+  </si>
+  <si>
+    <t>X(35)</t>
+  </si>
+  <si>
+    <t>Secretária aprova a tranferência</t>
+  </si>
+  <si>
+    <t>X(36)</t>
+  </si>
+  <si>
+    <t>Secretária altera turma do aluno</t>
+  </si>
+  <si>
+    <t>X(37)</t>
+  </si>
+  <si>
+    <t>Não há vaga disponível na turma</t>
+  </si>
+  <si>
+    <t>X(43)</t>
+  </si>
+  <si>
+    <t>Gerir o negócio</t>
+  </si>
+  <si>
+    <t>Cobrança de inadimplências</t>
+  </si>
+  <si>
+    <t>Falha</t>
+  </si>
+  <si>
+    <t>Ineficiência na cobrança das mensalidades</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aluno reclama que não recebeu cobrança da mensalidade </t>
+  </si>
+  <si>
+    <t>X(41)</t>
+  </si>
+  <si>
+    <t>Ineficiência no controle de entrada e saída de alunos das turmas</t>
+  </si>
+  <si>
+    <t>Ineficiência na elaboração de Cronogramas</t>
   </si>
   <si>
     <r>
@@ -155,226 +374,43 @@
     </r>
   </si>
   <si>
-    <t>Aluno entrega documentação e curso desejado</t>
-  </si>
-  <si>
-    <t>Secretária aprova documentação</t>
-  </si>
-  <si>
-    <t>Secretária cadastra o aluno</t>
-  </si>
-  <si>
-    <t>Secretária faz a cobrança da primeira mensalidade</t>
-  </si>
-  <si>
-    <t>X(3)</t>
-  </si>
-  <si>
-    <t>Aluno paga primeira mensalidade</t>
-  </si>
-  <si>
-    <t>X(4)</t>
-  </si>
-  <si>
-    <t>Secretária aprova o pagamento</t>
-  </si>
-  <si>
-    <t>X(5)</t>
-  </si>
-  <si>
-    <t>Secretária inclui o aluno na turma</t>
-  </si>
-  <si>
-    <t>X(6)</t>
-  </si>
-  <si>
-    <t>Finalização da matrícula</t>
-  </si>
-  <si>
-    <t>X(7)</t>
-  </si>
-  <si>
-    <t>FA</t>
-  </si>
-  <si>
-    <t>Secretária reprova da documentação</t>
-  </si>
-  <si>
-    <t>Aluno desiste do curso</t>
-  </si>
-  <si>
-    <t>Pagamento não realizado</t>
-  </si>
-  <si>
-    <t>Participação das aulas</t>
-  </si>
-  <si>
-    <t>Professor leciona aula</t>
-  </si>
-  <si>
-    <t>Aluno comparece à aula</t>
-  </si>
-  <si>
-    <t>X(12)</t>
-  </si>
-  <si>
-    <t>Professor registra presença</t>
-  </si>
-  <si>
-    <t>X(13)</t>
-  </si>
-  <si>
-    <t>Aluno realiza atividades</t>
-  </si>
-  <si>
-    <t>Professor avalia as atividades</t>
-  </si>
-  <si>
-    <t>X(15)</t>
-  </si>
-  <si>
-    <t>Professor registra as notas</t>
-  </si>
-  <si>
-    <t>X(16)</t>
-  </si>
-  <si>
-    <t>Escola valida a conclusão do módulo</t>
-  </si>
-  <si>
-    <t>Aluno não comparece às aulas</t>
-  </si>
-  <si>
-    <t>Professor registra ausência</t>
-  </si>
-  <si>
-    <t>X(19)</t>
-  </si>
-  <si>
-    <t>Aluno não realiza as provas</t>
-  </si>
-  <si>
-    <t>Trancamento de matrícula</t>
-  </si>
-  <si>
-    <t>Aluno solicita trancameto da matrícula</t>
-  </si>
-  <si>
-    <t>Secretária recebe a solicitação</t>
-  </si>
-  <si>
-    <t>X(22)</t>
-  </si>
-  <si>
-    <t>Secretária aprova a solicitação</t>
-  </si>
-  <si>
-    <t>X(23)</t>
-  </si>
-  <si>
-    <t>Secretária suspende cobrança das mensalidades</t>
-  </si>
-  <si>
-    <t>X(24)</t>
-  </si>
-  <si>
-    <t>Aluno é retidado da turma</t>
-  </si>
-  <si>
-    <t>Reabertura de matrícula</t>
-  </si>
-  <si>
-    <t>Aluno solicita reabertura da matrícula</t>
-  </si>
-  <si>
-    <t>Secretária compara cronograma e histórico do aluno</t>
-  </si>
-  <si>
-    <t>X(27)</t>
-  </si>
-  <si>
-    <t>Secretária aprova reabertura da matrícula</t>
-  </si>
-  <si>
-    <t>X(28)</t>
-  </si>
-  <si>
-    <t>Reativação das cobranças de mensalidades</t>
-  </si>
-  <si>
-    <t>X(29)</t>
-  </si>
-  <si>
-    <t>Inclusão do aluno na nova turma</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Informa Cronograma da turma </t>
-  </si>
-  <si>
-    <t>X(31)</t>
-  </si>
-  <si>
-    <t>Cronograma não coincide com aulas necessárias para o aluno</t>
-  </si>
-  <si>
-    <t>Transferência  de Turma</t>
-  </si>
-  <si>
-    <t>Aluno solicita transferência de turma</t>
-  </si>
-  <si>
-    <t>Secretária  recebe a solicitação</t>
-  </si>
-  <si>
-    <t>X(34)</t>
-  </si>
-  <si>
-    <t>Secretária consulta cronograma e vagas da turma</t>
-  </si>
-  <si>
-    <t>X(35)</t>
-  </si>
-  <si>
-    <t>Secretária aprova a tranferência</t>
-  </si>
-  <si>
-    <t>X(36)</t>
-  </si>
-  <si>
-    <t>Secretária altera turma do aluno</t>
-  </si>
-  <si>
-    <t>X(37)</t>
-  </si>
-  <si>
-    <t>Não há vaga disponível na turma</t>
-  </si>
-  <si>
-    <t>X(43)</t>
-  </si>
-  <si>
-    <t>Gerir o negócio</t>
-  </si>
-  <si>
-    <t>Cobrança de inadimplências</t>
-  </si>
-  <si>
-    <t>Falha</t>
-  </si>
-  <si>
-    <t>Ineficiência na cobrança das mensalidades</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aluno reclama que não recebeu cobrança da mensalidade </t>
-  </si>
-  <si>
-    <t>X(41)</t>
-  </si>
-  <si>
-    <t>Ineficiência no controle de entrada e saída de alunos das turmas</t>
-  </si>
-  <si>
-    <t>Ineficiência na elaboração de Cronogramas</t>
+    <t>Análise dos Eventos para cada Cenário</t>
+  </si>
+  <si>
+    <t>Banco envia extrato de pagamento de boletos</t>
+  </si>
+  <si>
+    <t>Secretaria trata resposta da posição do aluno</t>
+  </si>
+  <si>
+    <t>Ministrar Aulas</t>
+  </si>
+  <si>
+    <t>Professor realiza chamada</t>
+  </si>
+  <si>
+    <t>Professor aplica atividade</t>
+  </si>
+  <si>
+    <t>Negociar</t>
+  </si>
+  <si>
+    <t>Secretaria trata inadimplência dos alunos</t>
+  </si>
+  <si>
+    <t>Transferência</t>
+  </si>
+  <si>
+    <t>Aluno solicita transferência de curso</t>
+  </si>
+  <si>
+    <t>Trancamento</t>
+  </si>
+  <si>
+    <t>Aluno solicita o trancamento de matricula</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
   <si>
     <r>
@@ -382,9 +418,10 @@
     </r>
     <r>
       <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <rFont val="Arial"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
       <t>*</t>
     </r>
@@ -395,9 +432,10 @@
     </r>
     <r>
       <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <rFont val="Arial"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
       <t>*</t>
     </r>
@@ -408,28 +446,20 @@
     </r>
     <r>
       <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <rFont val="Arial"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
       <t>*</t>
     </r>
-  </si>
-  <si>
-    <t>Análise dos Eventos para cada Cenário</t>
-  </si>
-  <si>
-    <t>Banco envia extrato de pagamento de boletos</t>
-  </si>
-  <si>
-    <t>Secretaria trata inadimpência da primeira mesalidade</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -475,11 +505,38 @@
     <font>
       <b/>
       <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -522,8 +579,56 @@
         <bgColor rgb="FFB6D7A8"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFBFEBE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBBE0E3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFDE9D9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC9DAF8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="15">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -621,85 +726,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="medium">
+      <right style="thin">
         <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -707,7 +744,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
@@ -742,9 +779,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
@@ -770,42 +804,16 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -815,11 +823,77 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1039,7 +1113,7 @@
   <dimension ref="A1:P962"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1057,69 +1131,69 @@
     <col min="11" max="26" width="7.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="29"/>
+    <row r="1" spans="1:16" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A1" s="47" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
     </row>
     <row r="2" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="30"/>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
+      <c r="A2" s="32"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
       <c r="D2" s="32"/>
-      <c r="E2" s="33" t="s">
+      <c r="E2" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="32"/>
-      <c r="G2" s="33" t="s">
+      <c r="F2" s="51"/>
+      <c r="G2" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="22"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="33"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
     </row>
-    <row r="3" spans="1:16" ht="33" x14ac:dyDescent="0.25">
-      <c r="A3" s="34" t="s">
+    <row r="3" spans="1:16" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A3" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="35"/>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="48"/>
+      <c r="C3" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="50" t="s">
+        <v>108</v>
+      </c>
+      <c r="F3" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="50" t="s">
+        <v>109</v>
+      </c>
+      <c r="H3" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="I3" s="50" t="s">
+        <v>110</v>
+      </c>
+      <c r="J3" s="50" t="s">
         <v>7</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>10</v>
       </c>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
@@ -1128,26 +1202,26 @@
       <c r="P3" s="2"/>
     </row>
     <row r="4" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="36">
+        <v>1</v>
+      </c>
+      <c r="D4" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="5">
-        <v>1</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="10"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="39"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
@@ -1155,45 +1229,45 @@
       <c r="P4" s="2"/>
     </row>
     <row r="5" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="24"/>
-      <c r="B5" s="41"/>
-      <c r="C5" s="5">
+      <c r="A5" s="34"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="36">
         <v>2</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" s="9"/>
-      <c r="J5" s="10"/>
+      <c r="D5" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="38"/>
+      <c r="J5" s="39"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
+      <c r="N5" s="53"/>
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
     </row>
     <row r="6" spans="1:16" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="24"/>
-      <c r="B6" s="41"/>
-      <c r="C6" s="6">
+      <c r="A6" s="34"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="36">
         <v>3</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="E6" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="19"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="21"/>
+      <c r="D6" s="36" t="s">
+        <v>96</v>
+      </c>
+      <c r="E6" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="37"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="38"/>
+      <c r="J6" s="39"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
@@ -1201,37 +1275,136 @@
       <c r="P6" s="2"/>
     </row>
     <row r="7" spans="1:16" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="25"/>
-      <c r="B7" s="42" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" s="5">
+      <c r="A7" s="34"/>
+      <c r="B7" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="36">
         <v>4</v>
       </c>
-      <c r="D7" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="I7" s="9"/>
-      <c r="J7" s="12" t="s">
-        <v>18</v>
-      </c>
+      <c r="D7" s="36" t="s">
+        <v>97</v>
+      </c>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="I7" s="38"/>
+      <c r="J7" s="39"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
     </row>
-    <row r="8" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:16" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="43" t="s">
+        <v>98</v>
+      </c>
+      <c r="B8" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="36">
+        <v>5</v>
+      </c>
+      <c r="D8" s="36" t="s">
+        <v>99</v>
+      </c>
+      <c r="E8" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="40"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="44"/>
+      <c r="I8" s="38"/>
+      <c r="J8" s="39"/>
+    </row>
+    <row r="9" spans="1:16" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="43"/>
+      <c r="B9" s="35"/>
+      <c r="C9" s="36">
+        <v>6</v>
+      </c>
+      <c r="D9" s="36" t="s">
+        <v>100</v>
+      </c>
+      <c r="E9" s="37"/>
+      <c r="F9" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="38"/>
+      <c r="H9" s="44"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="39"/>
+    </row>
+    <row r="10" spans="1:16" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="45" t="s">
+        <v>101</v>
+      </c>
+      <c r="B10" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="36">
+        <v>7</v>
+      </c>
+      <c r="D10" s="36" t="s">
+        <v>102</v>
+      </c>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="I10" s="38"/>
+      <c r="J10" s="39"/>
+    </row>
+    <row r="11" spans="1:16" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="46" t="s">
+        <v>103</v>
+      </c>
+      <c r="B11" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="36">
+        <v>8</v>
+      </c>
+      <c r="D11" s="36" t="s">
+        <v>104</v>
+      </c>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="38"/>
+      <c r="J11" s="39"/>
+    </row>
+    <row r="12" spans="1:16" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="45" t="s">
+        <v>105</v>
+      </c>
+      <c r="B12" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="36">
+        <v>9</v>
+      </c>
+      <c r="D12" s="36" t="s">
+        <v>106</v>
+      </c>
+      <c r="E12" s="37"/>
+      <c r="F12" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="39"/>
+    </row>
     <row r="13" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="14" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="15" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2183,7 +2356,9 @@
     <row r="961" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="962" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="9">
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
     <mergeCell ref="A4:A7"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:D2"/>
@@ -2217,19 +2392,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="38"/>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="40" t="s">
+      <c r="A1" s="27"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="35"/>
-      <c r="G1" s="40" t="s">
+      <c r="F1" s="25"/>
+      <c r="G1" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
       <c r="J1" s="1"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
@@ -2238,10 +2413,10 @@
       <c r="P1" s="2"/>
     </row>
     <row r="2" spans="1:16" ht="33" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="35"/>
+      <c r="B2" s="25"/>
       <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
@@ -2249,22 +2424,22 @@
         <v>4</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>8</v>
-      </c>
       <c r="I2" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
@@ -2273,21 +2448,21 @@
       <c r="P2" s="2"/>
     </row>
     <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
-        <v>11</v>
+      <c r="A3" s="21" t="s">
+        <v>8</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C3" s="5">
         <v>1</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="8" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G3" s="9"/>
       <c r="H3" s="9"/>
@@ -2300,18 +2475,18 @@
       <c r="P3" s="2"/>
     </row>
     <row r="4" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="24"/>
-      <c r="B4" s="24"/>
+      <c r="A4" s="22"/>
+      <c r="B4" s="22"/>
       <c r="C4" s="5">
         <v>2</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
       <c r="G4" s="11" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
@@ -2323,18 +2498,18 @@
       <c r="P4" s="2"/>
     </row>
     <row r="5" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="24"/>
-      <c r="B5" s="24"/>
+      <c r="A5" s="22"/>
+      <c r="B5" s="22"/>
       <c r="C5" s="5">
         <v>3</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
       <c r="G5" s="11" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H5" s="9"/>
       <c r="I5" s="9"/>
@@ -2346,18 +2521,18 @@
       <c r="P5" s="2"/>
     </row>
     <row r="6" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="24"/>
-      <c r="B6" s="24"/>
+      <c r="A6" s="22"/>
+      <c r="B6" s="22"/>
       <c r="C6" s="5">
         <v>4</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
       <c r="G6" s="11" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
@@ -2369,16 +2544,16 @@
       <c r="P6" s="2"/>
     </row>
     <row r="7" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="24"/>
-      <c r="B7" s="24"/>
+      <c r="A7" s="22"/>
+      <c r="B7" s="22"/>
       <c r="C7" s="5">
         <v>5</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="9"/>
@@ -2392,18 +2567,18 @@
       <c r="P7" s="2"/>
     </row>
     <row r="8" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="24"/>
-      <c r="B8" s="24"/>
+      <c r="A8" s="22"/>
+      <c r="B8" s="22"/>
       <c r="C8" s="5">
         <v>6</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="G8" s="11" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
@@ -2415,18 +2590,18 @@
       <c r="P8" s="2"/>
     </row>
     <row r="9" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="24"/>
-      <c r="B9" s="24"/>
+      <c r="A9" s="22"/>
+      <c r="B9" s="22"/>
       <c r="C9" s="5">
         <v>7</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
       <c r="G9" s="11" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
@@ -2438,18 +2613,18 @@
       <c r="P9" s="2"/>
     </row>
     <row r="10" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="24"/>
-      <c r="B10" s="25"/>
+      <c r="A10" s="22"/>
+      <c r="B10" s="23"/>
       <c r="C10" s="5">
         <v>8</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
       <c r="G10" s="11" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
@@ -2461,20 +2636,20 @@
       <c r="P10" s="2"/>
     </row>
     <row r="11" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="24"/>
+      <c r="A11" s="22"/>
       <c r="B11" s="26" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C11" s="5">
         <v>9</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
       <c r="G11" s="11" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
@@ -2486,16 +2661,16 @@
       <c r="P11" s="2"/>
     </row>
     <row r="12" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="24"/>
-      <c r="B12" s="24"/>
+      <c r="A12" s="22"/>
+      <c r="B12" s="22"/>
       <c r="C12" s="5">
         <v>10</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F12" s="7"/>
       <c r="G12" s="9"/>
@@ -2509,20 +2684,20 @@
       <c r="P12" s="2"/>
     </row>
     <row r="13" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="25"/>
-      <c r="B13" s="25"/>
+      <c r="A13" s="23"/>
+      <c r="B13" s="23"/>
       <c r="C13" s="5">
         <v>11</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
       <c r="I13" s="11" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="J13" s="10"/>
       <c r="L13" s="2"/>
@@ -2532,23 +2707,23 @@
       <c r="P13" s="2"/>
     </row>
     <row r="14" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="36" t="s">
-        <v>39</v>
+      <c r="A14" s="30" t="s">
+        <v>35</v>
       </c>
       <c r="B14" s="26" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C14" s="5">
         <v>12</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
       <c r="G14" s="9"/>
       <c r="H14" s="11" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="I14" s="9"/>
       <c r="J14" s="10"/>
@@ -2559,16 +2734,16 @@
       <c r="P14" s="2"/>
     </row>
     <row r="15" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="24"/>
-      <c r="B15" s="24"/>
+      <c r="A15" s="22"/>
+      <c r="B15" s="22"/>
       <c r="C15" s="5">
         <v>13</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F15" s="7"/>
       <c r="G15" s="9"/>
@@ -2582,18 +2757,18 @@
       <c r="P15" s="2"/>
     </row>
     <row r="16" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="24"/>
-      <c r="B16" s="24"/>
+      <c r="A16" s="22"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="5">
         <v>14</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
       <c r="G16" s="11" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="H16" s="9"/>
       <c r="I16" s="9"/>
@@ -2605,16 +2780,16 @@
       <c r="P16" s="2"/>
     </row>
     <row r="17" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="24"/>
-      <c r="B17" s="24"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="5">
         <v>15</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F17" s="7"/>
       <c r="G17" s="9"/>
@@ -2628,18 +2803,18 @@
       <c r="P17" s="2"/>
     </row>
     <row r="18" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="24"/>
-      <c r="B18" s="24"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="5">
         <v>16</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
       <c r="G18" s="11" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="H18" s="9"/>
       <c r="I18" s="9"/>
@@ -2651,18 +2826,18 @@
       <c r="P18" s="2"/>
     </row>
     <row r="19" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="24"/>
-      <c r="B19" s="24"/>
+      <c r="A19" s="22"/>
+      <c r="B19" s="22"/>
       <c r="C19" s="5">
         <v>17</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
       <c r="G19" s="11" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="H19" s="9"/>
       <c r="I19" s="9"/>
@@ -2674,19 +2849,19 @@
       <c r="P19" s="2"/>
     </row>
     <row r="20" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="24"/>
-      <c r="B20" s="25"/>
+      <c r="A20" s="22"/>
+      <c r="B20" s="23"/>
       <c r="C20" s="5">
         <v>18</v>
       </c>
-      <c r="D20" s="13" t="s">
-        <v>50</v>
+      <c r="D20" s="12" t="s">
+        <v>46</v>
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
       <c r="G20" s="9"/>
       <c r="H20" s="11" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="I20" s="9"/>
       <c r="J20" s="10"/>
@@ -2697,18 +2872,18 @@
       <c r="P20" s="2"/>
     </row>
     <row r="21" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="24"/>
+      <c r="A21" s="22"/>
       <c r="B21" s="26" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C21" s="5">
         <v>19</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="9"/>
@@ -2722,18 +2897,18 @@
       <c r="P21" s="2"/>
     </row>
     <row r="22" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="24"/>
-      <c r="B22" s="24"/>
+      <c r="A22" s="22"/>
+      <c r="B22" s="22"/>
       <c r="C22" s="5">
         <v>20</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
       <c r="G22" s="11" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>
@@ -2745,17 +2920,17 @@
       <c r="P22" s="2"/>
     </row>
     <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="25"/>
-      <c r="B23" s="25"/>
+      <c r="A23" s="23"/>
+      <c r="B23" s="23"/>
       <c r="C23" s="5">
         <v>21</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E23" s="7"/>
       <c r="F23" s="8" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G23" s="9"/>
       <c r="H23" s="9"/>
@@ -2768,21 +2943,21 @@
       <c r="P23" s="2"/>
     </row>
     <row r="24" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="37" t="s">
-        <v>55</v>
+      <c r="A24" s="31" t="s">
+        <v>51</v>
       </c>
       <c r="B24" s="26" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C24" s="5">
         <v>22</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E24" s="7"/>
       <c r="F24" s="8" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G24" s="9"/>
       <c r="H24" s="9"/>
@@ -2795,18 +2970,18 @@
       <c r="P24" s="2"/>
     </row>
     <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="24"/>
-      <c r="B25" s="24"/>
+      <c r="A25" s="22"/>
+      <c r="B25" s="22"/>
       <c r="C25" s="5">
         <v>23</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
       <c r="G25" s="11" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="H25" s="9"/>
       <c r="I25" s="9"/>
@@ -2818,18 +2993,18 @@
       <c r="P25" s="2"/>
     </row>
     <row r="26" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="24"/>
-      <c r="B26" s="24"/>
+      <c r="A26" s="22"/>
+      <c r="B26" s="22"/>
       <c r="C26" s="5">
         <v>24</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
       <c r="G26" s="11" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="H26" s="9"/>
       <c r="I26" s="9"/>
@@ -2841,18 +3016,18 @@
       <c r="P26" s="2"/>
     </row>
     <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="24"/>
-      <c r="B27" s="24"/>
+      <c r="A27" s="22"/>
+      <c r="B27" s="22"/>
       <c r="C27" s="5">
         <v>25</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
       <c r="G27" s="11" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="H27" s="9"/>
       <c r="I27" s="9"/>
@@ -2864,18 +3039,18 @@
       <c r="P27" s="2"/>
     </row>
     <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="25"/>
-      <c r="B28" s="25"/>
+      <c r="A28" s="23"/>
+      <c r="B28" s="23"/>
       <c r="C28" s="5">
         <v>26</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E28" s="7"/>
       <c r="F28" s="7"/>
       <c r="G28" s="11" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="H28" s="9"/>
       <c r="I28" s="9"/>
@@ -2887,21 +3062,21 @@
       <c r="P28" s="2"/>
     </row>
     <row r="29" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="23" t="s">
-        <v>64</v>
+      <c r="A29" s="21" t="s">
+        <v>60</v>
       </c>
       <c r="B29" s="26" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C29" s="5">
         <v>27</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E29" s="7"/>
       <c r="F29" s="8" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G29" s="9"/>
       <c r="H29" s="9"/>
@@ -2914,18 +3089,18 @@
       <c r="P29" s="2"/>
     </row>
     <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="24"/>
-      <c r="B30" s="24"/>
+      <c r="A30" s="22"/>
+      <c r="B30" s="22"/>
       <c r="C30" s="5">
         <v>28</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E30" s="7"/>
       <c r="F30" s="7"/>
       <c r="G30" s="11" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="H30" s="9"/>
       <c r="I30" s="9"/>
@@ -2937,18 +3112,18 @@
       <c r="P30" s="2"/>
     </row>
     <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="24"/>
-      <c r="B31" s="24"/>
+      <c r="A31" s="22"/>
+      <c r="B31" s="22"/>
       <c r="C31" s="5">
         <v>29</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
       <c r="G31" s="11" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="H31" s="9"/>
       <c r="I31" s="9"/>
@@ -2960,18 +3135,18 @@
       <c r="P31" s="2"/>
     </row>
     <row r="32" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="24"/>
-      <c r="B32" s="24"/>
+      <c r="A32" s="22"/>
+      <c r="B32" s="22"/>
       <c r="C32" s="5">
         <v>30</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E32" s="7"/>
       <c r="F32" s="7"/>
       <c r="G32" s="11" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="H32" s="9"/>
       <c r="I32" s="9"/>
@@ -2983,18 +3158,18 @@
       <c r="P32" s="2"/>
     </row>
     <row r="33" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="24"/>
-      <c r="B33" s="24"/>
+      <c r="A33" s="22"/>
+      <c r="B33" s="22"/>
       <c r="C33" s="5">
         <v>31</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
       <c r="G33" s="11" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="H33" s="9"/>
       <c r="I33" s="9"/>
@@ -3006,18 +3181,18 @@
       <c r="P33" s="2"/>
     </row>
     <row r="34" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="24"/>
-      <c r="B34" s="25"/>
+      <c r="A34" s="22"/>
+      <c r="B34" s="23"/>
       <c r="C34" s="5">
         <v>32</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E34" s="7"/>
       <c r="F34" s="7"/>
       <c r="G34" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="H34" s="9"/>
       <c r="I34" s="9"/>
@@ -3029,20 +3204,20 @@
       <c r="P34" s="2"/>
     </row>
     <row r="35" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="25"/>
-      <c r="B35" s="14" t="s">
-        <v>35</v>
+      <c r="A35" s="23"/>
+      <c r="B35" s="13" t="s">
+        <v>31</v>
       </c>
       <c r="C35" s="5">
         <v>33</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E35" s="7"/>
       <c r="F35" s="7"/>
       <c r="G35" s="11" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="H35" s="9"/>
       <c r="I35" s="9"/>
@@ -3054,21 +3229,21 @@
       <c r="P35" s="2"/>
     </row>
     <row r="36" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="36" t="s">
-        <v>76</v>
+      <c r="A36" s="30" t="s">
+        <v>72</v>
       </c>
       <c r="B36" s="26" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C36" s="5">
         <v>34</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E36" s="7"/>
       <c r="F36" s="8" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G36" s="9"/>
       <c r="H36" s="9"/>
@@ -3081,18 +3256,18 @@
       <c r="P36" s="2"/>
     </row>
     <row r="37" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="24"/>
-      <c r="B37" s="24"/>
+      <c r="A37" s="22"/>
+      <c r="B37" s="22"/>
       <c r="C37" s="5">
         <v>35</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E37" s="7"/>
       <c r="F37" s="7"/>
       <c r="G37" s="11" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="H37" s="9"/>
       <c r="I37" s="9"/>
@@ -3104,18 +3279,18 @@
       <c r="P37" s="2"/>
     </row>
     <row r="38" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="24"/>
-      <c r="B38" s="24"/>
+      <c r="A38" s="22"/>
+      <c r="B38" s="22"/>
       <c r="C38" s="5">
         <v>36</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E38" s="7"/>
       <c r="F38" s="7"/>
       <c r="G38" s="11" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H38" s="9"/>
       <c r="I38" s="9"/>
@@ -3127,18 +3302,18 @@
       <c r="P38" s="2"/>
     </row>
     <row r="39" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="24"/>
-      <c r="B39" s="24"/>
+      <c r="A39" s="22"/>
+      <c r="B39" s="22"/>
       <c r="C39" s="5">
         <v>37</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E39" s="7"/>
       <c r="F39" s="7"/>
       <c r="G39" s="11" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="H39" s="9"/>
       <c r="I39" s="9"/>
@@ -3150,18 +3325,18 @@
       <c r="P39" s="2"/>
     </row>
     <row r="40" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="24"/>
-      <c r="B40" s="25"/>
+      <c r="A40" s="22"/>
+      <c r="B40" s="23"/>
       <c r="C40" s="5">
         <v>38</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E40" s="7"/>
       <c r="F40" s="7"/>
       <c r="G40" s="11" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="H40" s="9"/>
       <c r="I40" s="9"/>
@@ -3173,20 +3348,20 @@
       <c r="P40" s="2"/>
     </row>
     <row r="41" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="25"/>
-      <c r="B41" s="14" t="s">
-        <v>35</v>
+      <c r="A41" s="23"/>
+      <c r="B41" s="13" t="s">
+        <v>31</v>
       </c>
       <c r="C41" s="5">
         <v>39</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
       <c r="G41" s="11" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="H41" s="9"/>
       <c r="I41" s="9"/>
@@ -3198,25 +3373,25 @@
       <c r="P41" s="2"/>
     </row>
     <row r="42" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="37" t="s">
-        <v>88</v>
-      </c>
-      <c r="B42" s="15" t="s">
-        <v>12</v>
+      <c r="A42" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="B42" s="14" t="s">
+        <v>9</v>
       </c>
       <c r="C42" s="5">
         <v>40</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="9"/>
       <c r="H42" s="9"/>
       <c r="I42" s="9"/>
-      <c r="J42" s="16" t="s">
-        <v>14</v>
+      <c r="J42" s="15" t="s">
+        <v>11</v>
       </c>
       <c r="L42" s="2"/>
       <c r="M42" s="2"/>
@@ -3225,22 +3400,22 @@
       <c r="P42" s="2"/>
     </row>
     <row r="43" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="24"/>
+      <c r="A43" s="22"/>
       <c r="B43" s="26" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C43" s="5">
         <v>41</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="9"/>
       <c r="H43" s="9"/>
-      <c r="I43" s="17" t="s">
-        <v>34</v>
+      <c r="I43" s="16" t="s">
+        <v>30</v>
       </c>
       <c r="J43" s="10"/>
       <c r="L43" s="2"/>
@@ -3250,16 +3425,16 @@
       <c r="P43" s="2"/>
     </row>
     <row r="44" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="24"/>
-      <c r="B44" s="24"/>
+      <c r="A44" s="22"/>
+      <c r="B44" s="22"/>
       <c r="C44" s="5">
         <v>42</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E44" s="8" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F44" s="7"/>
       <c r="G44" s="9"/>
@@ -3273,20 +3448,20 @@
       <c r="P44" s="2"/>
     </row>
     <row r="45" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="24"/>
-      <c r="B45" s="24"/>
+      <c r="A45" s="22"/>
+      <c r="B45" s="22"/>
       <c r="C45" s="5">
         <v>43</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E45" s="7"/>
       <c r="F45" s="7"/>
       <c r="G45" s="9"/>
       <c r="H45" s="9"/>
-      <c r="I45" s="17" t="s">
-        <v>34</v>
+      <c r="I45" s="16" t="s">
+        <v>30</v>
       </c>
       <c r="J45" s="10"/>
       <c r="L45" s="2"/>
@@ -3296,22 +3471,22 @@
       <c r="P45" s="2"/>
     </row>
     <row r="46" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="25"/>
-      <c r="B46" s="25"/>
-      <c r="C46" s="18">
+      <c r="A46" s="23"/>
+      <c r="B46" s="23"/>
+      <c r="C46" s="17">
         <v>44</v>
       </c>
-      <c r="D46" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="E46" s="19"/>
-      <c r="F46" s="19"/>
-      <c r="G46" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="H46" s="20"/>
-      <c r="I46" s="20"/>
-      <c r="J46" s="21"/>
+      <c r="D46" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="E46" s="18"/>
+      <c r="F46" s="18"/>
+      <c r="G46" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="H46" s="19"/>
+      <c r="I46" s="19"/>
+      <c r="J46" s="20"/>
       <c r="L46" s="2"/>
       <c r="M46" s="2"/>
       <c r="N46" s="2"/>
@@ -4274,13 +4449,6 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:A13"/>
-    <mergeCell ref="B3:B10"/>
-    <mergeCell ref="B11:B13"/>
     <mergeCell ref="A14:A23"/>
     <mergeCell ref="B21:B23"/>
     <mergeCell ref="A36:A41"/>
@@ -4292,6 +4460,13 @@
     <mergeCell ref="A29:A35"/>
     <mergeCell ref="B29:B34"/>
     <mergeCell ref="B36:B40"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:A13"/>
+    <mergeCell ref="B3:B10"/>
+    <mergeCell ref="B11:B13"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -4318,19 +4493,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="38"/>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="40" t="s">
+      <c r="A1" s="27"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="35"/>
-      <c r="G1" s="40" t="s">
+      <c r="F1" s="25"/>
+      <c r="G1" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
       <c r="J1" s="1"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
@@ -4339,10 +4514,10 @@
       <c r="P1" s="2"/>
     </row>
     <row r="2" spans="1:16" ht="33" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="35"/>
+      <c r="B2" s="25"/>
       <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
@@ -4350,22 +4525,22 @@
         <v>4</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="F2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>8</v>
-      </c>
       <c r="I2" s="4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
@@ -4374,21 +4549,21 @@
       <c r="P2" s="2"/>
     </row>
     <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
-        <v>11</v>
+      <c r="A3" s="21" t="s">
+        <v>8</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C3" s="5">
         <v>1</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="8" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G3" s="9"/>
       <c r="H3" s="9"/>
@@ -4401,18 +4576,18 @@
       <c r="P3" s="2"/>
     </row>
     <row r="4" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="24"/>
-      <c r="B4" s="24"/>
+      <c r="A4" s="22"/>
+      <c r="B4" s="22"/>
       <c r="C4" s="5">
         <v>2</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
       <c r="G4" s="11" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
@@ -4424,18 +4599,18 @@
       <c r="P4" s="2"/>
     </row>
     <row r="5" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="24"/>
-      <c r="B5" s="24"/>
+      <c r="A5" s="22"/>
+      <c r="B5" s="22"/>
       <c r="C5" s="5">
         <v>3</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
       <c r="G5" s="11" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H5" s="9"/>
       <c r="I5" s="9"/>
@@ -4447,18 +4622,18 @@
       <c r="P5" s="2"/>
     </row>
     <row r="6" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="24"/>
-      <c r="B6" s="24"/>
+      <c r="A6" s="22"/>
+      <c r="B6" s="22"/>
       <c r="C6" s="5">
         <v>4</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
       <c r="G6" s="11" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
@@ -4470,16 +4645,16 @@
       <c r="P6" s="2"/>
     </row>
     <row r="7" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="24"/>
-      <c r="B7" s="24"/>
+      <c r="A7" s="22"/>
+      <c r="B7" s="22"/>
       <c r="C7" s="5">
         <v>5</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="9"/>
@@ -4493,18 +4668,18 @@
       <c r="P7" s="2"/>
     </row>
     <row r="8" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="24"/>
-      <c r="B8" s="24"/>
+      <c r="A8" s="22"/>
+      <c r="B8" s="22"/>
       <c r="C8" s="5">
         <v>6</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="G8" s="11" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
@@ -4516,18 +4691,18 @@
       <c r="P8" s="2"/>
     </row>
     <row r="9" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="24"/>
-      <c r="B9" s="24"/>
+      <c r="A9" s="22"/>
+      <c r="B9" s="22"/>
       <c r="C9" s="5">
         <v>7</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
       <c r="G9" s="11" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
@@ -4539,18 +4714,18 @@
       <c r="P9" s="2"/>
     </row>
     <row r="10" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="24"/>
-      <c r="B10" s="25"/>
+      <c r="A10" s="22"/>
+      <c r="B10" s="23"/>
       <c r="C10" s="5">
         <v>8</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
       <c r="G10" s="11" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
@@ -4562,20 +4737,20 @@
       <c r="P10" s="2"/>
     </row>
     <row r="11" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="24"/>
+      <c r="A11" s="22"/>
       <c r="B11" s="26" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C11" s="5">
         <v>9</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
       <c r="G11" s="11" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
@@ -4587,16 +4762,16 @@
       <c r="P11" s="2"/>
     </row>
     <row r="12" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="24"/>
-      <c r="B12" s="24"/>
+      <c r="A12" s="22"/>
+      <c r="B12" s="22"/>
       <c r="C12" s="5">
         <v>10</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F12" s="7"/>
       <c r="G12" s="9"/>
@@ -4610,20 +4785,20 @@
       <c r="P12" s="2"/>
     </row>
     <row r="13" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="25"/>
-      <c r="B13" s="25"/>
+      <c r="A13" s="23"/>
+      <c r="B13" s="23"/>
       <c r="C13" s="5">
         <v>11</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
       <c r="I13" s="11" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="J13" s="10"/>
       <c r="L13" s="2"/>
@@ -4633,23 +4808,23 @@
       <c r="P13" s="2"/>
     </row>
     <row r="14" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="36" t="s">
-        <v>39</v>
+      <c r="A14" s="30" t="s">
+        <v>35</v>
       </c>
       <c r="B14" s="26" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C14" s="5">
         <v>12</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
       <c r="G14" s="9"/>
       <c r="H14" s="11" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="I14" s="9"/>
       <c r="J14" s="10"/>
@@ -4660,16 +4835,16 @@
       <c r="P14" s="2"/>
     </row>
     <row r="15" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="24"/>
-      <c r="B15" s="24"/>
+      <c r="A15" s="22"/>
+      <c r="B15" s="22"/>
       <c r="C15" s="5">
         <v>13</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F15" s="7"/>
       <c r="G15" s="9"/>
@@ -4683,18 +4858,18 @@
       <c r="P15" s="2"/>
     </row>
     <row r="16" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="24"/>
-      <c r="B16" s="24"/>
+      <c r="A16" s="22"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="5">
         <v>14</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
       <c r="G16" s="11" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="H16" s="9"/>
       <c r="I16" s="9"/>
@@ -4706,16 +4881,16 @@
       <c r="P16" s="2"/>
     </row>
     <row r="17" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="24"/>
-      <c r="B17" s="24"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="5">
         <v>15</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F17" s="7"/>
       <c r="G17" s="9"/>
@@ -4729,18 +4904,18 @@
       <c r="P17" s="2"/>
     </row>
     <row r="18" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="24"/>
-      <c r="B18" s="24"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="5">
         <v>16</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
       <c r="G18" s="11" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="H18" s="9"/>
       <c r="I18" s="9"/>
@@ -4752,18 +4927,18 @@
       <c r="P18" s="2"/>
     </row>
     <row r="19" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="24"/>
-      <c r="B19" s="24"/>
+      <c r="A19" s="22"/>
+      <c r="B19" s="22"/>
       <c r="C19" s="5">
         <v>17</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
       <c r="G19" s="11" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="H19" s="9"/>
       <c r="I19" s="9"/>
@@ -4775,19 +4950,19 @@
       <c r="P19" s="2"/>
     </row>
     <row r="20" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="24"/>
-      <c r="B20" s="25"/>
+      <c r="A20" s="22"/>
+      <c r="B20" s="23"/>
       <c r="C20" s="5">
         <v>18</v>
       </c>
-      <c r="D20" s="13" t="s">
-        <v>50</v>
+      <c r="D20" s="12" t="s">
+        <v>46</v>
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
       <c r="G20" s="9"/>
       <c r="H20" s="11" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="I20" s="9"/>
       <c r="J20" s="10"/>
@@ -4798,18 +4973,18 @@
       <c r="P20" s="2"/>
     </row>
     <row r="21" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="24"/>
+      <c r="A21" s="22"/>
       <c r="B21" s="26" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C21" s="5">
         <v>19</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="9"/>
@@ -4823,18 +4998,18 @@
       <c r="P21" s="2"/>
     </row>
     <row r="22" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="24"/>
-      <c r="B22" s="24"/>
+      <c r="A22" s="22"/>
+      <c r="B22" s="22"/>
       <c r="C22" s="5">
         <v>20</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
       <c r="G22" s="11" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>
@@ -4846,17 +5021,17 @@
       <c r="P22" s="2"/>
     </row>
     <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="25"/>
-      <c r="B23" s="25"/>
+      <c r="A23" s="23"/>
+      <c r="B23" s="23"/>
       <c r="C23" s="5">
         <v>21</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E23" s="7"/>
       <c r="F23" s="8" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G23" s="9"/>
       <c r="H23" s="9"/>
@@ -4869,21 +5044,21 @@
       <c r="P23" s="2"/>
     </row>
     <row r="24" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="37" t="s">
-        <v>55</v>
+      <c r="A24" s="31" t="s">
+        <v>51</v>
       </c>
       <c r="B24" s="26" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C24" s="5">
         <v>22</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E24" s="7"/>
       <c r="F24" s="8" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G24" s="9"/>
       <c r="H24" s="9"/>
@@ -4896,18 +5071,18 @@
       <c r="P24" s="2"/>
     </row>
     <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="24"/>
-      <c r="B25" s="24"/>
+      <c r="A25" s="22"/>
+      <c r="B25" s="22"/>
       <c r="C25" s="5">
         <v>23</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
       <c r="G25" s="11" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="H25" s="9"/>
       <c r="I25" s="9"/>
@@ -4919,18 +5094,18 @@
       <c r="P25" s="2"/>
     </row>
     <row r="26" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="24"/>
-      <c r="B26" s="24"/>
+      <c r="A26" s="22"/>
+      <c r="B26" s="22"/>
       <c r="C26" s="5">
         <v>24</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
       <c r="G26" s="11" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="H26" s="9"/>
       <c r="I26" s="9"/>
@@ -4942,18 +5117,18 @@
       <c r="P26" s="2"/>
     </row>
     <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="24"/>
-      <c r="B27" s="24"/>
+      <c r="A27" s="22"/>
+      <c r="B27" s="22"/>
       <c r="C27" s="5">
         <v>25</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
       <c r="G27" s="11" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="H27" s="9"/>
       <c r="I27" s="9"/>
@@ -4965,18 +5140,18 @@
       <c r="P27" s="2"/>
     </row>
     <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="25"/>
-      <c r="B28" s="25"/>
+      <c r="A28" s="23"/>
+      <c r="B28" s="23"/>
       <c r="C28" s="5">
         <v>26</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E28" s="7"/>
       <c r="F28" s="7"/>
       <c r="G28" s="11" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="H28" s="9"/>
       <c r="I28" s="9"/>
@@ -4988,21 +5163,21 @@
       <c r="P28" s="2"/>
     </row>
     <row r="29" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="23" t="s">
-        <v>64</v>
+      <c r="A29" s="21" t="s">
+        <v>60</v>
       </c>
       <c r="B29" s="26" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C29" s="5">
         <v>27</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E29" s="7"/>
       <c r="F29" s="8" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G29" s="9"/>
       <c r="H29" s="9"/>
@@ -5015,18 +5190,18 @@
       <c r="P29" s="2"/>
     </row>
     <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="24"/>
-      <c r="B30" s="24"/>
+      <c r="A30" s="22"/>
+      <c r="B30" s="22"/>
       <c r="C30" s="5">
         <v>28</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E30" s="7"/>
       <c r="F30" s="7"/>
       <c r="G30" s="11" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="H30" s="9"/>
       <c r="I30" s="9"/>
@@ -5038,18 +5213,18 @@
       <c r="P30" s="2"/>
     </row>
     <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="24"/>
-      <c r="B31" s="24"/>
+      <c r="A31" s="22"/>
+      <c r="B31" s="22"/>
       <c r="C31" s="5">
         <v>29</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
       <c r="G31" s="11" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="H31" s="9"/>
       <c r="I31" s="9"/>
@@ -5061,18 +5236,18 @@
       <c r="P31" s="2"/>
     </row>
     <row r="32" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="24"/>
-      <c r="B32" s="24"/>
+      <c r="A32" s="22"/>
+      <c r="B32" s="22"/>
       <c r="C32" s="5">
         <v>30</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E32" s="7"/>
       <c r="F32" s="7"/>
       <c r="G32" s="11" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="H32" s="9"/>
       <c r="I32" s="9"/>
@@ -5084,18 +5259,18 @@
       <c r="P32" s="2"/>
     </row>
     <row r="33" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="24"/>
-      <c r="B33" s="24"/>
+      <c r="A33" s="22"/>
+      <c r="B33" s="22"/>
       <c r="C33" s="5">
         <v>31</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
       <c r="G33" s="11" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="H33" s="9"/>
       <c r="I33" s="9"/>
@@ -5107,18 +5282,18 @@
       <c r="P33" s="2"/>
     </row>
     <row r="34" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="24"/>
-      <c r="B34" s="25"/>
+      <c r="A34" s="22"/>
+      <c r="B34" s="23"/>
       <c r="C34" s="5">
         <v>32</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E34" s="7"/>
       <c r="F34" s="7"/>
       <c r="G34" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="H34" s="9"/>
       <c r="I34" s="9"/>
@@ -5130,20 +5305,20 @@
       <c r="P34" s="2"/>
     </row>
     <row r="35" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="25"/>
-      <c r="B35" s="14" t="s">
-        <v>35</v>
+      <c r="A35" s="23"/>
+      <c r="B35" s="13" t="s">
+        <v>31</v>
       </c>
       <c r="C35" s="5">
         <v>33</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E35" s="7"/>
       <c r="F35" s="7"/>
       <c r="G35" s="11" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="H35" s="9"/>
       <c r="I35" s="9"/>
@@ -5155,21 +5330,21 @@
       <c r="P35" s="2"/>
     </row>
     <row r="36" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="36" t="s">
-        <v>76</v>
+      <c r="A36" s="30" t="s">
+        <v>72</v>
       </c>
       <c r="B36" s="26" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C36" s="5">
         <v>34</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E36" s="7"/>
       <c r="F36" s="8" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G36" s="9"/>
       <c r="H36" s="9"/>
@@ -5182,18 +5357,18 @@
       <c r="P36" s="2"/>
     </row>
     <row r="37" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="24"/>
-      <c r="B37" s="24"/>
+      <c r="A37" s="22"/>
+      <c r="B37" s="22"/>
       <c r="C37" s="5">
         <v>35</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E37" s="7"/>
       <c r="F37" s="7"/>
       <c r="G37" s="11" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="H37" s="9"/>
       <c r="I37" s="9"/>
@@ -5205,18 +5380,18 @@
       <c r="P37" s="2"/>
     </row>
     <row r="38" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="24"/>
-      <c r="B38" s="24"/>
+      <c r="A38" s="22"/>
+      <c r="B38" s="22"/>
       <c r="C38" s="5">
         <v>36</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E38" s="7"/>
       <c r="F38" s="7"/>
       <c r="G38" s="11" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H38" s="9"/>
       <c r="I38" s="9"/>
@@ -5228,18 +5403,18 @@
       <c r="P38" s="2"/>
     </row>
     <row r="39" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="24"/>
-      <c r="B39" s="24"/>
+      <c r="A39" s="22"/>
+      <c r="B39" s="22"/>
       <c r="C39" s="5">
         <v>37</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E39" s="7"/>
       <c r="F39" s="7"/>
       <c r="G39" s="11" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="H39" s="9"/>
       <c r="I39" s="9"/>
@@ -5251,18 +5426,18 @@
       <c r="P39" s="2"/>
     </row>
     <row r="40" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="24"/>
-      <c r="B40" s="25"/>
+      <c r="A40" s="22"/>
+      <c r="B40" s="23"/>
       <c r="C40" s="5">
         <v>38</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E40" s="7"/>
       <c r="F40" s="7"/>
       <c r="G40" s="11" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="H40" s="9"/>
       <c r="I40" s="9"/>
@@ -5274,20 +5449,20 @@
       <c r="P40" s="2"/>
     </row>
     <row r="41" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="25"/>
-      <c r="B41" s="14" t="s">
-        <v>35</v>
+      <c r="A41" s="23"/>
+      <c r="B41" s="13" t="s">
+        <v>31</v>
       </c>
       <c r="C41" s="5">
         <v>39</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
       <c r="G41" s="11" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="H41" s="9"/>
       <c r="I41" s="9"/>
@@ -5299,25 +5474,25 @@
       <c r="P41" s="2"/>
     </row>
     <row r="42" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="37" t="s">
-        <v>88</v>
-      </c>
-      <c r="B42" s="15" t="s">
-        <v>12</v>
+      <c r="A42" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="B42" s="14" t="s">
+        <v>9</v>
       </c>
       <c r="C42" s="5">
         <v>40</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="9"/>
       <c r="H42" s="9"/>
       <c r="I42" s="9"/>
-      <c r="J42" s="16" t="s">
-        <v>14</v>
+      <c r="J42" s="15" t="s">
+        <v>11</v>
       </c>
       <c r="L42" s="2"/>
       <c r="M42" s="2"/>
@@ -5326,22 +5501,22 @@
       <c r="P42" s="2"/>
     </row>
     <row r="43" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="24"/>
+      <c r="A43" s="22"/>
       <c r="B43" s="26" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C43" s="5">
         <v>41</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="9"/>
       <c r="H43" s="9"/>
-      <c r="I43" s="17" t="s">
-        <v>34</v>
+      <c r="I43" s="16" t="s">
+        <v>30</v>
       </c>
       <c r="J43" s="10"/>
       <c r="L43" s="2"/>
@@ -5351,16 +5526,16 @@
       <c r="P43" s="2"/>
     </row>
     <row r="44" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="24"/>
-      <c r="B44" s="24"/>
+      <c r="A44" s="22"/>
+      <c r="B44" s="22"/>
       <c r="C44" s="5">
         <v>42</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E44" s="8" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F44" s="7"/>
       <c r="G44" s="9"/>
@@ -5374,20 +5549,20 @@
       <c r="P44" s="2"/>
     </row>
     <row r="45" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="24"/>
-      <c r="B45" s="24"/>
+      <c r="A45" s="22"/>
+      <c r="B45" s="22"/>
       <c r="C45" s="5">
         <v>43</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E45" s="7"/>
       <c r="F45" s="7"/>
       <c r="G45" s="9"/>
       <c r="H45" s="9"/>
-      <c r="I45" s="17" t="s">
-        <v>34</v>
+      <c r="I45" s="16" t="s">
+        <v>30</v>
       </c>
       <c r="J45" s="10"/>
       <c r="L45" s="2"/>
@@ -5397,22 +5572,22 @@
       <c r="P45" s="2"/>
     </row>
     <row r="46" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="25"/>
-      <c r="B46" s="25"/>
-      <c r="C46" s="18">
+      <c r="A46" s="23"/>
+      <c r="B46" s="23"/>
+      <c r="C46" s="17">
         <v>44</v>
       </c>
-      <c r="D46" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="E46" s="19"/>
-      <c r="F46" s="19"/>
-      <c r="G46" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="H46" s="20"/>
-      <c r="I46" s="20"/>
-      <c r="J46" s="21"/>
+      <c r="D46" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="E46" s="18"/>
+      <c r="F46" s="18"/>
+      <c r="G46" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="H46" s="19"/>
+      <c r="I46" s="19"/>
+      <c r="J46" s="20"/>
       <c r="L46" s="2"/>
       <c r="M46" s="2"/>
       <c r="N46" s="2"/>
@@ -6375,13 +6550,6 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:A13"/>
-    <mergeCell ref="B3:B10"/>
-    <mergeCell ref="B11:B13"/>
     <mergeCell ref="A14:A23"/>
     <mergeCell ref="B21:B23"/>
     <mergeCell ref="A36:A41"/>
@@ -6393,6 +6561,13 @@
     <mergeCell ref="A29:A35"/>
     <mergeCell ref="B29:B34"/>
     <mergeCell ref="B36:B40"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:A13"/>
+    <mergeCell ref="B3:B10"/>
+    <mergeCell ref="B11:B13"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
Atualização e Cenário Ministrar Aulas 16, 17, 18, 19, 20, 21 e 22
</commit_message>
<xml_diff>
--- a/Artefatos/17. Análise dos Eventos para cada Cenário.xlsx
+++ b/Artefatos/17. Análise dos Eventos para cada Cenário.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amand\OneDrive\Área de Trabalho\GIT\OPE-Madara\Artefatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24EE6ECD-5FFD-43ED-89F4-50D0B616BD48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEA99480-E965-4199-9D43-D77DDDD53F8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20520" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="116">
   <si>
     <t>Externo</t>
   </si>
@@ -63,9 +63,6 @@
   </si>
   <si>
     <t>X</t>
-  </si>
-  <si>
-    <t>Secretaria solicita o extrato da conta</t>
   </si>
   <si>
     <t>X(1)</t>
@@ -380,9 +377,6 @@
     <t>Banco envia extrato de pagamento de boletos</t>
   </si>
   <si>
-    <t>Secretaria trata resposta da posição do aluno</t>
-  </si>
-  <si>
     <t>Ministrar Aulas</t>
   </si>
   <si>
@@ -395,50 +389,7 @@
     <t>Negociar</t>
   </si>
   <si>
-    <t>Secretaria trata inadimplência dos alunos</t>
-  </si>
-  <si>
-    <t>Transferência</t>
-  </si>
-  <si>
     <t>Aluno solicita transferência de curso</t>
-  </si>
-  <si>
-    <t>Trancamento</t>
-  </si>
-  <si>
-    <t>Aluno solicita o trancamento de matricula</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <r>
-      <t>Previsível</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>*</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Relativo</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>*</t>
-    </r>
   </si>
   <si>
     <r>
@@ -454,12 +405,65 @@
       <t>*</t>
     </r>
   </si>
+  <si>
+    <t>Aluno responde presença</t>
+  </si>
+  <si>
+    <t>Aluno retorna atividade</t>
+  </si>
+  <si>
+    <t>Professor registra ocorrência</t>
+  </si>
+  <si>
+    <t>X(10)</t>
+  </si>
+  <si>
+    <t>X(11)</t>
+  </si>
+  <si>
+    <t>Transfe-rência</t>
+  </si>
+  <si>
+    <t>Tranca-mento</t>
+  </si>
+  <si>
+    <t>Extempo-râneo</t>
+  </si>
+  <si>
+    <t>Aluno solicita o trancamento de matrícula</t>
+  </si>
+  <si>
+    <t>Secretária trata resposta do aluno</t>
+  </si>
+  <si>
+    <t>Secretária solicita o extrato da conta</t>
+  </si>
+  <si>
+    <t>Secretária trata resposta da posição do aluno</t>
+  </si>
+  <si>
+    <r>
+      <t>Relativo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <t>Previsível*</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -516,12 +520,6 @@
       <family val="1"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
       <b/>
       <sz val="12"/>
       <color theme="1"/>
@@ -535,8 +533,28 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10.5"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="16">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -581,19 +599,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFBFEBE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFBBE0E3"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -611,24 +617,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
+        <fgColor rgb="FFFEFEB4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -740,11 +752,293 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
@@ -804,96 +1098,163 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -901,6 +1262,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFEFEB4"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1112,187 +1478,188 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P962"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.875" customWidth="1"/>
     <col min="2" max="2" width="3.25" customWidth="1"/>
-    <col min="3" max="3" width="3" customWidth="1"/>
-    <col min="4" max="4" width="28.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3" style="46" customWidth="1"/>
+    <col min="4" max="4" width="36.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.25" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.875" customWidth="1"/>
-    <col min="8" max="8" width="8.5" customWidth="1"/>
-    <col min="9" max="9" width="7.625" customWidth="1"/>
-    <col min="10" max="10" width="13.5" customWidth="1"/>
+    <col min="7" max="7" width="9.125" customWidth="1"/>
+    <col min="8" max="8" width="8.25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.375" customWidth="1"/>
+    <col min="10" max="10" width="8.875" bestFit="1" customWidth="1"/>
     <col min="11" max="26" width="7.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="47" t="s">
-        <v>95</v>
-      </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="47"/>
-    </row>
-    <row r="2" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="32"/>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="51" t="s">
+    <row r="1" spans="1:16" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="51" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="53"/>
+    </row>
+    <row r="2" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="62" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="63"/>
+      <c r="C2" s="66" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="68" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="51"/>
-      <c r="G2" s="52" t="s">
+      <c r="F2" s="56"/>
+      <c r="G2" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="33"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="74"/>
+      <c r="K2" s="43"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
     </row>
-    <row r="3" spans="1:16" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="48" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="48"/>
-      <c r="C3" s="49" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="50" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="50" t="s">
-        <v>108</v>
-      </c>
-      <c r="F3" s="50" t="s">
+    <row r="3" spans="1:16" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="64"/>
+      <c r="B3" s="65"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="76" t="s">
+        <v>115</v>
+      </c>
+      <c r="F3" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="50" t="s">
+      <c r="G3" s="75" t="s">
+        <v>114</v>
+      </c>
+      <c r="H3" s="54" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="54" t="s">
+        <v>101</v>
+      </c>
+      <c r="J3" s="70" t="s">
         <v>109</v>
       </c>
-      <c r="H3" s="50" t="s">
-        <v>6</v>
-      </c>
-      <c r="I3" s="50" t="s">
-        <v>110</v>
-      </c>
-      <c r="J3" s="50" t="s">
-        <v>7</v>
-      </c>
       <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
+      <c r="M3" s="72"/>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
     </row>
     <row r="4" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="36">
+      <c r="C4" s="44">
         <v>1</v>
       </c>
-      <c r="D4" s="36" t="s">
+      <c r="D4" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37" t="s">
+      <c r="E4" s="57"/>
+      <c r="F4" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="39"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="36"/>
       <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
+      <c r="M4" s="72"/>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
     </row>
     <row r="5" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="34"/>
-      <c r="B5" s="35"/>
-      <c r="C5" s="36">
+      <c r="A5" s="35"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="44">
         <v>2</v>
       </c>
-      <c r="D5" s="36" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="38" t="s">
+      <c r="D5" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="E5" s="57"/>
+      <c r="F5" s="57"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="I5" s="38"/>
-      <c r="J5" s="39"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="36"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
-      <c r="N5" s="53"/>
+      <c r="N5" s="23"/>
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
     </row>
-    <row r="6" spans="1:16" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="34"/>
-      <c r="B6" s="35"/>
-      <c r="C6" s="36">
+    <row r="6" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="35"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="44">
         <v>3</v>
       </c>
-      <c r="D6" s="36" t="s">
-        <v>96</v>
-      </c>
-      <c r="E6" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="37"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="38"/>
-      <c r="J6" s="39"/>
+      <c r="D6" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="E6" s="58" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="57"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="36"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
     </row>
-    <row r="7" spans="1:16" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="34"/>
-      <c r="B7" s="41" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" s="36">
+    <row r="7" spans="1:16" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A7" s="35"/>
+      <c r="B7" s="50" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="44">
         <v>4</v>
       </c>
-      <c r="D7" s="36" t="s">
-        <v>97</v>
-      </c>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="42" t="s">
-        <v>107</v>
-      </c>
-      <c r="I7" s="38"/>
-      <c r="J7" s="39"/>
+      <c r="D7" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="E7" s="57"/>
+      <c r="F7" s="57"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="22"/>
+      <c r="J7" s="36"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
@@ -1300,131 +1667,218 @@
       <c r="P7" s="2"/>
     </row>
     <row r="8" spans="1:16" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="43" t="s">
+      <c r="A8" s="61" t="s">
+        <v>96</v>
+      </c>
+      <c r="B8" s="47" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="44">
+        <v>5</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="E8" s="58"/>
+      <c r="F8" s="58"/>
+      <c r="G8" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="36"/>
+    </row>
+    <row r="9" spans="1:16" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A9" s="61"/>
+      <c r="B9" s="47"/>
+      <c r="C9" s="44">
+        <v>6</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="E9" s="58" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="58"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="36"/>
+    </row>
+    <row r="10" spans="1:16" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A10" s="61"/>
+      <c r="B10" s="47"/>
+      <c r="C10" s="44">
+        <v>7</v>
+      </c>
+      <c r="D10" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="B8" s="35" t="s">
+      <c r="E10" s="57"/>
+      <c r="F10" s="58"/>
+      <c r="G10" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="36"/>
+    </row>
+    <row r="11" spans="1:16" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A11" s="61"/>
+      <c r="B11" s="47"/>
+      <c r="C11" s="44">
+        <v>8</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="E11" s="58" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="58"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="36"/>
+    </row>
+    <row r="12" spans="1:16" ht="20.25" x14ac:dyDescent="0.2">
+      <c r="A12" s="61"/>
+      <c r="B12" s="50" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="44">
         <v>9</v>
       </c>
-      <c r="C8" s="36">
-        <v>5</v>
-      </c>
-      <c r="D8" s="36" t="s">
+      <c r="D12" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="E12" s="57"/>
+      <c r="F12" s="58"/>
+      <c r="G12" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="36"/>
+    </row>
+    <row r="13" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="35" t="s">
         <v>99</v>
       </c>
-      <c r="E8" s="40" t="s">
+      <c r="B13" s="47" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="44">
+        <v>10</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="E13" s="58"/>
+      <c r="F13" s="58"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="37" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A14" s="35"/>
+      <c r="B14" s="47"/>
+      <c r="C14" s="44">
+        <v>11</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="E14" s="58" t="s">
+        <v>105</v>
+      </c>
+      <c r="F14" s="58"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="22"/>
+      <c r="J14" s="36"/>
+    </row>
+    <row r="15" spans="1:16" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="35"/>
+      <c r="B15" s="47"/>
+      <c r="C15" s="44">
+        <v>12</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="E15" s="58"/>
+      <c r="F15" s="58"/>
+      <c r="G15" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="H15" s="22"/>
+      <c r="I15" s="22"/>
+      <c r="J15" s="36"/>
+    </row>
+    <row r="16" spans="1:16" ht="45" x14ac:dyDescent="0.2">
+      <c r="A16" s="38" t="s">
+        <v>107</v>
+      </c>
+      <c r="B16" s="48" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="44">
         <v>13</v>
       </c>
-      <c r="F8" s="40"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="44"/>
-      <c r="I8" s="38"/>
-      <c r="J8" s="39"/>
-    </row>
-    <row r="9" spans="1:16" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="43"/>
-      <c r="B9" s="35"/>
-      <c r="C9" s="36">
-        <v>6</v>
-      </c>
-      <c r="D9" s="36" t="s">
+      <c r="D16" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="E9" s="37"/>
-      <c r="F9" s="40" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="38"/>
-      <c r="H9" s="44"/>
-      <c r="I9" s="38"/>
-      <c r="J9" s="39"/>
-    </row>
-    <row r="10" spans="1:16" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="45" t="s">
-        <v>101</v>
-      </c>
-      <c r="B10" s="41" t="s">
+      <c r="E16" s="58"/>
+      <c r="F16" s="58" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="36"/>
+    </row>
+    <row r="17" spans="1:10" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="B17" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="36">
-        <v>7</v>
-      </c>
-      <c r="D10" s="36" t="s">
-        <v>102</v>
-      </c>
-      <c r="E10" s="40"/>
-      <c r="F10" s="40"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="42" t="s">
-        <v>107</v>
-      </c>
-      <c r="I10" s="38"/>
-      <c r="J10" s="39"/>
-    </row>
-    <row r="11" spans="1:16" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="46" t="s">
-        <v>103</v>
-      </c>
-      <c r="B11" s="41" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="36">
-        <v>8</v>
-      </c>
-      <c r="D11" s="36" t="s">
-        <v>104</v>
-      </c>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40" t="s">
-        <v>13</v>
-      </c>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="38"/>
-      <c r="J11" s="39"/>
-    </row>
-    <row r="12" spans="1:16" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="45" t="s">
-        <v>105</v>
-      </c>
-      <c r="B12" s="41" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="36">
-        <v>9</v>
-      </c>
-      <c r="D12" s="36" t="s">
-        <v>106</v>
-      </c>
-      <c r="E12" s="37"/>
-      <c r="F12" s="40" t="s">
-        <v>13</v>
-      </c>
-      <c r="G12" s="38"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="38"/>
-      <c r="J12" s="39"/>
-    </row>
-    <row r="13" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="C17" s="45">
+        <v>14</v>
+      </c>
+      <c r="D17" s="40" t="s">
+        <v>110</v>
+      </c>
+      <c r="E17" s="59"/>
+      <c r="F17" s="60" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" s="41"/>
+      <c r="H17" s="41"/>
+      <c r="I17" s="41"/>
+      <c r="J17" s="42"/>
+    </row>
+    <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2356,16 +2810,19 @@
     <row r="961" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="962" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
+  <mergeCells count="12">
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="A2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
     <mergeCell ref="A4:A7"/>
     <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:D2"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="G2:I2"/>
-    <mergeCell ref="A3:B3"/>
     <mergeCell ref="B4:B6"/>
+    <mergeCell ref="A8:A12"/>
+    <mergeCell ref="B8:B11"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -2392,19 +2849,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="27"/>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="29" t="s">
+      <c r="A1" s="30"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="25"/>
-      <c r="G1" s="29" t="s">
+      <c r="F1" s="32"/>
+      <c r="G1" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
       <c r="J1" s="1"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
@@ -2413,10 +2870,10 @@
       <c r="P1" s="2"/>
     </row>
     <row r="2" spans="1:16" ht="33" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="25"/>
+      <c r="B2" s="32"/>
       <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
@@ -2424,19 +2881,19 @@
         <v>4</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>6</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>7</v>
@@ -2448,17 +2905,17 @@
       <c r="P2" s="2"/>
     </row>
     <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="27" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="5">
         <v>1</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="8" t="s">
@@ -2475,18 +2932,18 @@
       <c r="P3" s="2"/>
     </row>
     <row r="4" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="22"/>
-      <c r="B4" s="22"/>
+      <c r="A4" s="25"/>
+      <c r="B4" s="25"/>
       <c r="C4" s="5">
         <v>2</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
       <c r="G4" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
@@ -2498,18 +2955,18 @@
       <c r="P4" s="2"/>
     </row>
     <row r="5" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
-      <c r="B5" s="22"/>
+      <c r="A5" s="25"/>
+      <c r="B5" s="25"/>
       <c r="C5" s="5">
         <v>3</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
       <c r="G5" s="11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H5" s="9"/>
       <c r="I5" s="9"/>
@@ -2521,18 +2978,18 @@
       <c r="P5" s="2"/>
     </row>
     <row r="6" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="22"/>
-      <c r="B6" s="22"/>
+      <c r="A6" s="25"/>
+      <c r="B6" s="25"/>
       <c r="C6" s="5">
         <v>4</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
       <c r="G6" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
@@ -2544,16 +3001,16 @@
       <c r="P6" s="2"/>
     </row>
     <row r="7" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="22"/>
-      <c r="B7" s="22"/>
+      <c r="A7" s="25"/>
+      <c r="B7" s="25"/>
       <c r="C7" s="5">
         <v>5</v>
       </c>
       <c r="D7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>23</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>24</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="9"/>
@@ -2567,18 +3024,18 @@
       <c r="P7" s="2"/>
     </row>
     <row r="8" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="22"/>
-      <c r="B8" s="22"/>
+      <c r="A8" s="25"/>
+      <c r="B8" s="25"/>
       <c r="C8" s="5">
         <v>6</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="G8" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
@@ -2590,18 +3047,18 @@
       <c r="P8" s="2"/>
     </row>
     <row r="9" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="22"/>
-      <c r="B9" s="22"/>
+      <c r="A9" s="25"/>
+      <c r="B9" s="25"/>
       <c r="C9" s="5">
         <v>7</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
       <c r="G9" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
@@ -2613,18 +3070,18 @@
       <c r="P9" s="2"/>
     </row>
     <row r="10" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="22"/>
-      <c r="B10" s="23"/>
+      <c r="A10" s="25"/>
+      <c r="B10" s="26"/>
       <c r="C10" s="5">
         <v>8</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
       <c r="G10" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
@@ -2636,20 +3093,20 @@
       <c r="P10" s="2"/>
     </row>
     <row r="11" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
-      <c r="B11" s="26" t="s">
-        <v>31</v>
+      <c r="A11" s="25"/>
+      <c r="B11" s="27" t="s">
+        <v>30</v>
       </c>
       <c r="C11" s="5">
         <v>9</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
       <c r="G11" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
@@ -2661,16 +3118,16 @@
       <c r="P11" s="2"/>
     </row>
     <row r="12" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="22"/>
-      <c r="B12" s="22"/>
+      <c r="A12" s="25"/>
+      <c r="B12" s="25"/>
       <c r="C12" s="5">
         <v>10</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F12" s="7"/>
       <c r="G12" s="9"/>
@@ -2684,20 +3141,20 @@
       <c r="P12" s="2"/>
     </row>
     <row r="13" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="23"/>
-      <c r="B13" s="23"/>
+      <c r="A13" s="26"/>
+      <c r="B13" s="26"/>
       <c r="C13" s="5">
         <v>11</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
       <c r="I13" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J13" s="10"/>
       <c r="L13" s="2"/>
@@ -2707,17 +3164,17 @@
       <c r="P13" s="2"/>
     </row>
     <row r="14" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" s="26" t="s">
+      <c r="A14" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="27" t="s">
         <v>9</v>
       </c>
       <c r="C14" s="5">
         <v>12</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
@@ -2734,16 +3191,16 @@
       <c r="P14" s="2"/>
     </row>
     <row r="15" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="22"/>
-      <c r="B15" s="22"/>
+      <c r="A15" s="25"/>
+      <c r="B15" s="25"/>
       <c r="C15" s="5">
         <v>13</v>
       </c>
       <c r="D15" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" s="8" t="s">
         <v>37</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>38</v>
       </c>
       <c r="F15" s="7"/>
       <c r="G15" s="9"/>
@@ -2757,18 +3214,18 @@
       <c r="P15" s="2"/>
     </row>
     <row r="16" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="22"/>
-      <c r="B16" s="22"/>
+      <c r="A16" s="25"/>
+      <c r="B16" s="25"/>
       <c r="C16" s="5">
         <v>14</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
       <c r="G16" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H16" s="9"/>
       <c r="I16" s="9"/>
@@ -2780,16 +3237,16 @@
       <c r="P16" s="2"/>
     </row>
     <row r="17" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
+      <c r="A17" s="25"/>
+      <c r="B17" s="25"/>
       <c r="C17" s="5">
         <v>15</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F17" s="7"/>
       <c r="G17" s="9"/>
@@ -2803,18 +3260,18 @@
       <c r="P17" s="2"/>
     </row>
     <row r="18" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
+      <c r="A18" s="25"/>
+      <c r="B18" s="25"/>
       <c r="C18" s="5">
         <v>16</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
       <c r="G18" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H18" s="9"/>
       <c r="I18" s="9"/>
@@ -2826,18 +3283,18 @@
       <c r="P18" s="2"/>
     </row>
     <row r="19" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
+      <c r="A19" s="25"/>
+      <c r="B19" s="25"/>
       <c r="C19" s="5">
         <v>17</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
       <c r="G19" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H19" s="9"/>
       <c r="I19" s="9"/>
@@ -2849,13 +3306,13 @@
       <c r="P19" s="2"/>
     </row>
     <row r="20" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="22"/>
-      <c r="B20" s="23"/>
+      <c r="A20" s="25"/>
+      <c r="B20" s="26"/>
       <c r="C20" s="5">
         <v>18</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
@@ -2872,18 +3329,18 @@
       <c r="P20" s="2"/>
     </row>
     <row r="21" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="22"/>
-      <c r="B21" s="26" t="s">
-        <v>31</v>
+      <c r="A21" s="25"/>
+      <c r="B21" s="27" t="s">
+        <v>30</v>
       </c>
       <c r="C21" s="5">
         <v>19</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="9"/>
@@ -2897,18 +3354,18 @@
       <c r="P21" s="2"/>
     </row>
     <row r="22" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="22"/>
-      <c r="B22" s="22"/>
+      <c r="A22" s="25"/>
+      <c r="B22" s="25"/>
       <c r="C22" s="5">
         <v>20</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
       <c r="G22" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>
@@ -2920,13 +3377,13 @@
       <c r="P22" s="2"/>
     </row>
     <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="23"/>
-      <c r="B23" s="23"/>
+      <c r="A23" s="26"/>
+      <c r="B23" s="26"/>
       <c r="C23" s="5">
         <v>21</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E23" s="7"/>
       <c r="F23" s="8" t="s">
@@ -2943,17 +3400,17 @@
       <c r="P23" s="2"/>
     </row>
     <row r="24" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="B24" s="26" t="s">
+      <c r="A24" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" s="27" t="s">
         <v>9</v>
       </c>
       <c r="C24" s="5">
         <v>22</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E24" s="7"/>
       <c r="F24" s="8" t="s">
@@ -2970,18 +3427,18 @@
       <c r="P24" s="2"/>
     </row>
     <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="22"/>
-      <c r="B25" s="22"/>
+      <c r="A25" s="25"/>
+      <c r="B25" s="25"/>
       <c r="C25" s="5">
         <v>23</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
       <c r="G25" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H25" s="9"/>
       <c r="I25" s="9"/>
@@ -2993,18 +3450,18 @@
       <c r="P25" s="2"/>
     </row>
     <row r="26" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="22"/>
-      <c r="B26" s="22"/>
+      <c r="A26" s="25"/>
+      <c r="B26" s="25"/>
       <c r="C26" s="5">
         <v>24</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
       <c r="G26" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H26" s="9"/>
       <c r="I26" s="9"/>
@@ -3016,18 +3473,18 @@
       <c r="P26" s="2"/>
     </row>
     <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="22"/>
-      <c r="B27" s="22"/>
+      <c r="A27" s="25"/>
+      <c r="B27" s="25"/>
       <c r="C27" s="5">
         <v>25</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
       <c r="G27" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H27" s="9"/>
       <c r="I27" s="9"/>
@@ -3039,18 +3496,18 @@
       <c r="P27" s="2"/>
     </row>
     <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="23"/>
-      <c r="B28" s="23"/>
+      <c r="A28" s="26"/>
+      <c r="B28" s="26"/>
       <c r="C28" s="5">
         <v>26</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E28" s="7"/>
       <c r="F28" s="7"/>
       <c r="G28" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H28" s="9"/>
       <c r="I28" s="9"/>
@@ -3062,17 +3519,17 @@
       <c r="P28" s="2"/>
     </row>
     <row r="29" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="B29" s="26" t="s">
+      <c r="A29" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="B29" s="27" t="s">
         <v>9</v>
       </c>
       <c r="C29" s="5">
         <v>27</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E29" s="7"/>
       <c r="F29" s="8" t="s">
@@ -3089,18 +3546,18 @@
       <c r="P29" s="2"/>
     </row>
     <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="22"/>
-      <c r="B30" s="22"/>
+      <c r="A30" s="25"/>
+      <c r="B30" s="25"/>
       <c r="C30" s="5">
         <v>28</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E30" s="7"/>
       <c r="F30" s="7"/>
       <c r="G30" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H30" s="9"/>
       <c r="I30" s="9"/>
@@ -3112,18 +3569,18 @@
       <c r="P30" s="2"/>
     </row>
     <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="22"/>
-      <c r="B31" s="22"/>
+      <c r="A31" s="25"/>
+      <c r="B31" s="25"/>
       <c r="C31" s="5">
         <v>29</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
       <c r="G31" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H31" s="9"/>
       <c r="I31" s="9"/>
@@ -3135,18 +3592,18 @@
       <c r="P31" s="2"/>
     </row>
     <row r="32" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="22"/>
-      <c r="B32" s="22"/>
+      <c r="A32" s="25"/>
+      <c r="B32" s="25"/>
       <c r="C32" s="5">
         <v>30</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E32" s="7"/>
       <c r="F32" s="7"/>
       <c r="G32" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H32" s="9"/>
       <c r="I32" s="9"/>
@@ -3158,18 +3615,18 @@
       <c r="P32" s="2"/>
     </row>
     <row r="33" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="22"/>
-      <c r="B33" s="22"/>
+      <c r="A33" s="25"/>
+      <c r="B33" s="25"/>
       <c r="C33" s="5">
         <v>31</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
       <c r="G33" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H33" s="9"/>
       <c r="I33" s="9"/>
@@ -3181,18 +3638,18 @@
       <c r="P33" s="2"/>
     </row>
     <row r="34" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="22"/>
-      <c r="B34" s="23"/>
+      <c r="A34" s="25"/>
+      <c r="B34" s="26"/>
       <c r="C34" s="5">
         <v>32</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E34" s="7"/>
       <c r="F34" s="7"/>
       <c r="G34" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H34" s="9"/>
       <c r="I34" s="9"/>
@@ -3204,20 +3661,20 @@
       <c r="P34" s="2"/>
     </row>
     <row r="35" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="23"/>
+      <c r="A35" s="26"/>
       <c r="B35" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C35" s="5">
         <v>33</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E35" s="7"/>
       <c r="F35" s="7"/>
       <c r="G35" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H35" s="9"/>
       <c r="I35" s="9"/>
@@ -3229,17 +3686,17 @@
       <c r="P35" s="2"/>
     </row>
     <row r="36" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="B36" s="26" t="s">
+      <c r="A36" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="B36" s="27" t="s">
         <v>9</v>
       </c>
       <c r="C36" s="5">
         <v>34</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E36" s="7"/>
       <c r="F36" s="8" t="s">
@@ -3256,18 +3713,18 @@
       <c r="P36" s="2"/>
     </row>
     <row r="37" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="22"/>
-      <c r="B37" s="22"/>
+      <c r="A37" s="25"/>
+      <c r="B37" s="25"/>
       <c r="C37" s="5">
         <v>35</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E37" s="7"/>
       <c r="F37" s="7"/>
       <c r="G37" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H37" s="9"/>
       <c r="I37" s="9"/>
@@ -3279,18 +3736,18 @@
       <c r="P37" s="2"/>
     </row>
     <row r="38" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="22"/>
-      <c r="B38" s="22"/>
+      <c r="A38" s="25"/>
+      <c r="B38" s="25"/>
       <c r="C38" s="5">
         <v>36</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E38" s="7"/>
       <c r="F38" s="7"/>
       <c r="G38" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H38" s="9"/>
       <c r="I38" s="9"/>
@@ -3302,18 +3759,18 @@
       <c r="P38" s="2"/>
     </row>
     <row r="39" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="22"/>
-      <c r="B39" s="22"/>
+      <c r="A39" s="25"/>
+      <c r="B39" s="25"/>
       <c r="C39" s="5">
         <v>37</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E39" s="7"/>
       <c r="F39" s="7"/>
       <c r="G39" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H39" s="9"/>
       <c r="I39" s="9"/>
@@ -3325,18 +3782,18 @@
       <c r="P39" s="2"/>
     </row>
     <row r="40" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="22"/>
-      <c r="B40" s="23"/>
+      <c r="A40" s="25"/>
+      <c r="B40" s="26"/>
       <c r="C40" s="5">
         <v>38</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E40" s="7"/>
       <c r="F40" s="7"/>
       <c r="G40" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H40" s="9"/>
       <c r="I40" s="9"/>
@@ -3348,20 +3805,20 @@
       <c r="P40" s="2"/>
     </row>
     <row r="41" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="23"/>
+      <c r="A41" s="26"/>
       <c r="B41" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C41" s="5">
         <v>39</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
       <c r="G41" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H41" s="9"/>
       <c r="I41" s="9"/>
@@ -3373,8 +3830,8 @@
       <c r="P41" s="2"/>
     </row>
     <row r="42" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="31" t="s">
-        <v>84</v>
+      <c r="A42" s="28" t="s">
+        <v>83</v>
       </c>
       <c r="B42" s="14" t="s">
         <v>9</v>
@@ -3383,7 +3840,7 @@
         <v>40</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
@@ -3400,22 +3857,22 @@
       <c r="P42" s="2"/>
     </row>
     <row r="43" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="22"/>
-      <c r="B43" s="26" t="s">
-        <v>86</v>
+      <c r="A43" s="25"/>
+      <c r="B43" s="27" t="s">
+        <v>85</v>
       </c>
       <c r="C43" s="5">
         <v>41</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="9"/>
       <c r="H43" s="9"/>
       <c r="I43" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J43" s="10"/>
       <c r="L43" s="2"/>
@@ -3425,16 +3882,16 @@
       <c r="P43" s="2"/>
     </row>
     <row r="44" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="22"/>
-      <c r="B44" s="22"/>
+      <c r="A44" s="25"/>
+      <c r="B44" s="25"/>
       <c r="C44" s="5">
         <v>42</v>
       </c>
       <c r="D44" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="E44" s="8" t="s">
         <v>88</v>
-      </c>
-      <c r="E44" s="8" t="s">
-        <v>89</v>
       </c>
       <c r="F44" s="7"/>
       <c r="G44" s="9"/>
@@ -3448,20 +3905,20 @@
       <c r="P44" s="2"/>
     </row>
     <row r="45" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="22"/>
-      <c r="B45" s="22"/>
+      <c r="A45" s="25"/>
+      <c r="B45" s="25"/>
       <c r="C45" s="5">
         <v>43</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E45" s="7"/>
       <c r="F45" s="7"/>
       <c r="G45" s="9"/>
       <c r="H45" s="9"/>
       <c r="I45" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J45" s="10"/>
       <c r="L45" s="2"/>
@@ -3471,18 +3928,18 @@
       <c r="P45" s="2"/>
     </row>
     <row r="46" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="23"/>
-      <c r="B46" s="23"/>
+      <c r="A46" s="26"/>
+      <c r="B46" s="26"/>
       <c r="C46" s="17">
         <v>44</v>
       </c>
       <c r="D46" s="17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E46" s="18"/>
       <c r="F46" s="18"/>
       <c r="G46" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H46" s="19"/>
       <c r="I46" s="19"/>
@@ -4449,6 +4906,13 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:A13"/>
+    <mergeCell ref="B3:B10"/>
+    <mergeCell ref="B11:B13"/>
     <mergeCell ref="A14:A23"/>
     <mergeCell ref="B21:B23"/>
     <mergeCell ref="A36:A41"/>
@@ -4460,13 +4924,6 @@
     <mergeCell ref="A29:A35"/>
     <mergeCell ref="B29:B34"/>
     <mergeCell ref="B36:B40"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:A13"/>
-    <mergeCell ref="B3:B10"/>
-    <mergeCell ref="B11:B13"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -4493,19 +4950,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="27"/>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="29" t="s">
+      <c r="A1" s="30"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="25"/>
-      <c r="G1" s="29" t="s">
+      <c r="F1" s="32"/>
+      <c r="G1" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
       <c r="J1" s="1"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
@@ -4514,10 +4971,10 @@
       <c r="P1" s="2"/>
     </row>
     <row r="2" spans="1:16" ht="33" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="25"/>
+      <c r="B2" s="32"/>
       <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
@@ -4525,19 +4982,19 @@
         <v>4</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>6</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>7</v>
@@ -4549,17 +5006,17 @@
       <c r="P2" s="2"/>
     </row>
     <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="27" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="5">
         <v>1</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="8" t="s">
@@ -4576,18 +5033,18 @@
       <c r="P3" s="2"/>
     </row>
     <row r="4" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="22"/>
-      <c r="B4" s="22"/>
+      <c r="A4" s="25"/>
+      <c r="B4" s="25"/>
       <c r="C4" s="5">
         <v>2</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
       <c r="G4" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
@@ -4599,18 +5056,18 @@
       <c r="P4" s="2"/>
     </row>
     <row r="5" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
-      <c r="B5" s="22"/>
+      <c r="A5" s="25"/>
+      <c r="B5" s="25"/>
       <c r="C5" s="5">
         <v>3</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
       <c r="G5" s="11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H5" s="9"/>
       <c r="I5" s="9"/>
@@ -4622,18 +5079,18 @@
       <c r="P5" s="2"/>
     </row>
     <row r="6" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="22"/>
-      <c r="B6" s="22"/>
+      <c r="A6" s="25"/>
+      <c r="B6" s="25"/>
       <c r="C6" s="5">
         <v>4</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
       <c r="G6" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
@@ -4645,16 +5102,16 @@
       <c r="P6" s="2"/>
     </row>
     <row r="7" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="22"/>
-      <c r="B7" s="22"/>
+      <c r="A7" s="25"/>
+      <c r="B7" s="25"/>
       <c r="C7" s="5">
         <v>5</v>
       </c>
       <c r="D7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>23</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>24</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="9"/>
@@ -4668,18 +5125,18 @@
       <c r="P7" s="2"/>
     </row>
     <row r="8" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="22"/>
-      <c r="B8" s="22"/>
+      <c r="A8" s="25"/>
+      <c r="B8" s="25"/>
       <c r="C8" s="5">
         <v>6</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="G8" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
@@ -4691,18 +5148,18 @@
       <c r="P8" s="2"/>
     </row>
     <row r="9" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="22"/>
-      <c r="B9" s="22"/>
+      <c r="A9" s="25"/>
+      <c r="B9" s="25"/>
       <c r="C9" s="5">
         <v>7</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
       <c r="G9" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
@@ -4714,18 +5171,18 @@
       <c r="P9" s="2"/>
     </row>
     <row r="10" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="22"/>
-      <c r="B10" s="23"/>
+      <c r="A10" s="25"/>
+      <c r="B10" s="26"/>
       <c r="C10" s="5">
         <v>8</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
       <c r="G10" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
@@ -4737,20 +5194,20 @@
       <c r="P10" s="2"/>
     </row>
     <row r="11" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
-      <c r="B11" s="26" t="s">
-        <v>31</v>
+      <c r="A11" s="25"/>
+      <c r="B11" s="27" t="s">
+        <v>30</v>
       </c>
       <c r="C11" s="5">
         <v>9</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
       <c r="G11" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
@@ -4762,16 +5219,16 @@
       <c r="P11" s="2"/>
     </row>
     <row r="12" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="22"/>
-      <c r="B12" s="22"/>
+      <c r="A12" s="25"/>
+      <c r="B12" s="25"/>
       <c r="C12" s="5">
         <v>10</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F12" s="7"/>
       <c r="G12" s="9"/>
@@ -4785,20 +5242,20 @@
       <c r="P12" s="2"/>
     </row>
     <row r="13" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="23"/>
-      <c r="B13" s="23"/>
+      <c r="A13" s="26"/>
+      <c r="B13" s="26"/>
       <c r="C13" s="5">
         <v>11</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
       <c r="I13" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J13" s="10"/>
       <c r="L13" s="2"/>
@@ -4808,17 +5265,17 @@
       <c r="P13" s="2"/>
     </row>
     <row r="14" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" s="26" t="s">
+      <c r="A14" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="27" t="s">
         <v>9</v>
       </c>
       <c r="C14" s="5">
         <v>12</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
@@ -4835,16 +5292,16 @@
       <c r="P14" s="2"/>
     </row>
     <row r="15" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="22"/>
-      <c r="B15" s="22"/>
+      <c r="A15" s="25"/>
+      <c r="B15" s="25"/>
       <c r="C15" s="5">
         <v>13</v>
       </c>
       <c r="D15" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" s="8" t="s">
         <v>37</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>38</v>
       </c>
       <c r="F15" s="7"/>
       <c r="G15" s="9"/>
@@ -4858,18 +5315,18 @@
       <c r="P15" s="2"/>
     </row>
     <row r="16" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="22"/>
-      <c r="B16" s="22"/>
+      <c r="A16" s="25"/>
+      <c r="B16" s="25"/>
       <c r="C16" s="5">
         <v>14</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
       <c r="G16" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H16" s="9"/>
       <c r="I16" s="9"/>
@@ -4881,16 +5338,16 @@
       <c r="P16" s="2"/>
     </row>
     <row r="17" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
+      <c r="A17" s="25"/>
+      <c r="B17" s="25"/>
       <c r="C17" s="5">
         <v>15</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F17" s="7"/>
       <c r="G17" s="9"/>
@@ -4904,18 +5361,18 @@
       <c r="P17" s="2"/>
     </row>
     <row r="18" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
+      <c r="A18" s="25"/>
+      <c r="B18" s="25"/>
       <c r="C18" s="5">
         <v>16</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
       <c r="G18" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H18" s="9"/>
       <c r="I18" s="9"/>
@@ -4927,18 +5384,18 @@
       <c r="P18" s="2"/>
     </row>
     <row r="19" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
+      <c r="A19" s="25"/>
+      <c r="B19" s="25"/>
       <c r="C19" s="5">
         <v>17</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
       <c r="G19" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H19" s="9"/>
       <c r="I19" s="9"/>
@@ -4950,13 +5407,13 @@
       <c r="P19" s="2"/>
     </row>
     <row r="20" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="22"/>
-      <c r="B20" s="23"/>
+      <c r="A20" s="25"/>
+      <c r="B20" s="26"/>
       <c r="C20" s="5">
         <v>18</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
@@ -4973,18 +5430,18 @@
       <c r="P20" s="2"/>
     </row>
     <row r="21" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="22"/>
-      <c r="B21" s="26" t="s">
-        <v>31</v>
+      <c r="A21" s="25"/>
+      <c r="B21" s="27" t="s">
+        <v>30</v>
       </c>
       <c r="C21" s="5">
         <v>19</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="9"/>
@@ -4998,18 +5455,18 @@
       <c r="P21" s="2"/>
     </row>
     <row r="22" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="22"/>
-      <c r="B22" s="22"/>
+      <c r="A22" s="25"/>
+      <c r="B22" s="25"/>
       <c r="C22" s="5">
         <v>20</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
       <c r="G22" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>
@@ -5021,13 +5478,13 @@
       <c r="P22" s="2"/>
     </row>
     <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="23"/>
-      <c r="B23" s="23"/>
+      <c r="A23" s="26"/>
+      <c r="B23" s="26"/>
       <c r="C23" s="5">
         <v>21</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E23" s="7"/>
       <c r="F23" s="8" t="s">
@@ -5044,17 +5501,17 @@
       <c r="P23" s="2"/>
     </row>
     <row r="24" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="B24" s="26" t="s">
+      <c r="A24" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" s="27" t="s">
         <v>9</v>
       </c>
       <c r="C24" s="5">
         <v>22</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E24" s="7"/>
       <c r="F24" s="8" t="s">
@@ -5071,18 +5528,18 @@
       <c r="P24" s="2"/>
     </row>
     <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="22"/>
-      <c r="B25" s="22"/>
+      <c r="A25" s="25"/>
+      <c r="B25" s="25"/>
       <c r="C25" s="5">
         <v>23</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
       <c r="G25" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H25" s="9"/>
       <c r="I25" s="9"/>
@@ -5094,18 +5551,18 @@
       <c r="P25" s="2"/>
     </row>
     <row r="26" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="22"/>
-      <c r="B26" s="22"/>
+      <c r="A26" s="25"/>
+      <c r="B26" s="25"/>
       <c r="C26" s="5">
         <v>24</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
       <c r="G26" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H26" s="9"/>
       <c r="I26" s="9"/>
@@ -5117,18 +5574,18 @@
       <c r="P26" s="2"/>
     </row>
     <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="22"/>
-      <c r="B27" s="22"/>
+      <c r="A27" s="25"/>
+      <c r="B27" s="25"/>
       <c r="C27" s="5">
         <v>25</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
       <c r="G27" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H27" s="9"/>
       <c r="I27" s="9"/>
@@ -5140,18 +5597,18 @@
       <c r="P27" s="2"/>
     </row>
     <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="23"/>
-      <c r="B28" s="23"/>
+      <c r="A28" s="26"/>
+      <c r="B28" s="26"/>
       <c r="C28" s="5">
         <v>26</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E28" s="7"/>
       <c r="F28" s="7"/>
       <c r="G28" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H28" s="9"/>
       <c r="I28" s="9"/>
@@ -5163,17 +5620,17 @@
       <c r="P28" s="2"/>
     </row>
     <row r="29" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="B29" s="26" t="s">
+      <c r="A29" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="B29" s="27" t="s">
         <v>9</v>
       </c>
       <c r="C29" s="5">
         <v>27</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E29" s="7"/>
       <c r="F29" s="8" t="s">
@@ -5190,18 +5647,18 @@
       <c r="P29" s="2"/>
     </row>
     <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="22"/>
-      <c r="B30" s="22"/>
+      <c r="A30" s="25"/>
+      <c r="B30" s="25"/>
       <c r="C30" s="5">
         <v>28</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E30" s="7"/>
       <c r="F30" s="7"/>
       <c r="G30" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H30" s="9"/>
       <c r="I30" s="9"/>
@@ -5213,18 +5670,18 @@
       <c r="P30" s="2"/>
     </row>
     <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="22"/>
-      <c r="B31" s="22"/>
+      <c r="A31" s="25"/>
+      <c r="B31" s="25"/>
       <c r="C31" s="5">
         <v>29</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
       <c r="G31" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H31" s="9"/>
       <c r="I31" s="9"/>
@@ -5236,18 +5693,18 @@
       <c r="P31" s="2"/>
     </row>
     <row r="32" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="22"/>
-      <c r="B32" s="22"/>
+      <c r="A32" s="25"/>
+      <c r="B32" s="25"/>
       <c r="C32" s="5">
         <v>30</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E32" s="7"/>
       <c r="F32" s="7"/>
       <c r="G32" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H32" s="9"/>
       <c r="I32" s="9"/>
@@ -5259,18 +5716,18 @@
       <c r="P32" s="2"/>
     </row>
     <row r="33" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="22"/>
-      <c r="B33" s="22"/>
+      <c r="A33" s="25"/>
+      <c r="B33" s="25"/>
       <c r="C33" s="5">
         <v>31</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
       <c r="G33" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H33" s="9"/>
       <c r="I33" s="9"/>
@@ -5282,18 +5739,18 @@
       <c r="P33" s="2"/>
     </row>
     <row r="34" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="22"/>
-      <c r="B34" s="23"/>
+      <c r="A34" s="25"/>
+      <c r="B34" s="26"/>
       <c r="C34" s="5">
         <v>32</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E34" s="7"/>
       <c r="F34" s="7"/>
       <c r="G34" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H34" s="9"/>
       <c r="I34" s="9"/>
@@ -5305,20 +5762,20 @@
       <c r="P34" s="2"/>
     </row>
     <row r="35" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="23"/>
+      <c r="A35" s="26"/>
       <c r="B35" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C35" s="5">
         <v>33</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E35" s="7"/>
       <c r="F35" s="7"/>
       <c r="G35" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H35" s="9"/>
       <c r="I35" s="9"/>
@@ -5330,17 +5787,17 @@
       <c r="P35" s="2"/>
     </row>
     <row r="36" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="B36" s="26" t="s">
+      <c r="A36" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="B36" s="27" t="s">
         <v>9</v>
       </c>
       <c r="C36" s="5">
         <v>34</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E36" s="7"/>
       <c r="F36" s="8" t="s">
@@ -5357,18 +5814,18 @@
       <c r="P36" s="2"/>
     </row>
     <row r="37" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="22"/>
-      <c r="B37" s="22"/>
+      <c r="A37" s="25"/>
+      <c r="B37" s="25"/>
       <c r="C37" s="5">
         <v>35</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E37" s="7"/>
       <c r="F37" s="7"/>
       <c r="G37" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H37" s="9"/>
       <c r="I37" s="9"/>
@@ -5380,18 +5837,18 @@
       <c r="P37" s="2"/>
     </row>
     <row r="38" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="22"/>
-      <c r="B38" s="22"/>
+      <c r="A38" s="25"/>
+      <c r="B38" s="25"/>
       <c r="C38" s="5">
         <v>36</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E38" s="7"/>
       <c r="F38" s="7"/>
       <c r="G38" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H38" s="9"/>
       <c r="I38" s="9"/>
@@ -5403,18 +5860,18 @@
       <c r="P38" s="2"/>
     </row>
     <row r="39" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="22"/>
-      <c r="B39" s="22"/>
+      <c r="A39" s="25"/>
+      <c r="B39" s="25"/>
       <c r="C39" s="5">
         <v>37</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E39" s="7"/>
       <c r="F39" s="7"/>
       <c r="G39" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H39" s="9"/>
       <c r="I39" s="9"/>
@@ -5426,18 +5883,18 @@
       <c r="P39" s="2"/>
     </row>
     <row r="40" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="22"/>
-      <c r="B40" s="23"/>
+      <c r="A40" s="25"/>
+      <c r="B40" s="26"/>
       <c r="C40" s="5">
         <v>38</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E40" s="7"/>
       <c r="F40" s="7"/>
       <c r="G40" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H40" s="9"/>
       <c r="I40" s="9"/>
@@ -5449,20 +5906,20 @@
       <c r="P40" s="2"/>
     </row>
     <row r="41" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="23"/>
+      <c r="A41" s="26"/>
       <c r="B41" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C41" s="5">
         <v>39</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
       <c r="G41" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H41" s="9"/>
       <c r="I41" s="9"/>
@@ -5474,8 +5931,8 @@
       <c r="P41" s="2"/>
     </row>
     <row r="42" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="31" t="s">
-        <v>84</v>
+      <c r="A42" s="28" t="s">
+        <v>83</v>
       </c>
       <c r="B42" s="14" t="s">
         <v>9</v>
@@ -5484,7 +5941,7 @@
         <v>40</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
@@ -5501,22 +5958,22 @@
       <c r="P42" s="2"/>
     </row>
     <row r="43" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="22"/>
-      <c r="B43" s="26" t="s">
-        <v>86</v>
+      <c r="A43" s="25"/>
+      <c r="B43" s="27" t="s">
+        <v>85</v>
       </c>
       <c r="C43" s="5">
         <v>41</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="9"/>
       <c r="H43" s="9"/>
       <c r="I43" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J43" s="10"/>
       <c r="L43" s="2"/>
@@ -5526,16 +5983,16 @@
       <c r="P43" s="2"/>
     </row>
     <row r="44" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="22"/>
-      <c r="B44" s="22"/>
+      <c r="A44" s="25"/>
+      <c r="B44" s="25"/>
       <c r="C44" s="5">
         <v>42</v>
       </c>
       <c r="D44" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="E44" s="8" t="s">
         <v>88</v>
-      </c>
-      <c r="E44" s="8" t="s">
-        <v>89</v>
       </c>
       <c r="F44" s="7"/>
       <c r="G44" s="9"/>
@@ -5549,20 +6006,20 @@
       <c r="P44" s="2"/>
     </row>
     <row r="45" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="22"/>
-      <c r="B45" s="22"/>
+      <c r="A45" s="25"/>
+      <c r="B45" s="25"/>
       <c r="C45" s="5">
         <v>43</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E45" s="7"/>
       <c r="F45" s="7"/>
       <c r="G45" s="9"/>
       <c r="H45" s="9"/>
       <c r="I45" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J45" s="10"/>
       <c r="L45" s="2"/>
@@ -5572,18 +6029,18 @@
       <c r="P45" s="2"/>
     </row>
     <row r="46" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="23"/>
-      <c r="B46" s="23"/>
+      <c r="A46" s="26"/>
+      <c r="B46" s="26"/>
       <c r="C46" s="17">
         <v>44</v>
       </c>
       <c r="D46" s="17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E46" s="18"/>
       <c r="F46" s="18"/>
       <c r="G46" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H46" s="19"/>
       <c r="I46" s="19"/>
@@ -6550,6 +7007,13 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:A13"/>
+    <mergeCell ref="B3:B10"/>
+    <mergeCell ref="B11:B13"/>
     <mergeCell ref="A14:A23"/>
     <mergeCell ref="B21:B23"/>
     <mergeCell ref="A36:A41"/>
@@ -6561,13 +7025,6 @@
     <mergeCell ref="A29:A35"/>
     <mergeCell ref="B29:B34"/>
     <mergeCell ref="B36:B40"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:A13"/>
-    <mergeCell ref="B3:B10"/>
-    <mergeCell ref="B11:B13"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
Inclusão  Capacidade 2_Ministrar Aulas e Artefato 23_ Matrizes
</commit_message>
<xml_diff>
--- a/Artefatos/17. Análise dos Eventos para cada Cenário.xlsx
+++ b/Artefatos/17. Análise dos Eventos para cada Cenário.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amand\OneDrive\Área de Trabalho\GIT\OPE-Madara\Artefatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEA99480-E965-4199-9D43-D77DDDD53F8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E11810C-6808-4F6A-8CAC-667CC8ECF1A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20520" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -640,7 +640,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -752,293 +752,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
@@ -1107,19 +825,38 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1132,129 +869,57 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1478,15 +1143,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P962"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:XFD16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.875" customWidth="1"/>
     <col min="2" max="2" width="3.25" customWidth="1"/>
-    <col min="3" max="3" width="3" style="46" customWidth="1"/>
+    <col min="3" max="3" width="3" style="25" customWidth="1"/>
     <col min="4" max="4" width="36.125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.25" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.125" bestFit="1" customWidth="1"/>
@@ -1497,42 +1162,42 @@
     <col min="11" max="26" width="7.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="51" t="s">
+    <row r="1" spans="1:16" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A1" s="47" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="53"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
     </row>
     <row r="2" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="62" t="s">
+      <c r="A2" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="66" t="s">
+      <c r="B2" s="48"/>
+      <c r="C2" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="68" t="s">
+      <c r="D2" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="71" t="s">
+      <c r="E2" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="56"/>
-      <c r="G2" s="55" t="s">
+      <c r="F2" s="49"/>
+      <c r="G2" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="73"/>
-      <c r="I2" s="73"/>
-      <c r="J2" s="74"/>
-      <c r="K2" s="43"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="46"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
@@ -1540,78 +1205,78 @@
       <c r="P2" s="2"/>
     </row>
     <row r="3" spans="1:16" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="64"/>
-      <c r="B3" s="65"/>
-      <c r="C3" s="67"/>
-      <c r="D3" s="69"/>
-      <c r="E3" s="76" t="s">
+      <c r="A3" s="48"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="33" t="s">
         <v>115</v>
       </c>
-      <c r="F3" s="54" t="s">
+      <c r="F3" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="75" t="s">
+      <c r="G3" s="32" t="s">
         <v>114</v>
       </c>
-      <c r="H3" s="54" t="s">
+      <c r="H3" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="54" t="s">
+      <c r="I3" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="J3" s="70" t="s">
+      <c r="J3" s="28" t="s">
         <v>109</v>
       </c>
       <c r="L3" s="2"/>
-      <c r="M3" s="72"/>
+      <c r="M3" s="31"/>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
     </row>
     <row r="4" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="47" t="s">
+      <c r="B4" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="44">
+      <c r="C4" s="24">
         <v>1</v>
       </c>
       <c r="D4" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="57"/>
-      <c r="F4" s="57" t="s">
+      <c r="E4" s="29"/>
+      <c r="F4" s="29" t="s">
         <v>11</v>
       </c>
       <c r="G4" s="22"/>
       <c r="H4" s="22"/>
       <c r="I4" s="22"/>
-      <c r="J4" s="36"/>
+      <c r="J4" s="53"/>
       <c r="L4" s="2"/>
-      <c r="M4" s="72"/>
+      <c r="M4" s="31"/>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
     </row>
     <row r="5" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="35"/>
-      <c r="B5" s="47"/>
-      <c r="C5" s="44">
+      <c r="A5" s="52"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="24">
         <v>2</v>
       </c>
       <c r="D5" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="E5" s="57"/>
-      <c r="F5" s="57"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
       <c r="G5" s="22"/>
       <c r="H5" s="22" t="s">
         <v>11</v>
       </c>
       <c r="I5" s="22"/>
-      <c r="J5" s="36"/>
+      <c r="J5" s="53"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="N5" s="23"/>
@@ -1619,22 +1284,22 @@
       <c r="P5" s="2"/>
     </row>
     <row r="6" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="35"/>
-      <c r="B6" s="47"/>
-      <c r="C6" s="44">
+      <c r="A6" s="52"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="24">
         <v>3</v>
       </c>
       <c r="D6" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="E6" s="58" t="s">
+      <c r="E6" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="57"/>
+      <c r="F6" s="29"/>
       <c r="G6" s="22"/>
       <c r="H6" s="22"/>
       <c r="I6" s="22"/>
-      <c r="J6" s="36"/>
+      <c r="J6" s="53"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
@@ -1642,24 +1307,24 @@
       <c r="P6" s="2"/>
     </row>
     <row r="7" spans="1:16" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="35"/>
-      <c r="B7" s="50" t="s">
+      <c r="A7" s="52"/>
+      <c r="B7" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="44">
+      <c r="C7" s="24">
         <v>4</v>
       </c>
       <c r="D7" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="E7" s="57"/>
-      <c r="F7" s="57"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
       <c r="G7" s="22"/>
       <c r="H7" s="22" t="s">
         <v>11</v>
       </c>
       <c r="I7" s="22"/>
-      <c r="J7" s="36"/>
+      <c r="J7" s="53"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
@@ -1667,204 +1332,215 @@
       <c r="P7" s="2"/>
     </row>
     <row r="8" spans="1:16" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="61" t="s">
+      <c r="A8" s="54" t="s">
         <v>96</v>
       </c>
-      <c r="B8" s="47" t="s">
+      <c r="B8" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="44">
+      <c r="C8" s="24">
         <v>5</v>
       </c>
       <c r="D8" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="E8" s="58"/>
-      <c r="F8" s="58"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
       <c r="G8" s="22" t="s">
         <v>12</v>
       </c>
       <c r="H8" s="22"/>
       <c r="I8" s="22"/>
-      <c r="J8" s="36"/>
+      <c r="J8" s="53"/>
     </row>
     <row r="9" spans="1:16" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="61"/>
-      <c r="B9" s="47"/>
-      <c r="C9" s="44">
+      <c r="A9" s="54"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="24">
         <v>6</v>
       </c>
       <c r="D9" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="E9" s="58" t="s">
+      <c r="E9" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="58"/>
+      <c r="F9" s="30"/>
       <c r="G9" s="22"/>
       <c r="H9" s="22"/>
       <c r="I9" s="22"/>
-      <c r="J9" s="36"/>
+      <c r="J9" s="53"/>
     </row>
     <row r="10" spans="1:16" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="61"/>
-      <c r="B10" s="47"/>
-      <c r="C10" s="44">
+      <c r="A10" s="54"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="24">
         <v>7</v>
       </c>
       <c r="D10" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="E10" s="57"/>
-      <c r="F10" s="58"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="30"/>
       <c r="G10" s="22" t="s">
         <v>25</v>
       </c>
       <c r="H10" s="22"/>
       <c r="I10" s="22"/>
-      <c r="J10" s="36"/>
+      <c r="J10" s="53"/>
     </row>
     <row r="11" spans="1:16" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="61"/>
-      <c r="B11" s="47"/>
-      <c r="C11" s="44">
+      <c r="A11" s="54"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="24">
         <v>8</v>
       </c>
       <c r="D11" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="E11" s="58" t="s">
+      <c r="E11" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="58"/>
+      <c r="F11" s="30"/>
       <c r="G11" s="22"/>
       <c r="H11" s="22"/>
       <c r="I11" s="22"/>
-      <c r="J11" s="36"/>
+      <c r="J11" s="53"/>
     </row>
     <row r="12" spans="1:16" ht="20.25" x14ac:dyDescent="0.2">
-      <c r="A12" s="61"/>
-      <c r="B12" s="50" t="s">
+      <c r="A12" s="54"/>
+      <c r="B12" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="44">
+      <c r="C12" s="24">
         <v>9</v>
       </c>
       <c r="D12" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="E12" s="57"/>
-      <c r="F12" s="58"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="30"/>
       <c r="G12" s="22" t="s">
         <v>25</v>
       </c>
       <c r="H12" s="22"/>
       <c r="I12" s="22"/>
-      <c r="J12" s="36"/>
+      <c r="J12" s="53"/>
     </row>
     <row r="13" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="35" t="s">
+      <c r="A13" s="52" t="s">
         <v>99</v>
       </c>
-      <c r="B13" s="47" t="s">
+      <c r="B13" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="44">
+      <c r="C13" s="24">
         <v>10</v>
       </c>
       <c r="D13" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="E13" s="58"/>
-      <c r="F13" s="58"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
       <c r="G13" s="22"/>
       <c r="H13" s="22"/>
       <c r="I13" s="22"/>
-      <c r="J13" s="37" t="s">
+      <c r="J13" s="55" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="35"/>
-      <c r="B14" s="47"/>
-      <c r="C14" s="44">
+      <c r="A14" s="52"/>
+      <c r="B14" s="34"/>
+      <c r="C14" s="24">
         <v>11</v>
       </c>
       <c r="D14" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="E14" s="58" t="s">
+      <c r="E14" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="F14" s="58"/>
+      <c r="F14" s="30"/>
       <c r="G14" s="22"/>
       <c r="H14" s="22"/>
       <c r="I14" s="22"/>
-      <c r="J14" s="36"/>
+      <c r="J14" s="53"/>
     </row>
     <row r="15" spans="1:16" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="35"/>
-      <c r="B15" s="47"/>
-      <c r="C15" s="44">
+      <c r="A15" s="52"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="24">
         <v>12</v>
       </c>
       <c r="D15" s="21" t="s">
         <v>111</v>
       </c>
-      <c r="E15" s="58"/>
-      <c r="F15" s="58"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
       <c r="G15" s="22" t="s">
         <v>106</v>
       </c>
       <c r="H15" s="22"/>
       <c r="I15" s="22"/>
-      <c r="J15" s="36"/>
+      <c r="J15" s="53"/>
     </row>
     <row r="16" spans="1:16" ht="45" x14ac:dyDescent="0.2">
-      <c r="A16" s="38" t="s">
+      <c r="A16" s="56" t="s">
         <v>107</v>
       </c>
-      <c r="B16" s="48" t="s">
+      <c r="B16" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="44">
+      <c r="C16" s="24">
         <v>13</v>
       </c>
       <c r="D16" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="E16" s="58"/>
-      <c r="F16" s="58" t="s">
-        <v>12</v>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30" t="s">
+        <v>11</v>
       </c>
       <c r="G16" s="22"/>
       <c r="H16" s="22"/>
       <c r="I16" s="22"/>
-      <c r="J16" s="36"/>
-    </row>
-    <row r="17" spans="1:10" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="39" t="s">
+      <c r="J16" s="53"/>
+    </row>
+    <row r="17" spans="1:10" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="57" t="s">
         <v>108</v>
       </c>
-      <c r="B17" s="49" t="s">
+      <c r="B17" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="45">
+      <c r="C17" s="24">
         <v>14</v>
       </c>
-      <c r="D17" s="40" t="s">
+      <c r="D17" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="E17" s="59"/>
-      <c r="F17" s="60" t="s">
-        <v>12</v>
-      </c>
-      <c r="G17" s="41"/>
-      <c r="H17" s="41"/>
-      <c r="I17" s="41"/>
-      <c r="J17" s="42"/>
-    </row>
-    <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="53"/>
+    </row>
+    <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="58"/>
+      <c r="B18" s="58"/>
+      <c r="C18" s="59"/>
+      <c r="D18" s="58"/>
+      <c r="E18" s="58"/>
+      <c r="F18" s="58"/>
+      <c r="G18" s="58"/>
+      <c r="H18" s="58"/>
+      <c r="I18" s="58"/>
+      <c r="J18" s="58"/>
+    </row>
     <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2811,18 +2487,18 @@
     <row r="962" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="A8:A12"/>
+    <mergeCell ref="B8:B11"/>
     <mergeCell ref="A13:A15"/>
     <mergeCell ref="B13:B15"/>
     <mergeCell ref="A2:B3"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="A4:A7"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="A8:A12"/>
-    <mergeCell ref="B8:B11"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -2849,19 +2525,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="30"/>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="33" t="s">
+      <c r="A1" s="35"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="32"/>
-      <c r="G1" s="33" t="s">
+      <c r="F1" s="37"/>
+      <c r="G1" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
       <c r="J1" s="1"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
@@ -2870,10 +2546,10 @@
       <c r="P1" s="2"/>
     </row>
     <row r="2" spans="1:16" ht="33" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="32"/>
+      <c r="B2" s="37"/>
       <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
@@ -2905,10 +2581,10 @@
       <c r="P2" s="2"/>
     </row>
     <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="43" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="5">
@@ -2932,8 +2608,8 @@
       <c r="P3" s="2"/>
     </row>
     <row r="4" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="25"/>
-      <c r="B4" s="25"/>
+      <c r="A4" s="41"/>
+      <c r="B4" s="41"/>
       <c r="C4" s="5">
         <v>2</v>
       </c>
@@ -2955,8 +2631,8 @@
       <c r="P4" s="2"/>
     </row>
     <row r="5" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="25"/>
-      <c r="B5" s="25"/>
+      <c r="A5" s="41"/>
+      <c r="B5" s="41"/>
       <c r="C5" s="5">
         <v>3</v>
       </c>
@@ -2978,8 +2654,8 @@
       <c r="P5" s="2"/>
     </row>
     <row r="6" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="25"/>
-      <c r="B6" s="25"/>
+      <c r="A6" s="41"/>
+      <c r="B6" s="41"/>
       <c r="C6" s="5">
         <v>4</v>
       </c>
@@ -3001,8 +2677,8 @@
       <c r="P6" s="2"/>
     </row>
     <row r="7" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="25"/>
-      <c r="B7" s="25"/>
+      <c r="A7" s="41"/>
+      <c r="B7" s="41"/>
       <c r="C7" s="5">
         <v>5</v>
       </c>
@@ -3024,8 +2700,8 @@
       <c r="P7" s="2"/>
     </row>
     <row r="8" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="25"/>
-      <c r="B8" s="25"/>
+      <c r="A8" s="41"/>
+      <c r="B8" s="41"/>
       <c r="C8" s="5">
         <v>6</v>
       </c>
@@ -3047,8 +2723,8 @@
       <c r="P8" s="2"/>
     </row>
     <row r="9" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="25"/>
-      <c r="B9" s="25"/>
+      <c r="A9" s="41"/>
+      <c r="B9" s="41"/>
       <c r="C9" s="5">
         <v>7</v>
       </c>
@@ -3070,8 +2746,8 @@
       <c r="P9" s="2"/>
     </row>
     <row r="10" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="25"/>
-      <c r="B10" s="26"/>
+      <c r="A10" s="41"/>
+      <c r="B10" s="42"/>
       <c r="C10" s="5">
         <v>8</v>
       </c>
@@ -3093,8 +2769,8 @@
       <c r="P10" s="2"/>
     </row>
     <row r="11" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="25"/>
-      <c r="B11" s="27" t="s">
+      <c r="A11" s="41"/>
+      <c r="B11" s="43" t="s">
         <v>30</v>
       </c>
       <c r="C11" s="5">
@@ -3118,8 +2794,8 @@
       <c r="P11" s="2"/>
     </row>
     <row r="12" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="25"/>
-      <c r="B12" s="25"/>
+      <c r="A12" s="41"/>
+      <c r="B12" s="41"/>
       <c r="C12" s="5">
         <v>10</v>
       </c>
@@ -3141,8 +2817,8 @@
       <c r="P12" s="2"/>
     </row>
     <row r="13" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="26"/>
-      <c r="B13" s="26"/>
+      <c r="A13" s="42"/>
+      <c r="B13" s="42"/>
       <c r="C13" s="5">
         <v>11</v>
       </c>
@@ -3164,10 +2840,10 @@
       <c r="P13" s="2"/>
     </row>
     <row r="14" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="24" t="s">
+      <c r="A14" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="43" t="s">
         <v>9</v>
       </c>
       <c r="C14" s="5">
@@ -3191,8 +2867,8 @@
       <c r="P14" s="2"/>
     </row>
     <row r="15" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="25"/>
-      <c r="B15" s="25"/>
+      <c r="A15" s="41"/>
+      <c r="B15" s="41"/>
       <c r="C15" s="5">
         <v>13</v>
       </c>
@@ -3214,8 +2890,8 @@
       <c r="P15" s="2"/>
     </row>
     <row r="16" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="25"/>
-      <c r="B16" s="25"/>
+      <c r="A16" s="41"/>
+      <c r="B16" s="41"/>
       <c r="C16" s="5">
         <v>14</v>
       </c>
@@ -3237,8 +2913,8 @@
       <c r="P16" s="2"/>
     </row>
     <row r="17" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="25"/>
-      <c r="B17" s="25"/>
+      <c r="A17" s="41"/>
+      <c r="B17" s="41"/>
       <c r="C17" s="5">
         <v>15</v>
       </c>
@@ -3260,8 +2936,8 @@
       <c r="P17" s="2"/>
     </row>
     <row r="18" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="25"/>
-      <c r="B18" s="25"/>
+      <c r="A18" s="41"/>
+      <c r="B18" s="41"/>
       <c r="C18" s="5">
         <v>16</v>
       </c>
@@ -3283,8 +2959,8 @@
       <c r="P18" s="2"/>
     </row>
     <row r="19" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="25"/>
-      <c r="B19" s="25"/>
+      <c r="A19" s="41"/>
+      <c r="B19" s="41"/>
       <c r="C19" s="5">
         <v>17</v>
       </c>
@@ -3306,8 +2982,8 @@
       <c r="P19" s="2"/>
     </row>
     <row r="20" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="25"/>
-      <c r="B20" s="26"/>
+      <c r="A20" s="41"/>
+      <c r="B20" s="42"/>
       <c r="C20" s="5">
         <v>18</v>
       </c>
@@ -3329,8 +3005,8 @@
       <c r="P20" s="2"/>
     </row>
     <row r="21" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="25"/>
-      <c r="B21" s="27" t="s">
+      <c r="A21" s="41"/>
+      <c r="B21" s="43" t="s">
         <v>30</v>
       </c>
       <c r="C21" s="5">
@@ -3354,8 +3030,8 @@
       <c r="P21" s="2"/>
     </row>
     <row r="22" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="25"/>
-      <c r="B22" s="25"/>
+      <c r="A22" s="41"/>
+      <c r="B22" s="41"/>
       <c r="C22" s="5">
         <v>20</v>
       </c>
@@ -3377,8 +3053,8 @@
       <c r="P22" s="2"/>
     </row>
     <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="26"/>
-      <c r="B23" s="26"/>
+      <c r="A23" s="42"/>
+      <c r="B23" s="42"/>
       <c r="C23" s="5">
         <v>21</v>
       </c>
@@ -3400,10 +3076,10 @@
       <c r="P23" s="2"/>
     </row>
     <row r="24" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="28" t="s">
+      <c r="A24" s="45" t="s">
         <v>50</v>
       </c>
-      <c r="B24" s="27" t="s">
+      <c r="B24" s="43" t="s">
         <v>9</v>
       </c>
       <c r="C24" s="5">
@@ -3427,8 +3103,8 @@
       <c r="P24" s="2"/>
     </row>
     <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="25"/>
-      <c r="B25" s="25"/>
+      <c r="A25" s="41"/>
+      <c r="B25" s="41"/>
       <c r="C25" s="5">
         <v>23</v>
       </c>
@@ -3450,8 +3126,8 @@
       <c r="P25" s="2"/>
     </row>
     <row r="26" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="25"/>
-      <c r="B26" s="25"/>
+      <c r="A26" s="41"/>
+      <c r="B26" s="41"/>
       <c r="C26" s="5">
         <v>24</v>
       </c>
@@ -3473,8 +3149,8 @@
       <c r="P26" s="2"/>
     </row>
     <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="25"/>
-      <c r="B27" s="25"/>
+      <c r="A27" s="41"/>
+      <c r="B27" s="41"/>
       <c r="C27" s="5">
         <v>25</v>
       </c>
@@ -3496,8 +3172,8 @@
       <c r="P27" s="2"/>
     </row>
     <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="26"/>
-      <c r="B28" s="26"/>
+      <c r="A28" s="42"/>
+      <c r="B28" s="42"/>
       <c r="C28" s="5">
         <v>26</v>
       </c>
@@ -3519,10 +3195,10 @@
       <c r="P28" s="2"/>
     </row>
     <row r="29" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="29" t="s">
+      <c r="A29" s="40" t="s">
         <v>59</v>
       </c>
-      <c r="B29" s="27" t="s">
+      <c r="B29" s="43" t="s">
         <v>9</v>
       </c>
       <c r="C29" s="5">
@@ -3546,8 +3222,8 @@
       <c r="P29" s="2"/>
     </row>
     <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="25"/>
-      <c r="B30" s="25"/>
+      <c r="A30" s="41"/>
+      <c r="B30" s="41"/>
       <c r="C30" s="5">
         <v>28</v>
       </c>
@@ -3569,8 +3245,8 @@
       <c r="P30" s="2"/>
     </row>
     <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="25"/>
-      <c r="B31" s="25"/>
+      <c r="A31" s="41"/>
+      <c r="B31" s="41"/>
       <c r="C31" s="5">
         <v>29</v>
       </c>
@@ -3592,8 +3268,8 @@
       <c r="P31" s="2"/>
     </row>
     <row r="32" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="25"/>
-      <c r="B32" s="25"/>
+      <c r="A32" s="41"/>
+      <c r="B32" s="41"/>
       <c r="C32" s="5">
         <v>30</v>
       </c>
@@ -3615,8 +3291,8 @@
       <c r="P32" s="2"/>
     </row>
     <row r="33" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="25"/>
-      <c r="B33" s="25"/>
+      <c r="A33" s="41"/>
+      <c r="B33" s="41"/>
       <c r="C33" s="5">
         <v>31</v>
       </c>
@@ -3638,8 +3314,8 @@
       <c r="P33" s="2"/>
     </row>
     <row r="34" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="25"/>
-      <c r="B34" s="26"/>
+      <c r="A34" s="41"/>
+      <c r="B34" s="42"/>
       <c r="C34" s="5">
         <v>32</v>
       </c>
@@ -3661,7 +3337,7 @@
       <c r="P34" s="2"/>
     </row>
     <row r="35" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="26"/>
+      <c r="A35" s="42"/>
       <c r="B35" s="13" t="s">
         <v>30</v>
       </c>
@@ -3686,10 +3362,10 @@
       <c r="P35" s="2"/>
     </row>
     <row r="36" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="24" t="s">
+      <c r="A36" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="B36" s="27" t="s">
+      <c r="B36" s="43" t="s">
         <v>9</v>
       </c>
       <c r="C36" s="5">
@@ -3713,8 +3389,8 @@
       <c r="P36" s="2"/>
     </row>
     <row r="37" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="25"/>
-      <c r="B37" s="25"/>
+      <c r="A37" s="41"/>
+      <c r="B37" s="41"/>
       <c r="C37" s="5">
         <v>35</v>
       </c>
@@ -3736,8 +3412,8 @@
       <c r="P37" s="2"/>
     </row>
     <row r="38" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="25"/>
-      <c r="B38" s="25"/>
+      <c r="A38" s="41"/>
+      <c r="B38" s="41"/>
       <c r="C38" s="5">
         <v>36</v>
       </c>
@@ -3759,8 +3435,8 @@
       <c r="P38" s="2"/>
     </row>
     <row r="39" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="25"/>
-      <c r="B39" s="25"/>
+      <c r="A39" s="41"/>
+      <c r="B39" s="41"/>
       <c r="C39" s="5">
         <v>37</v>
       </c>
@@ -3782,8 +3458,8 @@
       <c r="P39" s="2"/>
     </row>
     <row r="40" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="25"/>
-      <c r="B40" s="26"/>
+      <c r="A40" s="41"/>
+      <c r="B40" s="42"/>
       <c r="C40" s="5">
         <v>38</v>
       </c>
@@ -3805,7 +3481,7 @@
       <c r="P40" s="2"/>
     </row>
     <row r="41" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="26"/>
+      <c r="A41" s="42"/>
       <c r="B41" s="13" t="s">
         <v>30</v>
       </c>
@@ -3830,7 +3506,7 @@
       <c r="P41" s="2"/>
     </row>
     <row r="42" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="28" t="s">
+      <c r="A42" s="45" t="s">
         <v>83</v>
       </c>
       <c r="B42" s="14" t="s">
@@ -3857,8 +3533,8 @@
       <c r="P42" s="2"/>
     </row>
     <row r="43" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="25"/>
-      <c r="B43" s="27" t="s">
+      <c r="A43" s="41"/>
+      <c r="B43" s="43" t="s">
         <v>85</v>
       </c>
       <c r="C43" s="5">
@@ -3882,8 +3558,8 @@
       <c r="P43" s="2"/>
     </row>
     <row r="44" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="25"/>
-      <c r="B44" s="25"/>
+      <c r="A44" s="41"/>
+      <c r="B44" s="41"/>
       <c r="C44" s="5">
         <v>42</v>
       </c>
@@ -3905,8 +3581,8 @@
       <c r="P44" s="2"/>
     </row>
     <row r="45" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="25"/>
-      <c r="B45" s="25"/>
+      <c r="A45" s="41"/>
+      <c r="B45" s="41"/>
       <c r="C45" s="5">
         <v>43</v>
       </c>
@@ -3928,8 +3604,8 @@
       <c r="P45" s="2"/>
     </row>
     <row r="46" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="26"/>
-      <c r="B46" s="26"/>
+      <c r="A46" s="42"/>
+      <c r="B46" s="42"/>
       <c r="C46" s="17">
         <v>44</v>
       </c>
@@ -4906,13 +4582,6 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:A13"/>
-    <mergeCell ref="B3:B10"/>
-    <mergeCell ref="B11:B13"/>
     <mergeCell ref="A14:A23"/>
     <mergeCell ref="B21:B23"/>
     <mergeCell ref="A36:A41"/>
@@ -4924,6 +4593,13 @@
     <mergeCell ref="A29:A35"/>
     <mergeCell ref="B29:B34"/>
     <mergeCell ref="B36:B40"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:A13"/>
+    <mergeCell ref="B3:B10"/>
+    <mergeCell ref="B11:B13"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -4950,19 +4626,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="30"/>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="33" t="s">
+      <c r="A1" s="35"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="32"/>
-      <c r="G1" s="33" t="s">
+      <c r="F1" s="37"/>
+      <c r="G1" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
       <c r="J1" s="1"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
@@ -4971,10 +4647,10 @@
       <c r="P1" s="2"/>
     </row>
     <row r="2" spans="1:16" ht="33" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="32"/>
+      <c r="B2" s="37"/>
       <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
@@ -5006,10 +4682,10 @@
       <c r="P2" s="2"/>
     </row>
     <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="43" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="5">
@@ -5033,8 +4709,8 @@
       <c r="P3" s="2"/>
     </row>
     <row r="4" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="25"/>
-      <c r="B4" s="25"/>
+      <c r="A4" s="41"/>
+      <c r="B4" s="41"/>
       <c r="C4" s="5">
         <v>2</v>
       </c>
@@ -5056,8 +4732,8 @@
       <c r="P4" s="2"/>
     </row>
     <row r="5" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="25"/>
-      <c r="B5" s="25"/>
+      <c r="A5" s="41"/>
+      <c r="B5" s="41"/>
       <c r="C5" s="5">
         <v>3</v>
       </c>
@@ -5079,8 +4755,8 @@
       <c r="P5" s="2"/>
     </row>
     <row r="6" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="25"/>
-      <c r="B6" s="25"/>
+      <c r="A6" s="41"/>
+      <c r="B6" s="41"/>
       <c r="C6" s="5">
         <v>4</v>
       </c>
@@ -5102,8 +4778,8 @@
       <c r="P6" s="2"/>
     </row>
     <row r="7" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="25"/>
-      <c r="B7" s="25"/>
+      <c r="A7" s="41"/>
+      <c r="B7" s="41"/>
       <c r="C7" s="5">
         <v>5</v>
       </c>
@@ -5125,8 +4801,8 @@
       <c r="P7" s="2"/>
     </row>
     <row r="8" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="25"/>
-      <c r="B8" s="25"/>
+      <c r="A8" s="41"/>
+      <c r="B8" s="41"/>
       <c r="C8" s="5">
         <v>6</v>
       </c>
@@ -5148,8 +4824,8 @@
       <c r="P8" s="2"/>
     </row>
     <row r="9" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="25"/>
-      <c r="B9" s="25"/>
+      <c r="A9" s="41"/>
+      <c r="B9" s="41"/>
       <c r="C9" s="5">
         <v>7</v>
       </c>
@@ -5171,8 +4847,8 @@
       <c r="P9" s="2"/>
     </row>
     <row r="10" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="25"/>
-      <c r="B10" s="26"/>
+      <c r="A10" s="41"/>
+      <c r="B10" s="42"/>
       <c r="C10" s="5">
         <v>8</v>
       </c>
@@ -5194,8 +4870,8 @@
       <c r="P10" s="2"/>
     </row>
     <row r="11" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="25"/>
-      <c r="B11" s="27" t="s">
+      <c r="A11" s="41"/>
+      <c r="B11" s="43" t="s">
         <v>30</v>
       </c>
       <c r="C11" s="5">
@@ -5219,8 +4895,8 @@
       <c r="P11" s="2"/>
     </row>
     <row r="12" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="25"/>
-      <c r="B12" s="25"/>
+      <c r="A12" s="41"/>
+      <c r="B12" s="41"/>
       <c r="C12" s="5">
         <v>10</v>
       </c>
@@ -5242,8 +4918,8 @@
       <c r="P12" s="2"/>
     </row>
     <row r="13" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="26"/>
-      <c r="B13" s="26"/>
+      <c r="A13" s="42"/>
+      <c r="B13" s="42"/>
       <c r="C13" s="5">
         <v>11</v>
       </c>
@@ -5265,10 +4941,10 @@
       <c r="P13" s="2"/>
     </row>
     <row r="14" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="24" t="s">
+      <c r="A14" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="43" t="s">
         <v>9</v>
       </c>
       <c r="C14" s="5">
@@ -5292,8 +4968,8 @@
       <c r="P14" s="2"/>
     </row>
     <row r="15" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="25"/>
-      <c r="B15" s="25"/>
+      <c r="A15" s="41"/>
+      <c r="B15" s="41"/>
       <c r="C15" s="5">
         <v>13</v>
       </c>
@@ -5315,8 +4991,8 @@
       <c r="P15" s="2"/>
     </row>
     <row r="16" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="25"/>
-      <c r="B16" s="25"/>
+      <c r="A16" s="41"/>
+      <c r="B16" s="41"/>
       <c r="C16" s="5">
         <v>14</v>
       </c>
@@ -5338,8 +5014,8 @@
       <c r="P16" s="2"/>
     </row>
     <row r="17" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="25"/>
-      <c r="B17" s="25"/>
+      <c r="A17" s="41"/>
+      <c r="B17" s="41"/>
       <c r="C17" s="5">
         <v>15</v>
       </c>
@@ -5361,8 +5037,8 @@
       <c r="P17" s="2"/>
     </row>
     <row r="18" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="25"/>
-      <c r="B18" s="25"/>
+      <c r="A18" s="41"/>
+      <c r="B18" s="41"/>
       <c r="C18" s="5">
         <v>16</v>
       </c>
@@ -5384,8 +5060,8 @@
       <c r="P18" s="2"/>
     </row>
     <row r="19" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="25"/>
-      <c r="B19" s="25"/>
+      <c r="A19" s="41"/>
+      <c r="B19" s="41"/>
       <c r="C19" s="5">
         <v>17</v>
       </c>
@@ -5407,8 +5083,8 @@
       <c r="P19" s="2"/>
     </row>
     <row r="20" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="25"/>
-      <c r="B20" s="26"/>
+      <c r="A20" s="41"/>
+      <c r="B20" s="42"/>
       <c r="C20" s="5">
         <v>18</v>
       </c>
@@ -5430,8 +5106,8 @@
       <c r="P20" s="2"/>
     </row>
     <row r="21" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="25"/>
-      <c r="B21" s="27" t="s">
+      <c r="A21" s="41"/>
+      <c r="B21" s="43" t="s">
         <v>30</v>
       </c>
       <c r="C21" s="5">
@@ -5455,8 +5131,8 @@
       <c r="P21" s="2"/>
     </row>
     <row r="22" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="25"/>
-      <c r="B22" s="25"/>
+      <c r="A22" s="41"/>
+      <c r="B22" s="41"/>
       <c r="C22" s="5">
         <v>20</v>
       </c>
@@ -5478,8 +5154,8 @@
       <c r="P22" s="2"/>
     </row>
     <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="26"/>
-      <c r="B23" s="26"/>
+      <c r="A23" s="42"/>
+      <c r="B23" s="42"/>
       <c r="C23" s="5">
         <v>21</v>
       </c>
@@ -5501,10 +5177,10 @@
       <c r="P23" s="2"/>
     </row>
     <row r="24" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="28" t="s">
+      <c r="A24" s="45" t="s">
         <v>50</v>
       </c>
-      <c r="B24" s="27" t="s">
+      <c r="B24" s="43" t="s">
         <v>9</v>
       </c>
       <c r="C24" s="5">
@@ -5528,8 +5204,8 @@
       <c r="P24" s="2"/>
     </row>
     <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="25"/>
-      <c r="B25" s="25"/>
+      <c r="A25" s="41"/>
+      <c r="B25" s="41"/>
       <c r="C25" s="5">
         <v>23</v>
       </c>
@@ -5551,8 +5227,8 @@
       <c r="P25" s="2"/>
     </row>
     <row r="26" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="25"/>
-      <c r="B26" s="25"/>
+      <c r="A26" s="41"/>
+      <c r="B26" s="41"/>
       <c r="C26" s="5">
         <v>24</v>
       </c>
@@ -5574,8 +5250,8 @@
       <c r="P26" s="2"/>
     </row>
     <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="25"/>
-      <c r="B27" s="25"/>
+      <c r="A27" s="41"/>
+      <c r="B27" s="41"/>
       <c r="C27" s="5">
         <v>25</v>
       </c>
@@ -5597,8 +5273,8 @@
       <c r="P27" s="2"/>
     </row>
     <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="26"/>
-      <c r="B28" s="26"/>
+      <c r="A28" s="42"/>
+      <c r="B28" s="42"/>
       <c r="C28" s="5">
         <v>26</v>
       </c>
@@ -5620,10 +5296,10 @@
       <c r="P28" s="2"/>
     </row>
     <row r="29" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="29" t="s">
+      <c r="A29" s="40" t="s">
         <v>59</v>
       </c>
-      <c r="B29" s="27" t="s">
+      <c r="B29" s="43" t="s">
         <v>9</v>
       </c>
       <c r="C29" s="5">
@@ -5647,8 +5323,8 @@
       <c r="P29" s="2"/>
     </row>
     <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="25"/>
-      <c r="B30" s="25"/>
+      <c r="A30" s="41"/>
+      <c r="B30" s="41"/>
       <c r="C30" s="5">
         <v>28</v>
       </c>
@@ -5670,8 +5346,8 @@
       <c r="P30" s="2"/>
     </row>
     <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="25"/>
-      <c r="B31" s="25"/>
+      <c r="A31" s="41"/>
+      <c r="B31" s="41"/>
       <c r="C31" s="5">
         <v>29</v>
       </c>
@@ -5693,8 +5369,8 @@
       <c r="P31" s="2"/>
     </row>
     <row r="32" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="25"/>
-      <c r="B32" s="25"/>
+      <c r="A32" s="41"/>
+      <c r="B32" s="41"/>
       <c r="C32" s="5">
         <v>30</v>
       </c>
@@ -5716,8 +5392,8 @@
       <c r="P32" s="2"/>
     </row>
     <row r="33" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="25"/>
-      <c r="B33" s="25"/>
+      <c r="A33" s="41"/>
+      <c r="B33" s="41"/>
       <c r="C33" s="5">
         <v>31</v>
       </c>
@@ -5739,8 +5415,8 @@
       <c r="P33" s="2"/>
     </row>
     <row r="34" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="25"/>
-      <c r="B34" s="26"/>
+      <c r="A34" s="41"/>
+      <c r="B34" s="42"/>
       <c r="C34" s="5">
         <v>32</v>
       </c>
@@ -5762,7 +5438,7 @@
       <c r="P34" s="2"/>
     </row>
     <row r="35" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="26"/>
+      <c r="A35" s="42"/>
       <c r="B35" s="13" t="s">
         <v>30</v>
       </c>
@@ -5787,10 +5463,10 @@
       <c r="P35" s="2"/>
     </row>
     <row r="36" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="24" t="s">
+      <c r="A36" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="B36" s="27" t="s">
+      <c r="B36" s="43" t="s">
         <v>9</v>
       </c>
       <c r="C36" s="5">
@@ -5814,8 +5490,8 @@
       <c r="P36" s="2"/>
     </row>
     <row r="37" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="25"/>
-      <c r="B37" s="25"/>
+      <c r="A37" s="41"/>
+      <c r="B37" s="41"/>
       <c r="C37" s="5">
         <v>35</v>
       </c>
@@ -5837,8 +5513,8 @@
       <c r="P37" s="2"/>
     </row>
     <row r="38" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="25"/>
-      <c r="B38" s="25"/>
+      <c r="A38" s="41"/>
+      <c r="B38" s="41"/>
       <c r="C38" s="5">
         <v>36</v>
       </c>
@@ -5860,8 +5536,8 @@
       <c r="P38" s="2"/>
     </row>
     <row r="39" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="25"/>
-      <c r="B39" s="25"/>
+      <c r="A39" s="41"/>
+      <c r="B39" s="41"/>
       <c r="C39" s="5">
         <v>37</v>
       </c>
@@ -5883,8 +5559,8 @@
       <c r="P39" s="2"/>
     </row>
     <row r="40" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="25"/>
-      <c r="B40" s="26"/>
+      <c r="A40" s="41"/>
+      <c r="B40" s="42"/>
       <c r="C40" s="5">
         <v>38</v>
       </c>
@@ -5906,7 +5582,7 @@
       <c r="P40" s="2"/>
     </row>
     <row r="41" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="26"/>
+      <c r="A41" s="42"/>
       <c r="B41" s="13" t="s">
         <v>30</v>
       </c>
@@ -5931,7 +5607,7 @@
       <c r="P41" s="2"/>
     </row>
     <row r="42" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="28" t="s">
+      <c r="A42" s="45" t="s">
         <v>83</v>
       </c>
       <c r="B42" s="14" t="s">
@@ -5958,8 +5634,8 @@
       <c r="P42" s="2"/>
     </row>
     <row r="43" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="25"/>
-      <c r="B43" s="27" t="s">
+      <c r="A43" s="41"/>
+      <c r="B43" s="43" t="s">
         <v>85</v>
       </c>
       <c r="C43" s="5">
@@ -5983,8 +5659,8 @@
       <c r="P43" s="2"/>
     </row>
     <row r="44" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="25"/>
-      <c r="B44" s="25"/>
+      <c r="A44" s="41"/>
+      <c r="B44" s="41"/>
       <c r="C44" s="5">
         <v>42</v>
       </c>
@@ -6006,8 +5682,8 @@
       <c r="P44" s="2"/>
     </row>
     <row r="45" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="25"/>
-      <c r="B45" s="25"/>
+      <c r="A45" s="41"/>
+      <c r="B45" s="41"/>
       <c r="C45" s="5">
         <v>43</v>
       </c>
@@ -6029,8 +5705,8 @@
       <c r="P45" s="2"/>
     </row>
     <row r="46" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="26"/>
-      <c r="B46" s="26"/>
+      <c r="A46" s="42"/>
+      <c r="B46" s="42"/>
       <c r="C46" s="17">
         <v>44</v>
       </c>
@@ -7007,13 +6683,6 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:A13"/>
-    <mergeCell ref="B3:B10"/>
-    <mergeCell ref="B11:B13"/>
     <mergeCell ref="A14:A23"/>
     <mergeCell ref="B21:B23"/>
     <mergeCell ref="A36:A41"/>
@@ -7025,6 +6694,13 @@
     <mergeCell ref="A29:A35"/>
     <mergeCell ref="B29:B34"/>
     <mergeCell ref="B36:B40"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:A13"/>
+    <mergeCell ref="B3:B10"/>
+    <mergeCell ref="B11:B13"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
Algumas ultimas alterações Correção ac05
</commit_message>
<xml_diff>
--- a/Artefatos/17. Análise dos Eventos para cada Cenário.xlsx
+++ b/Artefatos/17. Análise dos Eventos para cada Cenário.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amand\OneDrive\Área de Trabalho\GIT\OPE-Madara\Artefatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F7F9AB5-0C2F-4648-ADE4-1DEA6685F03D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{546B9102-6A8B-4C5B-868B-FB11629EFFFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20520" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="REALIZACAO_MATRICULA" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="39">
   <si>
     <t>Externo</t>
   </si>
@@ -66,9 +66,6 @@
     <t>X(2)</t>
   </si>
   <si>
-    <t>X(3)</t>
-  </si>
-  <si>
     <t>X(5)</t>
   </si>
   <si>
@@ -76,27 +73,6 @@
   </si>
   <si>
     <t>FA</t>
-  </si>
-  <si>
-    <t>Gerir o negócio</t>
-  </si>
-  <si>
-    <t>Cobrança de inadimplências</t>
-  </si>
-  <si>
-    <t>Falha</t>
-  </si>
-  <si>
-    <t>Ineficiência na cobrança das mensalidades</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aluno reclama que não recebeu cobrança da mensalidade </t>
-  </si>
-  <si>
-    <t>Ineficiência no controle de entrada e saída de alunos das turmas</t>
-  </si>
-  <si>
-    <t>Ineficiência na elaboração de Cronogramas</t>
   </si>
   <si>
     <t>Análise dos Eventos para cada Cenário</t>
@@ -186,31 +162,19 @@
   <si>
     <t>Previsível*</t>
   </si>
+  <si>
+    <t>Aluno Responde solicitação de posição</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
     </font>
     <font>
       <sz val="11"/>
@@ -272,30 +236,12 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFBFEBE"/>
-        <bgColor rgb="FFFBFEBE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFBBE0E3"/>
-        <bgColor rgb="FFBBE0E3"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFDE9D9"/>
-        <bgColor rgb="FFFDE9D9"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -341,75 +287,17 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor rgb="FFB6D7A8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -431,115 +319,91 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -760,17 +624,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P962"/>
+  <dimension ref="A1:P957"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.875" customWidth="1"/>
     <col min="2" max="2" width="3.25" customWidth="1"/>
-    <col min="3" max="3" width="3" style="12" customWidth="1"/>
+    <col min="3" max="3" width="3" style="6" customWidth="1"/>
     <col min="4" max="4" width="36.125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.25" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.125" bestFit="1" customWidth="1"/>
@@ -782,41 +646,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
+      <c r="A1" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
     </row>
     <row r="2" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33" t="s">
+      <c r="B2" s="23"/>
+      <c r="C2" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="33" t="s">
+      <c r="D2" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="28"/>
-      <c r="G2" s="29" t="s">
+      <c r="F2" s="25"/>
+      <c r="G2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="21"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="15"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
@@ -824,101 +688,101 @@
       <c r="P2" s="1"/>
     </row>
     <row r="3" spans="1:16" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="33"/>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="F3" s="15" t="s">
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="H3" s="15" t="s">
+      <c r="G3" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="15" t="s">
+      <c r="I3" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="J3" s="15" t="s">
-        <v>39</v>
-      </c>
       <c r="L3" s="1"/>
-      <c r="M3" s="18"/>
+      <c r="M3" s="12"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
     </row>
     <row r="4" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="5">
         <v>1</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16" t="s">
+      <c r="E4" s="10"/>
+      <c r="F4" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="23"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="17"/>
       <c r="L4" s="1"/>
-      <c r="M4" s="18"/>
+      <c r="M4" s="12"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
     </row>
     <row r="5" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="32"/>
-      <c r="B5" s="30"/>
-      <c r="C5" s="11">
+      <c r="A5" s="21"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="5">
         <v>2</v>
       </c>
-      <c r="D5" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9" t="s">
+      <c r="D5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="9"/>
-      <c r="J5" s="23"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="17"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
-      <c r="N5" s="10"/>
+      <c r="N5" s="4"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
     </row>
     <row r="6" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="32"/>
-      <c r="B6" s="30"/>
-      <c r="C6" s="11">
+      <c r="A6" s="21"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="5">
         <v>3</v>
       </c>
-      <c r="D6" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="17" t="s">
+      <c r="D6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="16"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="23"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="17"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
@@ -926,24 +790,27 @@
       <c r="P6" s="1"/>
     </row>
     <row r="7" spans="1:16" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="32"/>
-      <c r="B7" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="11">
+      <c r="A7" s="21"/>
+      <c r="B7" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="5">
         <v>4</v>
       </c>
-      <c r="D7" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9" t="s">
+      <c r="D7" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I7" s="9"/>
-      <c r="J7" s="23"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="28" t="s">
+        <v>38</v>
+      </c>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
@@ -951,299 +818,211 @@
       <c r="P7" s="1"/>
     </row>
     <row r="8" spans="1:16" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="30" t="s">
+      <c r="A8" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="5">
         <v>5</v>
       </c>
-      <c r="D8" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="9" t="s">
+      <c r="D8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="23"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="17"/>
     </row>
     <row r="9" spans="1:16" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="31"/>
-      <c r="B9" s="30"/>
-      <c r="C9" s="11">
+      <c r="A9" s="27"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="5">
         <v>6</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="17"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="23"/>
+      <c r="D9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="11"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="17"/>
     </row>
     <row r="10" spans="1:16" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="31"/>
-      <c r="B10" s="30"/>
-      <c r="C10" s="11">
+      <c r="A10" s="27"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="5">
         <v>7</v>
       </c>
-      <c r="D10" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" s="16"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="23"/>
+      <c r="D10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="10"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="17"/>
     </row>
     <row r="11" spans="1:16" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="31"/>
-      <c r="B11" s="30"/>
-      <c r="C11" s="11">
+      <c r="A11" s="27"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="5">
         <v>8</v>
       </c>
-      <c r="D11" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="F11" s="17"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="23"/>
+      <c r="D11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="11"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="17"/>
     </row>
     <row r="12" spans="1:16" ht="20.25" x14ac:dyDescent="0.2">
-      <c r="A12" s="31"/>
-      <c r="B12" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="11">
+      <c r="A12" s="27"/>
+      <c r="B12" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="5">
         <v>9</v>
       </c>
-      <c r="D12" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E12" s="16"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="23"/>
+      <c r="D12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="10"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="17"/>
     </row>
     <row r="13" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="32" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="30" t="s">
+      <c r="A13" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="11">
+      <c r="C13" s="5">
         <v>10</v>
       </c>
-      <c r="D13" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="24" t="s">
+      <c r="D13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="18" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="32"/>
-      <c r="B14" s="30"/>
-      <c r="C14" s="11">
+      <c r="A14" s="21"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="5">
         <v>11</v>
       </c>
-      <c r="D14" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E14" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="F14" s="17"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="23"/>
+      <c r="D14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" s="11"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="17"/>
     </row>
     <row r="15" spans="1:16" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="32"/>
-      <c r="B15" s="30"/>
-      <c r="C15" s="11">
+      <c r="A15" s="21"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="5">
         <v>12</v>
       </c>
-      <c r="D15" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="23"/>
+      <c r="D15" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="28" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="16" spans="1:16" ht="45" x14ac:dyDescent="0.2">
-      <c r="A16" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="B16" s="13" t="s">
+      <c r="A16" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="11">
+      <c r="C16" s="5">
         <v>13</v>
       </c>
-      <c r="D16" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17" t="s">
+      <c r="D16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="23"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="17"/>
     </row>
     <row r="17" spans="1:10" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="B17" s="13" t="s">
+      <c r="A17" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="11">
+      <c r="C17" s="5">
         <v>14</v>
       </c>
-      <c r="D17" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E17" s="16"/>
-      <c r="F17" s="17" t="s">
+      <c r="D17" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" s="10"/>
+      <c r="F17" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="23"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="17"/>
     </row>
-    <row r="18" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="37" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" s="2">
-        <v>15</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="38"/>
-      <c r="B19" s="36" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" s="2">
-        <v>16</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="J19" s="7"/>
-    </row>
-    <row r="20" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="38"/>
-      <c r="B20" s="34"/>
-      <c r="C20" s="2">
-        <v>17</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="7"/>
-    </row>
-    <row r="21" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="38"/>
-      <c r="B21" s="34"/>
-      <c r="C21" s="2">
-        <v>18</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J21" s="7"/>
-    </row>
-    <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="39"/>
-      <c r="B22" s="35"/>
-      <c r="C22" s="4">
-        <v>19</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="7"/>
-    </row>
+    <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2179,18 +1958,8 @@
     <row r="955" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="956" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="957" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="958" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="959" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="960" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="961" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="962" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="A18:A22"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="A2:B3"/>
+  <mergeCells count="12">
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="A4:A7"/>
@@ -2198,6 +1967,9 @@
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="G2:I2"/>
     <mergeCell ref="B4:B6"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="A2:B3"/>
     <mergeCell ref="A8:A12"/>
     <mergeCell ref="B8:B11"/>
   </mergeCells>

</xml_diff>